<commit_message>
update generated data Triggered by 030a11fb54b994d722dbbd6e93ae6bc699d7971b
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H334"/>
+  <dimension ref="A1:H333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9272,46 +9272,50 @@
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>TSN</t>
+          <t>NRT</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Tianjin, China</t>
+          <t>Tokyo, Japan</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Tianjin</t>
+          <t>Tokyo</t>
         </is>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G235" t="inlineStr"/>
-      <c r="H235" t="inlineStr"/>
+          <t>JP</t>
+        </is>
+      </c>
+      <c r="G235" t="n">
+        <v>35.7647018433</v>
+      </c>
+      <c r="H235" t="n">
+        <v>140.386001587</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>NRT</t>
+          <t>ULN</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Tokyo, Japan</t>
+          <t>Ulaanbaatar, Mongolia</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -9321,35 +9325,35 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>Tokyo</t>
+          <t>Ulaanbaatar</t>
         </is>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Mongolia</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="G236" t="n">
-        <v>35.7647018433</v>
+        <v>47.8431015015</v>
       </c>
       <c r="H236" t="n">
-        <v>140.386001587</v>
+        <v>106.766998291</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>ULN</t>
+          <t>VTE</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Ulaanbaatar, Mongolia</t>
+          <t>Vientiane, Laos</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -9359,255 +9363,251 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>Ulaanbaatar</t>
+          <t>Vientiane</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Mongolia</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>LA</t>
         </is>
       </c>
       <c r="G237" t="n">
-        <v>47.8431015015</v>
+        <v>17.9757</v>
       </c>
       <c r="H237" t="n">
-        <v>106.766998291</v>
+        <v>102.5683</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>VTE</t>
+          <t>KHN</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Vientiane, Laos</t>
+          <t>Nanchang, China</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>Vientiane</t>
+          <t>Nanchang</t>
         </is>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Laos</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>LA</t>
-        </is>
-      </c>
-      <c r="G238" t="n">
-        <v>17.9757</v>
-      </c>
-      <c r="H238" t="n">
-        <v>102.5683</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G238" t="inlineStr"/>
+      <c r="H238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>KHN</t>
+          <t>EVN</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Nanchang, China</t>
+          <t>Yerevan, Armenia</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>Nanchang</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Armenia</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G239" t="inlineStr"/>
-      <c r="H239" t="inlineStr"/>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="G239" t="n">
+        <v>40.1473007202</v>
+      </c>
+      <c r="H239" t="n">
+        <v>44.3959007263</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>EVN</t>
+          <t>JOG</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Yerevan, Armenia</t>
+          <t>Yogyakarta, Indonesia</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>Yerevan</t>
+          <t>Yogyakarta</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>Armenia</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>AM</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="G240" t="n">
-        <v>40.1473007202</v>
+        <v>-7.7881798744</v>
       </c>
       <c r="H240" t="n">
-        <v>44.3959007263</v>
+        <v>110.4319992065</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>JOG</t>
+          <t>ZGN</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Yogyakarta, Indonesia</t>
+          <t>Zhongshan, China</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Yogyakarta</t>
+          <t>Zhongshan</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="G241" t="n">
-        <v>-7.7881798744</v>
-      </c>
-      <c r="H241" t="n">
-        <v>110.4319992065</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr"/>
+      <c r="H241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>ZGN</t>
+          <t>CGY</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Zhongshan, China</t>
+          <t>Cagayan de Oro, Philippines</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Zhongshan</t>
+          <t>Cagayan de Oro</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G242" t="inlineStr"/>
-      <c r="H242" t="inlineStr"/>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="G242" t="n">
+        <v>8.415619850200001</v>
+      </c>
+      <c r="H242" t="n">
+        <v>124.611000061</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>CGY</t>
+          <t>WHU</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Cagayan de Oro, Philippines</t>
+          <t>Wuhu, China</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Cagayan de Oro</t>
+          <t>Wuhu</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>PH</t>
-        </is>
-      </c>
-      <c r="G243" t="n">
-        <v>8.415619850200001</v>
-      </c>
-      <c r="H243" t="n">
-        <v>124.611000061</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr"/>
+      <c r="H243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>WHU</t>
+          <t>HYN</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Wuhu, China</t>
+          <t>Taizhou, China</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -9617,7 +9617,7 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>Wuhu</t>
+          <t>Taizhou</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
@@ -9636,46 +9636,50 @@
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>HYN</t>
+          <t>COK</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Taizhou, China</t>
+          <t>Kochi, India</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Taizhou</t>
+          <t>Kochi</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G245" t="inlineStr"/>
-      <c r="H245" t="inlineStr"/>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="G245" t="n">
+        <v>9.9312</v>
+      </c>
+      <c r="H245" t="n">
+        <v>76.26730000000001</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>DPS</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Kochi, India</t>
+          <t>Denpasar, Indonesia</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -9685,35 +9689,35 @@
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Kochi</t>
+          <t>Denpasar</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="G246" t="n">
-        <v>9.9312</v>
+        <v>-8.748169899000001</v>
       </c>
       <c r="H246" t="n">
-        <v>76.26730000000001</v>
+        <v>115.1669998169</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>DPS</t>
+          <t>CNN</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Denpasar, Indonesia</t>
+          <t>Kannur, India</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -9723,73 +9727,69 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Denpasar</t>
+          <t>Kannur</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G247" t="n">
-        <v>-8.748169899000001</v>
+        <v>11.915858</v>
       </c>
       <c r="H247" t="n">
-        <v>115.1669998169</v>
+        <v>75.55094</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>CNN</t>
+          <t>SZX</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Kannur, India</t>
+          <t>Shenzhen, China</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Kannur</t>
+          <t>Shenzhen</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="G248" t="n">
-        <v>11.915858</v>
-      </c>
-      <c r="H248" t="n">
-        <v>75.55094</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G248" t="inlineStr"/>
+      <c r="H248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>SZX</t>
+          <t>KWE</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Shenzhen, China</t>
+          <t>Guiyang, China</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -9799,7 +9799,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Shenzhen</t>
+          <t>Guiyang</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -9818,12 +9818,12 @@
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>KWE</t>
+          <t>HGH</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Guiyang, China</t>
+          <t>Shaoxing, China</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -9833,7 +9833,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Guiyang</t>
+          <t>Shaoxing</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
@@ -9852,12 +9852,12 @@
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>HGH</t>
+          <t>CZX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Shaoxing, China</t>
+          <t>Changzhou, China</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -9867,7 +9867,7 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Shaoxing</t>
+          <t>Changzhou</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
@@ -9886,12 +9886,12 @@
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>CZX</t>
+          <t>KMG</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Changzhou, China</t>
+          <t>Kunming, China</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -9901,7 +9901,7 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>Changzhou</t>
+          <t>Kunming</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
@@ -9920,84 +9920,84 @@
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>KMG</t>
+          <t>CNX</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Kunming, China</t>
+          <t>Chiang Mai, Thailand</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>Kunming</t>
+          <t>Chiang Mai</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G253" t="inlineStr"/>
-      <c r="H253" t="inlineStr"/>
+          <t>TH</t>
+        </is>
+      </c>
+      <c r="G253" t="n">
+        <v>18.7667999268</v>
+      </c>
+      <c r="H253" t="n">
+        <v>98.962600708</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>CNX</t>
+          <t>CGO</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Chiang Mai, Thailand</t>
+          <t>Zhengzhou, China</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Chiang Mai</t>
+          <t>Zhengzhou</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t>TH</t>
-        </is>
-      </c>
-      <c r="G254" t="n">
-        <v>18.7667999268</v>
-      </c>
-      <c r="H254" t="n">
-        <v>98.962600708</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G254" t="inlineStr"/>
+      <c r="H254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>CGO</t>
+          <t>TYN</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Zhengzhou, China</t>
+          <t>Yangquan, China</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -10007,7 +10007,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Zhengzhou</t>
+          <t>Yangquan</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
@@ -10026,12 +10026,12 @@
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>TYN</t>
+          <t>CSX</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Yangquan, China</t>
+          <t>Changsha, China</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -10041,7 +10041,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Yangquan</t>
+          <t>Changsha</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
@@ -10060,12 +10060,12 @@
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>CSX</t>
+          <t>DLC</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Changsha, China</t>
+          <t>Dalian, China</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -10075,7 +10075,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Changsha</t>
+          <t>Dalian</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
@@ -10094,12 +10094,12 @@
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>DLC</t>
+          <t>BHY</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Dalian, China</t>
+          <t>Beihai, China</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -10109,7 +10109,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Dalian</t>
+          <t>Beihai</t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
@@ -10128,12 +10128,12 @@
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>BHY</t>
+          <t>CKG</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Beihai, China</t>
+          <t>Chongqing, China</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -10143,7 +10143,7 @@
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Beihai</t>
+          <t>Chongqing</t>
         </is>
       </c>
       <c r="E259" t="inlineStr">
@@ -10162,12 +10162,12 @@
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>CKG</t>
+          <t>HFE</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Chongqing, China</t>
+          <t>Huainan, China</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -10177,7 +10177,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Chongqing</t>
+          <t>Huainan</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
@@ -10196,12 +10196,12 @@
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>HFE</t>
+          <t>XFN</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Huainan, China</t>
+          <t>Xiangyang, China</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -10211,7 +10211,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Huainan</t>
+          <t>Xiangyang</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
@@ -10230,12 +10230,12 @@
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>XFN</t>
+          <t>XNN</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Xiangyang, China</t>
+          <t>Xining, China</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -10245,7 +10245,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Xiangyang</t>
+          <t>Xining</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
@@ -10264,118 +10264,122 @@
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>XNN</t>
+          <t>DAD</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Xining, China</t>
+          <t>Da Nang, Vietnam</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Xining</t>
+          <t>Da Nang</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Vietnam</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G263" t="inlineStr"/>
-      <c r="H263" t="inlineStr"/>
+          <t>VN</t>
+        </is>
+      </c>
+      <c r="G263" t="n">
+        <v>16.02636</v>
+      </c>
+      <c r="H263" t="n">
+        <v>108.20869</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>DAD</t>
+          <t>JXG</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Da Nang, Vietnam</t>
+          <t>Jiaxing, China</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Da Nang</t>
+          <t>Jiaxing</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>VN</t>
-        </is>
-      </c>
-      <c r="G264" t="n">
-        <v>16.02636</v>
-      </c>
-      <c r="H264" t="n">
-        <v>108.20869</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr"/>
+      <c r="H264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>JXG</t>
+          <t>CRK</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Jiaxing, China</t>
+          <t>Tarlac City, Philippines</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Jiaxing</t>
+          <t>Tarlac City</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G265" t="inlineStr"/>
-      <c r="H265" t="inlineStr"/>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="G265" t="n">
+        <v>15.1859</v>
+      </c>
+      <c r="H265" t="n">
+        <v>120.5599</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>CRK</t>
+          <t>PBH</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Tarlac City, Philippines</t>
+          <t>Thimphu, Bhutan</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -10385,73 +10389,69 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Tarlac City</t>
+          <t>Thimphu</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Bhutan</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>BT</t>
         </is>
       </c>
       <c r="G266" t="n">
-        <v>15.1859</v>
+        <v>27.4712</v>
       </c>
       <c r="H266" t="n">
-        <v>120.5599</v>
+        <v>89.6339</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>PBH</t>
+          <t>XIY</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Thimphu, Bhutan</t>
+          <t>Baoji, China</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Thimphu</t>
+          <t>Baoji</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Bhutan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>BT</t>
-        </is>
-      </c>
-      <c r="G267" t="n">
-        <v>27.4712</v>
-      </c>
-      <c r="H267" t="n">
-        <v>89.6339</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr"/>
+      <c r="H267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>XIY</t>
+          <t>CTU</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Baoji, China</t>
+          <t>Chengdu, China</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -10461,7 +10461,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Baoji</t>
+          <t>Chengdu</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
@@ -10480,118 +10480,122 @@
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>CTU</t>
+          <t>NQZ</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Chengdu, China</t>
+          <t>Astana, Kazakhstan</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Chengdu</t>
+          <t>Astana</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G269" t="inlineStr"/>
-      <c r="H269" t="inlineStr"/>
+          <t>KZ</t>
+        </is>
+      </c>
+      <c r="G269" t="n">
+        <v>51.167801</v>
+      </c>
+      <c r="H269" t="n">
+        <v>71.418893</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>NQZ</t>
+          <t>NNG</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Astana, Kazakhstan</t>
+          <t>Nanning, China</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Astana</t>
+          <t>Nanning</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G270" t="n">
-        <v>51.167801</v>
-      </c>
-      <c r="H270" t="n">
-        <v>71.418893</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G270" t="inlineStr"/>
+      <c r="H270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>NNG</t>
+          <t>KCH</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Nanning, China</t>
+          <t>Kuching, Malaysia</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Nanning</t>
+          <t>Kuching</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G271" t="inlineStr"/>
-      <c r="H271" t="inlineStr"/>
+          <t>MY</t>
+        </is>
+      </c>
+      <c r="G271" t="n">
+        <v>1.709727</v>
+      </c>
+      <c r="H271" t="n">
+        <v>110.353455</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>KCH</t>
+          <t>AKX</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Kuching, Malaysia</t>
+          <t>Aktobe, Kazakhstan</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -10601,107 +10605,107 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Kuching</t>
+          <t>Aktobe</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>MY</t>
+          <t>KZ</t>
         </is>
       </c>
       <c r="G272" t="n">
-        <v>1.709727</v>
+        <v>50.286922</v>
       </c>
       <c r="H272" t="n">
-        <v>110.353455</v>
+        <v>57.224121</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>AKX</t>
+          <t>TEN</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Aktobe, Kazakhstan</t>
+          <t>Tongren, China</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Aktobe</t>
+          <t>Tongren</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G273" t="n">
-        <v>50.286922</v>
-      </c>
-      <c r="H273" t="n">
-        <v>57.224121</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G273" t="inlineStr"/>
+      <c r="H273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>TEN</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Tongren, China</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Tongren</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G274" t="inlineStr"/>
-      <c r="H274" t="inlineStr"/>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="G274" t="n">
+        <v>38.94449997</v>
+      </c>
+      <c r="H274" t="n">
+        <v>-77.45580292</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10711,7 +10715,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -10725,21 +10729,21 @@
         </is>
       </c>
       <c r="G275" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H275" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10749,7 +10753,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -10763,21 +10767,21 @@
         </is>
       </c>
       <c r="G276" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="H276" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10787,7 +10791,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -10801,21 +10805,21 @@
         </is>
       </c>
       <c r="G277" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="H277" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10825,35 +10829,35 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G278" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="H278" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10863,35 +10867,35 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G279" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H279" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10901,7 +10905,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10915,21 +10919,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="H280" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10939,7 +10943,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10953,21 +10957,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H281" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -10977,7 +10981,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -10991,21 +10995,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H282" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11015,7 +11019,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11029,21 +11033,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H283" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11053,7 +11057,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11067,21 +11071,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H284" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11091,7 +11095,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11105,21 +11109,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H285" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11129,7 +11133,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11143,21 +11147,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H286" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11167,7 +11171,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11181,21 +11185,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="H287" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11205,7 +11209,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11219,21 +11223,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H288" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11243,7 +11247,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -11257,21 +11261,21 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H289" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11281,7 +11285,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11295,21 +11299,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="H290" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11319,7 +11323,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -11333,21 +11337,21 @@
         </is>
       </c>
       <c r="G291" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="H291" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11357,7 +11361,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>McAllen</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
@@ -11371,21 +11375,21 @@
         </is>
       </c>
       <c r="G292" t="n">
-        <v>33.94250107</v>
+        <v>26.17580032</v>
       </c>
       <c r="H292" t="n">
-        <v>-118.4079971</v>
+        <v>-98.23860168</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11395,7 +11399,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -11409,21 +11413,21 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H293" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11433,35 +11437,35 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G294" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H294" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11471,35 +11475,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H295" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11509,7 +11513,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11523,21 +11527,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H296" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11547,35 +11551,35 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G297" t="n">
-        <v>44.8819999695</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H297" t="n">
-        <v>-93.22180175779999</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11585,35 +11589,35 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G298" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H298" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11623,7 +11627,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
@@ -11637,21 +11641,21 @@
         </is>
       </c>
       <c r="G299" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H299" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11661,7 +11665,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -11675,21 +11679,21 @@
         </is>
       </c>
       <c r="G300" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H300" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11699,7 +11703,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11713,21 +11717,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H301" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11737,35 +11741,35 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G302" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H302" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11775,35 +11779,35 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G303" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H303" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11813,7 +11817,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -11827,21 +11831,21 @@
         </is>
       </c>
       <c r="G304" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="H304" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11851,7 +11855,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
@@ -11865,21 +11869,21 @@
         </is>
       </c>
       <c r="G305" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="H305" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11889,7 +11893,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11903,21 +11907,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="H306" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11927,35 +11931,35 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G307" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H307" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11965,35 +11969,35 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G308" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H308" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12003,7 +12007,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12017,21 +12021,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="H309" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12041,7 +12045,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -12055,21 +12059,21 @@
         </is>
       </c>
       <c r="G310" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H310" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12079,7 +12083,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -12093,21 +12097,21 @@
         </is>
       </c>
       <c r="G311" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H311" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12117,7 +12121,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
@@ -12131,21 +12135,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H312" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12155,35 +12159,35 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G313" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H313" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12193,35 +12197,35 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G314" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H314" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12231,12 +12235,12 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -12245,21 +12249,21 @@
         </is>
       </c>
       <c r="G315" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H315" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12269,12 +12273,12 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -12283,21 +12287,21 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H316" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12307,7 +12311,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12321,21 +12325,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H317" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12345,35 +12349,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H318" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12383,7 +12387,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
@@ -12397,21 +12401,21 @@
         </is>
       </c>
       <c r="G319" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="H319" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12421,7 +12425,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
@@ -12435,21 +12439,21 @@
         </is>
       </c>
       <c r="G320" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H320" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12459,35 +12463,35 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G321" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H321" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12497,35 +12501,35 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G322" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="H322" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12535,35 +12539,35 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="H323" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12573,7 +12577,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
@@ -12587,21 +12591,21 @@
         </is>
       </c>
       <c r="G324" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="H324" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12611,7 +12615,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12625,21 +12629,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="H325" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12649,35 +12653,35 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G326" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H326" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12687,35 +12691,35 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G327" t="n">
-        <v>20.5217990875</v>
+        <v>29.429461</v>
       </c>
       <c r="H327" t="n">
-        <v>-103.3109970093</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12725,7 +12729,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12739,21 +12743,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>29.429461</v>
+        <v>41.50069</v>
       </c>
       <c r="H328" t="n">
-        <v>-98.487061</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12763,7 +12767,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12777,21 +12781,21 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>41.50069</v>
+        <v>35.93543</v>
       </c>
       <c r="H329" t="n">
-        <v>-81.68411999999999</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -12801,7 +12805,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -12815,21 +12819,21 @@
         </is>
       </c>
       <c r="G330" t="n">
-        <v>35.93543</v>
+        <v>35.46655</v>
       </c>
       <c r="H330" t="n">
-        <v>-78.88075000000001</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -12839,7 +12843,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
@@ -12853,21 +12857,21 @@
         </is>
       </c>
       <c r="G331" t="n">
-        <v>35.46655</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H331" t="n">
-        <v>-97.65373</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -12877,7 +12881,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Anchorage</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
@@ -12891,21 +12895,21 @@
         </is>
       </c>
       <c r="G332" t="n">
-        <v>27.9755001068</v>
+        <v>61.158555</v>
       </c>
       <c r="H332" t="n">
-        <v>-82.533203125</v>
+        <v>-149.890208</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -12915,61 +12919,23 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G333" t="n">
-        <v>61.158555</v>
+        <v>44.64601</v>
       </c>
       <c r="H333" t="n">
-        <v>-149.890208</v>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334" s="1" t="inlineStr">
-        <is>
-          <t>YHZ</t>
-        </is>
-      </c>
-      <c r="B334" t="inlineStr">
-        <is>
-          <t>Halifax, Canada</t>
-        </is>
-      </c>
-      <c r="C334" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="D334" t="inlineStr">
-        <is>
-          <t>Halifax</t>
-        </is>
-      </c>
-      <c r="E334" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F334" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="G334" t="n">
-        <v>44.64601</v>
-      </c>
-      <c r="H334" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 3a7bd562397115fa1ae7163737036613d45794d2
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H334"/>
+  <dimension ref="A1:H333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10200,12 +10200,12 @@
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>HFE</t>
+          <t>XFN</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Huainan, China</t>
+          <t>Xiangyang, China</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -10215,7 +10215,7 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Huainan</t>
+          <t>Xiangyang</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
@@ -10234,12 +10234,12 @@
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>XFN</t>
+          <t>XNN</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Xiangyang, China</t>
+          <t>Xining, China</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -10249,7 +10249,7 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Xiangyang</t>
+          <t>Xining</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
@@ -10268,118 +10268,122 @@
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>XNN</t>
+          <t>DAD</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Xining, China</t>
+          <t>Da Nang, Vietnam</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Xining</t>
+          <t>Da Nang</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Vietnam</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G263" t="inlineStr"/>
-      <c r="H263" t="inlineStr"/>
+          <t>VN</t>
+        </is>
+      </c>
+      <c r="G263" t="n">
+        <v>16.02636</v>
+      </c>
+      <c r="H263" t="n">
+        <v>108.20869</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>DAD</t>
+          <t>JXG</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Da Nang, Vietnam</t>
+          <t>Jiaxing, China</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Da Nang</t>
+          <t>Jiaxing</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>VN</t>
-        </is>
-      </c>
-      <c r="G264" t="n">
-        <v>16.02636</v>
-      </c>
-      <c r="H264" t="n">
-        <v>108.20869</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr"/>
+      <c r="H264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>JXG</t>
+          <t>CRK</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Jiaxing, China</t>
+          <t>Tarlac City, Philippines</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Jiaxing</t>
+          <t>Tarlac City</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G265" t="inlineStr"/>
-      <c r="H265" t="inlineStr"/>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="G265" t="n">
+        <v>15.1859</v>
+      </c>
+      <c r="H265" t="n">
+        <v>120.5599</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>CRK</t>
+          <t>PBH</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Tarlac City, Philippines</t>
+          <t>Thimphu, Bhutan</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -10389,73 +10393,69 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Tarlac City</t>
+          <t>Thimphu</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Bhutan</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>BT</t>
         </is>
       </c>
       <c r="G266" t="n">
-        <v>15.1859</v>
+        <v>27.4712</v>
       </c>
       <c r="H266" t="n">
-        <v>120.5599</v>
+        <v>89.6339</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>PBH</t>
+          <t>XIY</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Thimphu, Bhutan</t>
+          <t>Baoji, China</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Thimphu</t>
+          <t>Baoji</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Bhutan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>BT</t>
-        </is>
-      </c>
-      <c r="G267" t="n">
-        <v>27.4712</v>
-      </c>
-      <c r="H267" t="n">
-        <v>89.6339</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr"/>
+      <c r="H267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>XIY</t>
+          <t>CTU</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Baoji, China</t>
+          <t>Chengdu, China</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -10465,7 +10465,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Baoji</t>
+          <t>Chengdu</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
@@ -10484,118 +10484,122 @@
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>CTU</t>
+          <t>NQZ</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Chengdu, China</t>
+          <t>Astana, Kazakhstan</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Chengdu</t>
+          <t>Astana</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G269" t="inlineStr"/>
-      <c r="H269" t="inlineStr"/>
+          <t>KZ</t>
+        </is>
+      </c>
+      <c r="G269" t="n">
+        <v>51.167801</v>
+      </c>
+      <c r="H269" t="n">
+        <v>71.418893</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>NQZ</t>
+          <t>NNG</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Astana, Kazakhstan</t>
+          <t>Nanning, China</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Astana</t>
+          <t>Nanning</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G270" t="n">
-        <v>51.167801</v>
-      </c>
-      <c r="H270" t="n">
-        <v>71.418893</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G270" t="inlineStr"/>
+      <c r="H270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>NNG</t>
+          <t>KCH</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Nanning, China</t>
+          <t>Kuching, Malaysia</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Nanning</t>
+          <t>Kuching</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G271" t="inlineStr"/>
-      <c r="H271" t="inlineStr"/>
+          <t>MY</t>
+        </is>
+      </c>
+      <c r="G271" t="n">
+        <v>1.709727</v>
+      </c>
+      <c r="H271" t="n">
+        <v>110.353455</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>KCH</t>
+          <t>AKX</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Kuching, Malaysia</t>
+          <t>Aktobe, Kazakhstan</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -10605,107 +10609,107 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Kuching</t>
+          <t>Aktobe</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>MY</t>
+          <t>KZ</t>
         </is>
       </c>
       <c r="G272" t="n">
-        <v>1.709727</v>
+        <v>50.286922</v>
       </c>
       <c r="H272" t="n">
-        <v>110.353455</v>
+        <v>57.224121</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>AKX</t>
+          <t>TEN</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Aktobe, Kazakhstan</t>
+          <t>Tongren, China</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Aktobe</t>
+          <t>Tongren</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G273" t="n">
-        <v>50.286922</v>
-      </c>
-      <c r="H273" t="n">
-        <v>57.224121</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G273" t="inlineStr"/>
+      <c r="H273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>TEN</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Tongren, China</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Tongren</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G274" t="inlineStr"/>
-      <c r="H274" t="inlineStr"/>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="G274" t="n">
+        <v>38.94449997</v>
+      </c>
+      <c r="H274" t="n">
+        <v>-77.45580292</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10715,7 +10719,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -10729,21 +10733,21 @@
         </is>
       </c>
       <c r="G275" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H275" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10753,7 +10757,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -10767,21 +10771,21 @@
         </is>
       </c>
       <c r="G276" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="H276" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10791,7 +10795,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -10805,21 +10809,21 @@
         </is>
       </c>
       <c r="G277" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="H277" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10829,35 +10833,35 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G278" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="H278" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10867,35 +10871,35 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G279" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H279" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10905,7 +10909,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10919,21 +10923,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="H280" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10943,7 +10947,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10957,21 +10961,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H281" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -10981,7 +10985,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -10995,21 +10999,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H282" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11019,7 +11023,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11033,21 +11037,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H283" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11057,7 +11061,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11071,21 +11075,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H284" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11095,7 +11099,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11109,21 +11113,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H285" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11133,7 +11137,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11147,21 +11151,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H286" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11171,7 +11175,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11185,21 +11189,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="H287" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11209,7 +11213,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11223,21 +11227,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H288" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11247,7 +11251,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -11261,21 +11265,21 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H289" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11285,7 +11289,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11299,21 +11303,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="H290" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11323,7 +11327,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -11337,21 +11341,21 @@
         </is>
       </c>
       <c r="G291" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="H291" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11361,7 +11365,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>McAllen</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
@@ -11375,21 +11379,21 @@
         </is>
       </c>
       <c r="G292" t="n">
-        <v>33.94250107</v>
+        <v>26.17580032</v>
       </c>
       <c r="H292" t="n">
-        <v>-118.4079971</v>
+        <v>-98.23860168</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11399,7 +11403,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -11413,21 +11417,21 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H293" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11437,35 +11441,35 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G294" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H294" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11475,35 +11479,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H295" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11513,7 +11517,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11527,21 +11531,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H296" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11551,35 +11555,35 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G297" t="n">
-        <v>44.8819999695</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H297" t="n">
-        <v>-93.22180175779999</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11589,35 +11593,35 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G298" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H298" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11627,7 +11631,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
@@ -11641,21 +11645,21 @@
         </is>
       </c>
       <c r="G299" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H299" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11665,7 +11669,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -11679,21 +11683,21 @@
         </is>
       </c>
       <c r="G300" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H300" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11703,7 +11707,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11717,21 +11721,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H301" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11741,35 +11745,35 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G302" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H302" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11779,35 +11783,35 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G303" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H303" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11817,7 +11821,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -11831,21 +11835,21 @@
         </is>
       </c>
       <c r="G304" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="H304" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11855,7 +11859,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
@@ -11869,21 +11873,21 @@
         </is>
       </c>
       <c r="G305" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="H305" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11893,7 +11897,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11907,21 +11911,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="H306" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11931,35 +11935,35 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G307" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H307" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11969,35 +11973,35 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G308" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H308" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12007,7 +12011,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12021,21 +12025,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="H309" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12045,7 +12049,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -12059,21 +12063,21 @@
         </is>
       </c>
       <c r="G310" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H310" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12083,7 +12087,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -12097,21 +12101,21 @@
         </is>
       </c>
       <c r="G311" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H311" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12121,7 +12125,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
@@ -12135,21 +12139,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H312" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12159,35 +12163,35 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G313" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H313" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12197,35 +12201,35 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G314" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H314" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12235,12 +12239,12 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -12249,21 +12253,21 @@
         </is>
       </c>
       <c r="G315" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H315" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12273,12 +12277,12 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -12287,21 +12291,21 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H316" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12311,7 +12315,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12325,21 +12329,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H317" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12349,35 +12353,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H318" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12387,7 +12391,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
@@ -12401,21 +12405,21 @@
         </is>
       </c>
       <c r="G319" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="H319" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12425,7 +12429,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
@@ -12439,21 +12443,21 @@
         </is>
       </c>
       <c r="G320" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H320" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12463,35 +12467,35 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G321" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H321" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12501,35 +12505,35 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G322" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="H322" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12539,35 +12543,35 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="H323" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12577,7 +12581,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
@@ -12591,21 +12595,21 @@
         </is>
       </c>
       <c r="G324" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="H324" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12615,7 +12619,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12629,21 +12633,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="H325" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12653,35 +12657,35 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G326" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H326" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12691,35 +12695,35 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G327" t="n">
-        <v>20.5217990875</v>
+        <v>29.429461</v>
       </c>
       <c r="H327" t="n">
-        <v>-103.3109970093</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12729,7 +12733,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12743,21 +12747,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>29.429461</v>
+        <v>41.50069</v>
       </c>
       <c r="H328" t="n">
-        <v>-98.487061</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12767,7 +12771,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12781,21 +12785,21 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>41.50069</v>
+        <v>35.93543</v>
       </c>
       <c r="H329" t="n">
-        <v>-81.68411999999999</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -12805,7 +12809,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -12819,21 +12823,21 @@
         </is>
       </c>
       <c r="G330" t="n">
-        <v>35.93543</v>
+        <v>35.46655</v>
       </c>
       <c r="H330" t="n">
-        <v>-78.88075000000001</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -12843,7 +12847,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
@@ -12857,21 +12861,21 @@
         </is>
       </c>
       <c r="G331" t="n">
-        <v>35.46655</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H331" t="n">
-        <v>-97.65373</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -12881,7 +12885,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Anchorage</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
@@ -12895,21 +12899,21 @@
         </is>
       </c>
       <c r="G332" t="n">
-        <v>27.9755001068</v>
+        <v>61.158555</v>
       </c>
       <c r="H332" t="n">
-        <v>-82.533203125</v>
+        <v>-149.890208</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -12919,61 +12923,23 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G333" t="n">
-        <v>61.158555</v>
+        <v>44.64601</v>
       </c>
       <c r="H333" t="n">
-        <v>-149.890208</v>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334" s="1" t="inlineStr">
-        <is>
-          <t>YHZ</t>
-        </is>
-      </c>
-      <c r="B334" t="inlineStr">
-        <is>
-          <t>Halifax, Canada</t>
-        </is>
-      </c>
-      <c r="C334" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="D334" t="inlineStr">
-        <is>
-          <t>Halifax</t>
-        </is>
-      </c>
-      <c r="E334" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F334" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="G334" t="n">
-        <v>44.64601</v>
-      </c>
-      <c r="H334" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 094d9173b2091e651dd68a45a9231d8fb91e7161
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H331"/>
+  <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10162,118 +10162,122 @@
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>XNN</t>
+          <t>DAD</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Xining, China</t>
+          <t>Da Nang, Vietnam</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Xining</t>
+          <t>Da Nang</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Vietnam</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G260" t="inlineStr"/>
-      <c r="H260" t="inlineStr"/>
+          <t>VN</t>
+        </is>
+      </c>
+      <c r="G260" t="n">
+        <v>16.02636</v>
+      </c>
+      <c r="H260" t="n">
+        <v>108.20869</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>DAD</t>
+          <t>JXG</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Da Nang, Vietnam</t>
+          <t>Jiaxing, China</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Da Nang</t>
+          <t>Jiaxing</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>VN</t>
-        </is>
-      </c>
-      <c r="G261" t="n">
-        <v>16.02636</v>
-      </c>
-      <c r="H261" t="n">
-        <v>108.20869</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr"/>
+      <c r="H261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>JXG</t>
+          <t>CRK</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Jiaxing, China</t>
+          <t>Tarlac City, Philippines</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Jiaxing</t>
+          <t>Tarlac City</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G262" t="inlineStr"/>
-      <c r="H262" t="inlineStr"/>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="G262" t="n">
+        <v>15.1859</v>
+      </c>
+      <c r="H262" t="n">
+        <v>120.5599</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>CRK</t>
+          <t>PBH</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Tarlac City, Philippines</t>
+          <t>Thimphu, Bhutan</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -10283,73 +10287,69 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Tarlac City</t>
+          <t>Thimphu</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Bhutan</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>BT</t>
         </is>
       </c>
       <c r="G263" t="n">
-        <v>15.1859</v>
+        <v>27.4712</v>
       </c>
       <c r="H263" t="n">
-        <v>120.5599</v>
+        <v>89.6339</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>PBH</t>
+          <t>XIY</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Thimphu, Bhutan</t>
+          <t>Baoji, China</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Thimphu</t>
+          <t>Baoji</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Bhutan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>BT</t>
-        </is>
-      </c>
-      <c r="G264" t="n">
-        <v>27.4712</v>
-      </c>
-      <c r="H264" t="n">
-        <v>89.6339</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr"/>
+      <c r="H264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>XIY</t>
+          <t>CTU</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Baoji, China</t>
+          <t>Chengdu, China</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -10359,7 +10359,7 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Baoji</t>
+          <t>Chengdu</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
@@ -10378,118 +10378,122 @@
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>CTU</t>
+          <t>NQZ</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Chengdu, China</t>
+          <t>Astana, Kazakhstan</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Chengdu</t>
+          <t>Astana</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G266" t="inlineStr"/>
-      <c r="H266" t="inlineStr"/>
+          <t>KZ</t>
+        </is>
+      </c>
+      <c r="G266" t="n">
+        <v>51.167801</v>
+      </c>
+      <c r="H266" t="n">
+        <v>71.418893</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>NQZ</t>
+          <t>NNG</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Astana, Kazakhstan</t>
+          <t>Nanning, China</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Astana</t>
+          <t>Nanning</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G267" t="n">
-        <v>51.167801</v>
-      </c>
-      <c r="H267" t="n">
-        <v>71.418893</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr"/>
+      <c r="H267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>NNG</t>
+          <t>KCH</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Nanning, China</t>
+          <t>Kuching, Malaysia</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Nanning</t>
+          <t>Kuching</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G268" t="inlineStr"/>
-      <c r="H268" t="inlineStr"/>
+          <t>MY</t>
+        </is>
+      </c>
+      <c r="G268" t="n">
+        <v>1.709727</v>
+      </c>
+      <c r="H268" t="n">
+        <v>110.353455</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>KCH</t>
+          <t>AKX</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Kuching, Malaysia</t>
+          <t>Aktobe, Kazakhstan</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -10499,107 +10503,107 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Kuching</t>
+          <t>Aktobe</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>MY</t>
+          <t>KZ</t>
         </is>
       </c>
       <c r="G269" t="n">
-        <v>1.709727</v>
+        <v>50.286922</v>
       </c>
       <c r="H269" t="n">
-        <v>110.353455</v>
+        <v>57.224121</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>AKX</t>
+          <t>TEN</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Aktobe, Kazakhstan</t>
+          <t>Tongren, China</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Aktobe</t>
+          <t>Tongren</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G270" t="n">
-        <v>50.286922</v>
-      </c>
-      <c r="H270" t="n">
-        <v>57.224121</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G270" t="inlineStr"/>
+      <c r="H270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>TEN</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Tongren, China</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Tongren</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G271" t="inlineStr"/>
-      <c r="H271" t="inlineStr"/>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="G271" t="n">
+        <v>38.94449997</v>
+      </c>
+      <c r="H271" t="n">
+        <v>-77.45580292</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -10609,7 +10613,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
@@ -10623,21 +10627,21 @@
         </is>
       </c>
       <c r="G272" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H272" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -10647,7 +10651,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -10661,21 +10665,21 @@
         </is>
       </c>
       <c r="G273" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="H273" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -10685,7 +10689,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -10699,21 +10703,21 @@
         </is>
       </c>
       <c r="G274" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="H274" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10723,35 +10727,35 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G275" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="H275" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10761,35 +10765,35 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G276" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H276" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10799,7 +10803,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -10813,21 +10817,21 @@
         </is>
       </c>
       <c r="G277" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="H277" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10837,7 +10841,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -10851,21 +10855,21 @@
         </is>
       </c>
       <c r="G278" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H278" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10875,7 +10879,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -10889,21 +10893,21 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H279" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10913,7 +10917,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10927,21 +10931,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H280" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10951,7 +10955,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10965,21 +10969,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H281" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -10989,7 +10993,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -11003,21 +11007,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H282" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11027,7 +11031,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11041,21 +11045,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H283" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11065,7 +11069,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11079,21 +11083,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="H284" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11103,7 +11107,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11117,21 +11121,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H285" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11141,7 +11145,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11155,21 +11159,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H286" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11179,7 +11183,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11193,21 +11197,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="H287" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11217,7 +11221,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11231,21 +11235,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="H288" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11255,7 +11259,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>McAllen</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -11269,21 +11273,21 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>33.94250107</v>
+        <v>26.17580032</v>
       </c>
       <c r="H289" t="n">
-        <v>-118.4079971</v>
+        <v>-98.23860168</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11293,7 +11297,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11307,21 +11311,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H290" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11331,35 +11335,35 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G291" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H291" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11369,35 +11373,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H292" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11407,7 +11411,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -11421,21 +11425,21 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H293" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11445,35 +11449,35 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G294" t="n">
-        <v>44.8819999695</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H294" t="n">
-        <v>-93.22180175779999</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11483,35 +11487,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H295" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11521,7 +11525,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11535,21 +11539,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H296" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11559,7 +11563,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -11573,21 +11577,21 @@
         </is>
       </c>
       <c r="G297" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H297" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11597,7 +11601,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -11611,21 +11615,21 @@
         </is>
       </c>
       <c r="G298" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H298" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11635,35 +11639,35 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G299" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H299" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11673,35 +11677,35 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G300" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H300" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11711,7 +11715,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11725,21 +11729,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="H301" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11749,7 +11753,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -11763,21 +11767,21 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="H302" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11787,7 +11791,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -11801,21 +11805,21 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="H303" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11825,35 +11829,35 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G304" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H304" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11863,35 +11867,35 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H305" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11901,7 +11905,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11915,21 +11919,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="H306" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11939,7 +11943,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11953,21 +11957,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H307" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11977,7 +11981,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -11991,21 +11995,21 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H308" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12015,7 +12019,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12029,21 +12033,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H309" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12053,35 +12057,35 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G310" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H310" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12091,35 +12095,35 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G311" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H311" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12129,12 +12133,12 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -12143,21 +12147,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H312" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12167,12 +12171,12 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -12181,21 +12185,21 @@
         </is>
       </c>
       <c r="G313" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H313" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12205,7 +12209,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -12219,21 +12223,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H314" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12243,35 +12247,35 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G315" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H315" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12281,7 +12285,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -12295,21 +12299,21 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="H316" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12319,7 +12323,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12333,21 +12337,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H317" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12357,35 +12361,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H318" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12395,35 +12399,35 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G319" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="H319" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12433,35 +12437,35 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G320" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="H320" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12471,7 +12475,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -12485,21 +12489,21 @@
         </is>
       </c>
       <c r="G321" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="H321" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12509,7 +12513,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -12523,21 +12527,21 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="H322" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12547,35 +12551,35 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H323" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12585,35 +12589,35 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G324" t="n">
-        <v>20.5217990875</v>
+        <v>29.429461</v>
       </c>
       <c r="H324" t="n">
-        <v>-103.3109970093</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12623,7 +12627,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12637,21 +12641,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>29.429461</v>
+        <v>41.50069</v>
       </c>
       <c r="H325" t="n">
-        <v>-98.487061</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12661,7 +12665,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12675,21 +12679,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>41.50069</v>
+        <v>35.93543</v>
       </c>
       <c r="H326" t="n">
-        <v>-81.68411999999999</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12699,7 +12703,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12713,21 +12717,21 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>35.93543</v>
+        <v>35.46655</v>
       </c>
       <c r="H327" t="n">
-        <v>-78.88075000000001</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12737,7 +12741,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12751,21 +12755,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>35.46655</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H328" t="n">
-        <v>-97.65373</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12775,7 +12779,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Anchorage</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12789,21 +12793,21 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>27.9755001068</v>
+        <v>61.158555</v>
       </c>
       <c r="H329" t="n">
-        <v>-82.533203125</v>
+        <v>-149.890208</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -12813,61 +12817,23 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G330" t="n">
-        <v>61.158555</v>
+        <v>44.64601</v>
       </c>
       <c r="H330" t="n">
-        <v>-149.890208</v>
-      </c>
-    </row>
-    <row r="331">
-      <c r="A331" s="1" t="inlineStr">
-        <is>
-          <t>YHZ</t>
-        </is>
-      </c>
-      <c r="B331" t="inlineStr">
-        <is>
-          <t>Halifax, Canada</t>
-        </is>
-      </c>
-      <c r="C331" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="D331" t="inlineStr">
-        <is>
-          <t>Halifax</t>
-        </is>
-      </c>
-      <c r="E331" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F331" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="G331" t="n">
-        <v>44.64601</v>
-      </c>
-      <c r="H331" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 23de733e02812f50b212a387e897caed819081b9
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H331"/>
+  <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8684,46 +8684,46 @@
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>LHW</t>
+          <t>MFM</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Lanzhou, China</t>
+          <t>Macau</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Lanzhou</t>
-        </is>
-      </c>
-      <c r="E219" t="inlineStr">
-        <is>
-          <t>China</t>
-        </is>
-      </c>
+          <t>Macau</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr"/>
       <c r="F219" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G219" t="inlineStr"/>
-      <c r="H219" t="inlineStr"/>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="G219" t="n">
+        <v>22.1495990753</v>
+      </c>
+      <c r="H219" t="n">
+        <v>113.592002869</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>MFM</t>
+          <t>MLE</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Macau</t>
+          <t>Male, Maldives</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -8733,31 +8733,35 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>Macau</t>
-        </is>
-      </c>
-      <c r="E220" t="inlineStr"/>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Maldives</t>
+        </is>
+      </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MV</t>
         </is>
       </c>
       <c r="G220" t="n">
-        <v>22.1495990753</v>
+        <v>4.1748</v>
       </c>
       <c r="H220" t="n">
-        <v>113.592002869</v>
+        <v>73.50888</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>MLE</t>
+          <t>MNL</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Male, Maldives</t>
+          <t>Manila, Philippines</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -8767,35 +8771,35 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Manila</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>Maldives</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>MV</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="G221" t="n">
-        <v>4.1748</v>
+        <v>14.508600235</v>
       </c>
       <c r="H221" t="n">
-        <v>73.50888</v>
+        <v>121.019996643</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>MNL</t>
+          <t>BOM</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Manila, Philippines</t>
+          <t>Mumbai, India</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -8805,35 +8809,35 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Manila</t>
+          <t>Mumbai</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G222" t="n">
-        <v>14.508600235</v>
+        <v>19.0886993408</v>
       </c>
       <c r="H222" t="n">
-        <v>121.019996643</v>
+        <v>72.8678970337</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>BOM</t>
+          <t>NAG</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Mumbai, India</t>
+          <t>Nagpur, India</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -8843,7 +8847,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Nagpur</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
@@ -8857,21 +8861,21 @@
         </is>
       </c>
       <c r="G223" t="n">
-        <v>19.0886993408</v>
+        <v>21.1610714</v>
       </c>
       <c r="H223" t="n">
-        <v>72.8678970337</v>
+        <v>79.0024702</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>NAG</t>
+          <t>OKA</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Nagpur, India</t>
+          <t>Naha, Japan</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -8881,35 +8885,35 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>Nagpur</t>
+          <t>Naha</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="G224" t="n">
-        <v>21.1610714</v>
+        <v>26.1958</v>
       </c>
       <c r="H224" t="n">
-        <v>79.0024702</v>
+        <v>127.646</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>OKA</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Naha, Japan</t>
+          <t>New Delhi, India</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -8919,35 +8923,35 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>Naha</t>
+          <t>New Delhi</t>
         </is>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G225" t="n">
-        <v>26.1958</v>
+        <v>28.5664997101</v>
       </c>
       <c r="H225" t="n">
-        <v>127.646</v>
+        <v>77.1031036377</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>DEL</t>
+          <t>KIX</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>New Delhi, India</t>
+          <t>Osaka, Japan</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -8957,35 +8961,35 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>New Delhi</t>
+          <t>Osaka</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="G226" t="n">
-        <v>28.5664997101</v>
+        <v>34.4272994995</v>
       </c>
       <c r="H226" t="n">
-        <v>77.1031036377</v>
+        <v>135.244003296</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>KIX</t>
+          <t>PAT</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Osaka, Japan</t>
+          <t>Patna, India</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -8995,35 +8999,35 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Osaka</t>
+          <t>Patna</t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G227" t="n">
-        <v>34.4272994995</v>
+        <v>25.591299057</v>
       </c>
       <c r="H227" t="n">
-        <v>135.244003296</v>
+        <v>85.0879974365</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>PAT</t>
+          <t>PNH</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Patna, India</t>
+          <t>Phnom Penh, Cambodia</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -9033,179 +9037,179 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Patna</t>
+          <t>Phnom Penh</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Cambodia</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>KH</t>
         </is>
       </c>
       <c r="G228" t="n">
-        <v>25.591299057</v>
+        <v>11.5466003418</v>
       </c>
       <c r="H228" t="n">
-        <v>85.0879974365</v>
+        <v>104.84400177</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>PNH</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Phnom Penh, Cambodia</t>
+          <t>Qingdao, China</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Phnom Penh</t>
+          <t>Qingdao</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Cambodia</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>KH</t>
-        </is>
-      </c>
-      <c r="G229" t="n">
-        <v>11.5466003418</v>
-      </c>
-      <c r="H229" t="n">
-        <v>104.84400177</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr"/>
+      <c r="H229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>ICN</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Qingdao, China</t>
+          <t>Seoul, South Korea</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Qingdao</t>
+          <t>Seoul</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G230" t="inlineStr"/>
-      <c r="H230" t="inlineStr"/>
+          <t>KR</t>
+        </is>
+      </c>
+      <c r="G230" t="n">
+        <v>37.4691009521</v>
+      </c>
+      <c r="H230" t="n">
+        <v>126.450996399</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>ICN</t>
+          <t>SHA</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Seoul, South Korea</t>
+          <t>Shanghai, China</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>Seoul</t>
+          <t>Shanghai</t>
         </is>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>KR</t>
-        </is>
-      </c>
-      <c r="G231" t="n">
-        <v>37.4691009521</v>
-      </c>
-      <c r="H231" t="n">
-        <v>126.450996399</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr"/>
+      <c r="H231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>SHA</t>
+          <t>SIN</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Shanghai, China</t>
+          <t>Singapore, Singapore</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Shanghai</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G232" t="inlineStr"/>
-      <c r="H232" t="inlineStr"/>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="G232" t="n">
+        <v>1.3501900434</v>
+      </c>
+      <c r="H232" t="n">
+        <v>103.994003296</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>SIN</t>
+          <t>URT</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Singapore, Singapore</t>
+          <t>Surat Thani, Thailand</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -9215,35 +9219,35 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Surat Thani</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>SG</t>
+          <t>TH</t>
         </is>
       </c>
       <c r="G233" t="n">
-        <v>1.3501900434</v>
+        <v>9.1325998306</v>
       </c>
       <c r="H233" t="n">
-        <v>103.994003296</v>
+        <v>99.135597229</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>URT</t>
+          <t>TPE</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Surat Thani, Thailand</t>
+          <t>Taipei</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -9253,35 +9257,31 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Surat Thani</t>
-        </is>
-      </c>
-      <c r="E234" t="inlineStr">
-        <is>
-          <t>Thailand</t>
-        </is>
-      </c>
+          <t>Taipei</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr"/>
       <c r="F234" t="inlineStr">
         <is>
-          <t>TH</t>
+          <t>TW</t>
         </is>
       </c>
       <c r="G234" t="n">
-        <v>9.1325998306</v>
+        <v>25.0776996613</v>
       </c>
       <c r="H234" t="n">
-        <v>99.135597229</v>
+        <v>121.233001709</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>TPE</t>
+          <t>NRT</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Taipei</t>
+          <t>Tokyo, Japan</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -9291,31 +9291,35 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Taipei</t>
-        </is>
-      </c>
-      <c r="E235" t="inlineStr"/>
+          <t>Tokyo</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>TW</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="G235" t="n">
-        <v>25.0776996613</v>
+        <v>35.7647018433</v>
       </c>
       <c r="H235" t="n">
-        <v>121.233001709</v>
+        <v>140.386001587</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>NRT</t>
+          <t>ULN</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Tokyo, Japan</t>
+          <t>Ulaanbaatar, Mongolia</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -9325,35 +9329,35 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>Tokyo</t>
+          <t>Ulaanbaatar</t>
         </is>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Mongolia</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="G236" t="n">
-        <v>35.7647018433</v>
+        <v>47.8431015015</v>
       </c>
       <c r="H236" t="n">
-        <v>140.386001587</v>
+        <v>106.766998291</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>ULN</t>
+          <t>VTE</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Ulaanbaatar, Mongolia</t>
+          <t>Vientiane, Laos</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -9363,217 +9367,217 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>Ulaanbaatar</t>
+          <t>Vientiane</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Mongolia</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>LA</t>
         </is>
       </c>
       <c r="G237" t="n">
-        <v>47.8431015015</v>
+        <v>17.9757</v>
       </c>
       <c r="H237" t="n">
-        <v>106.766998291</v>
+        <v>102.5683</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>VTE</t>
+          <t>KHN</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Vientiane, Laos</t>
+          <t>Nanchang, China</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>Vientiane</t>
+          <t>Nanchang</t>
         </is>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Laos</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>LA</t>
-        </is>
-      </c>
-      <c r="G238" t="n">
-        <v>17.9757</v>
-      </c>
-      <c r="H238" t="n">
-        <v>102.5683</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G238" t="inlineStr"/>
+      <c r="H238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>KHN</t>
+          <t>EVN</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Nanchang, China</t>
+          <t>Yerevan, Armenia</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>Nanchang</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Armenia</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G239" t="inlineStr"/>
-      <c r="H239" t="inlineStr"/>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="G239" t="n">
+        <v>40.1473007202</v>
+      </c>
+      <c r="H239" t="n">
+        <v>44.3959007263</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>EVN</t>
+          <t>JOG</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Yerevan, Armenia</t>
+          <t>Yogyakarta, Indonesia</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>Yerevan</t>
+          <t>Yogyakarta</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>Armenia</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>AM</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="G240" t="n">
-        <v>40.1473007202</v>
+        <v>-7.7881798744</v>
       </c>
       <c r="H240" t="n">
-        <v>44.3959007263</v>
+        <v>110.4319992065</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>JOG</t>
+          <t>ZGN</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Yogyakarta, Indonesia</t>
+          <t>Zhongshan, China</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Yogyakarta</t>
+          <t>Zhongshan</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="G241" t="n">
-        <v>-7.7881798744</v>
-      </c>
-      <c r="H241" t="n">
-        <v>110.4319992065</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr"/>
+      <c r="H241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>ZGN</t>
+          <t>CGY</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Zhongshan, China</t>
+          <t>Cagayan de Oro, Philippines</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Zhongshan</t>
+          <t>Cagayan de Oro</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G242" t="inlineStr"/>
-      <c r="H242" t="inlineStr"/>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="G242" t="n">
+        <v>8.415619850200001</v>
+      </c>
+      <c r="H242" t="n">
+        <v>124.611000061</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>CGY</t>
+          <t>COK</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Cagayan de Oro, Philippines</t>
+          <t>Kochi, India</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -9583,35 +9587,35 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Cagayan de Oro</t>
+          <t>Kochi</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G243" t="n">
-        <v>8.415619850200001</v>
+        <v>9.9312</v>
       </c>
       <c r="H243" t="n">
-        <v>124.611000061</v>
+        <v>76.26730000000001</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>DPS</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Kochi, India</t>
+          <t>Denpasar, Indonesia</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -9621,35 +9625,35 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>Kochi</t>
+          <t>Denpasar</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="G244" t="n">
-        <v>9.9312</v>
+        <v>-8.748169899000001</v>
       </c>
       <c r="H244" t="n">
-        <v>76.26730000000001</v>
+        <v>115.1669998169</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>DPS</t>
+          <t>CNN</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Denpasar, Indonesia</t>
+          <t>Kannur, India</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -9659,73 +9663,69 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Denpasar</t>
+          <t>Kannur</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G245" t="n">
-        <v>-8.748169899000001</v>
+        <v>11.915858</v>
       </c>
       <c r="H245" t="n">
-        <v>115.1669998169</v>
+        <v>75.55094</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>CNN</t>
+          <t>SZX</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Kannur, India</t>
+          <t>Shenzhen, China</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Kannur</t>
+          <t>Shenzhen</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="G246" t="n">
-        <v>11.915858</v>
-      </c>
-      <c r="H246" t="n">
-        <v>75.55094</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr"/>
+      <c r="H246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>SZX</t>
+          <t>KWE</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Shenzhen, China</t>
+          <t>Guiyang, China</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -9735,7 +9735,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Shenzhen</t>
+          <t>Guiyang</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
@@ -9754,12 +9754,12 @@
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>KWE</t>
+          <t>HGH</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Guiyang, China</t>
+          <t>Shaoxing, China</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -9769,7 +9769,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Guiyang</t>
+          <t>Shaoxing</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -9788,12 +9788,12 @@
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>HGH</t>
+          <t>CZX</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Shaoxing, China</t>
+          <t>Changzhou, China</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -9803,7 +9803,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Shaoxing</t>
+          <t>Changzhou</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -9822,12 +9822,12 @@
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>CZX</t>
+          <t>KMG</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Changzhou, China</t>
+          <t>Kunming, China</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -9837,7 +9837,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Changzhou</t>
+          <t>Kunming</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
@@ -9856,84 +9856,84 @@
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>KMG</t>
+          <t>CNX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Kunming, China</t>
+          <t>Chiang Mai, Thailand</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Kunming</t>
+          <t>Chiang Mai</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G251" t="inlineStr"/>
-      <c r="H251" t="inlineStr"/>
+          <t>TH</t>
+        </is>
+      </c>
+      <c r="G251" t="n">
+        <v>18.7667999268</v>
+      </c>
+      <c r="H251" t="n">
+        <v>98.962600708</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>CNX</t>
+          <t>CGO</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Chiang Mai, Thailand</t>
+          <t>Zhengzhou, China</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>Chiang Mai</t>
+          <t>Zhengzhou</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>TH</t>
-        </is>
-      </c>
-      <c r="G252" t="n">
-        <v>18.7667999268</v>
-      </c>
-      <c r="H252" t="n">
-        <v>98.962600708</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr"/>
+      <c r="H252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>CGO</t>
+          <t>TYN</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Zhengzhou, China</t>
+          <t>Yangquan, China</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -9943,7 +9943,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>Zhengzhou</t>
+          <t>Yangquan</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
@@ -9962,12 +9962,12 @@
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>TYN</t>
+          <t>CSX</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Yangquan, China</t>
+          <t>Changsha, China</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -9977,7 +9977,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Yangquan</t>
+          <t>Changsha</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
@@ -9996,12 +9996,12 @@
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>CSX</t>
+          <t>DLC</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Changsha, China</t>
+          <t>Dalian, China</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -10011,7 +10011,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Changsha</t>
+          <t>Dalian</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
@@ -10030,12 +10030,12 @@
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>DLC</t>
+          <t>BHY</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Dalian, China</t>
+          <t>Beihai, China</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -10045,7 +10045,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Dalian</t>
+          <t>Beihai</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
@@ -10064,12 +10064,12 @@
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>BHY</t>
+          <t>CKG</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Beihai, China</t>
+          <t>Chongqing, China</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -10079,7 +10079,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Beihai</t>
+          <t>Chongqing</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
@@ -10098,12 +10098,12 @@
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>CKG</t>
+          <t>XFN</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Chongqing, China</t>
+          <t>Xiangyang, China</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -10113,7 +10113,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Chongqing</t>
+          <t>Xiangyang</t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
@@ -10132,118 +10132,122 @@
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>XFN</t>
+          <t>DAD</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Xiangyang, China</t>
+          <t>Da Nang, Vietnam</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Xiangyang</t>
+          <t>Da Nang</t>
         </is>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Vietnam</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G259" t="inlineStr"/>
-      <c r="H259" t="inlineStr"/>
+          <t>VN</t>
+        </is>
+      </c>
+      <c r="G259" t="n">
+        <v>16.02636</v>
+      </c>
+      <c r="H259" t="n">
+        <v>108.20869</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>DAD</t>
+          <t>JXG</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Da Nang, Vietnam</t>
+          <t>Jiaxing, China</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Da Nang</t>
+          <t>Jiaxing</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>VN</t>
-        </is>
-      </c>
-      <c r="G260" t="n">
-        <v>16.02636</v>
-      </c>
-      <c r="H260" t="n">
-        <v>108.20869</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr"/>
+      <c r="H260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>JXG</t>
+          <t>CRK</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Jiaxing, China</t>
+          <t>Tarlac City, Philippines</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Jiaxing</t>
+          <t>Tarlac City</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G261" t="inlineStr"/>
-      <c r="H261" t="inlineStr"/>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="G261" t="n">
+        <v>15.1859</v>
+      </c>
+      <c r="H261" t="n">
+        <v>120.5599</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>CRK</t>
+          <t>PBH</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Tarlac City, Philippines</t>
+          <t>Thimphu, Bhutan</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -10253,73 +10257,69 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Tarlac City</t>
+          <t>Thimphu</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Bhutan</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>BT</t>
         </is>
       </c>
       <c r="G262" t="n">
-        <v>15.1859</v>
+        <v>27.4712</v>
       </c>
       <c r="H262" t="n">
-        <v>120.5599</v>
+        <v>89.6339</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>PBH</t>
+          <t>XIY</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Thimphu, Bhutan</t>
+          <t>Baoji, China</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Thimphu</t>
+          <t>Baoji</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>Bhutan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>BT</t>
-        </is>
-      </c>
-      <c r="G263" t="n">
-        <v>27.4712</v>
-      </c>
-      <c r="H263" t="n">
-        <v>89.6339</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr"/>
+      <c r="H263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>XIY</t>
+          <t>CTU</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Baoji, China</t>
+          <t>Chengdu, China</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -10329,7 +10329,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Baoji</t>
+          <t>Chengdu</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
@@ -10348,118 +10348,122 @@
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>CTU</t>
+          <t>NQZ</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Chengdu, China</t>
+          <t>Astana, Kazakhstan</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Chengdu</t>
+          <t>Astana</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G265" t="inlineStr"/>
-      <c r="H265" t="inlineStr"/>
+          <t>KZ</t>
+        </is>
+      </c>
+      <c r="G265" t="n">
+        <v>51.167801</v>
+      </c>
+      <c r="H265" t="n">
+        <v>71.418893</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>NQZ</t>
+          <t>NNG</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Astana, Kazakhstan</t>
+          <t>Nanning, China</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Astana</t>
+          <t>Nanning</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G266" t="n">
-        <v>51.167801</v>
-      </c>
-      <c r="H266" t="n">
-        <v>71.418893</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr"/>
+      <c r="H266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>NNG</t>
+          <t>KCH</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Nanning, China</t>
+          <t>Kuching, Malaysia</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Nanning</t>
+          <t>Kuching</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G267" t="inlineStr"/>
-      <c r="H267" t="inlineStr"/>
+          <t>MY</t>
+        </is>
+      </c>
+      <c r="G267" t="n">
+        <v>1.709727</v>
+      </c>
+      <c r="H267" t="n">
+        <v>110.353455</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>KCH</t>
+          <t>AKX</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Kuching, Malaysia</t>
+          <t>Aktobe, Kazakhstan</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -10469,73 +10473,69 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Kuching</t>
+          <t>Aktobe</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>MY</t>
+          <t>KZ</t>
         </is>
       </c>
       <c r="G268" t="n">
-        <v>1.709727</v>
+        <v>50.286922</v>
       </c>
       <c r="H268" t="n">
-        <v>110.353455</v>
+        <v>57.224121</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>AKX</t>
+          <t>TEN</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Aktobe, Kazakhstan</t>
+          <t>Tongren, China</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Aktobe</t>
+          <t>Tongren</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G269" t="n">
-        <v>50.286922</v>
-      </c>
-      <c r="H269" t="n">
-        <v>57.224121</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr"/>
+      <c r="H269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>TEN</t>
+          <t>HYN</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Tongren, China</t>
+          <t>Taizhou, China</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -10545,7 +10545,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Tongren</t>
+          <t>Taizhou</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
@@ -10564,46 +10564,50 @@
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>HYN</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Taizhou, China</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Taizhou</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G271" t="inlineStr"/>
-      <c r="H271" t="inlineStr"/>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="G271" t="n">
+        <v>38.94449997</v>
+      </c>
+      <c r="H271" t="n">
+        <v>-77.45580292</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -10613,7 +10617,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
@@ -10627,21 +10631,21 @@
         </is>
       </c>
       <c r="G272" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H272" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -10651,7 +10655,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -10665,21 +10669,21 @@
         </is>
       </c>
       <c r="G273" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="H273" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -10689,7 +10693,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -10703,21 +10707,21 @@
         </is>
       </c>
       <c r="G274" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="H274" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10727,35 +10731,35 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G275" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="H275" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10765,35 +10769,35 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G276" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H276" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10803,7 +10807,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -10817,21 +10821,21 @@
         </is>
       </c>
       <c r="G277" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="H277" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10841,7 +10845,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -10855,21 +10859,21 @@
         </is>
       </c>
       <c r="G278" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H278" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10879,7 +10883,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -10893,21 +10897,21 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H279" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10917,7 +10921,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10931,21 +10935,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H280" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10955,7 +10959,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10969,21 +10973,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H281" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -10993,7 +10997,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -11007,21 +11011,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H282" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11031,7 +11035,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11045,21 +11049,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H283" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11069,7 +11073,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11083,21 +11087,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="H284" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11107,7 +11111,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11121,21 +11125,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H285" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11145,7 +11149,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11159,21 +11163,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H286" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11183,7 +11187,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11197,21 +11201,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="H287" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11221,7 +11225,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11235,21 +11239,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="H288" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11259,7 +11263,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>McAllen</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -11273,21 +11277,21 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>33.94250107</v>
+        <v>26.17580032</v>
       </c>
       <c r="H289" t="n">
-        <v>-118.4079971</v>
+        <v>-98.23860168</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11297,7 +11301,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11311,21 +11315,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H290" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11335,35 +11339,35 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G291" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H291" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11373,35 +11377,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H292" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11411,7 +11415,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -11425,21 +11429,21 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H293" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11449,35 +11453,35 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G294" t="n">
-        <v>44.8819999695</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H294" t="n">
-        <v>-93.22180175779999</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11487,35 +11491,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H295" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11525,7 +11529,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11539,21 +11543,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H296" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11563,7 +11567,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -11577,21 +11581,21 @@
         </is>
       </c>
       <c r="G297" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H297" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11601,7 +11605,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -11615,21 +11619,21 @@
         </is>
       </c>
       <c r="G298" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H298" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11639,35 +11643,35 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G299" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H299" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11677,35 +11681,35 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G300" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H300" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11715,7 +11719,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11729,21 +11733,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="H301" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11753,7 +11757,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -11767,21 +11771,21 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="H302" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11791,7 +11795,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -11805,21 +11809,21 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="H303" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11829,35 +11833,35 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G304" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H304" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11867,35 +11871,35 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H305" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11905,7 +11909,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11919,21 +11923,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="H306" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11943,7 +11947,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11957,21 +11961,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H307" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11981,7 +11985,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -11995,21 +11999,21 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H308" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12019,7 +12023,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12033,21 +12037,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H309" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12057,35 +12061,35 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G310" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H310" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12095,35 +12099,35 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G311" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H311" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12133,12 +12137,12 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -12147,21 +12151,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H312" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12171,12 +12175,12 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -12185,21 +12189,21 @@
         </is>
       </c>
       <c r="G313" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H313" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12209,7 +12213,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -12223,21 +12227,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H314" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12247,35 +12251,35 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G315" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H315" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12285,7 +12289,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -12299,21 +12303,21 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="H316" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12323,7 +12327,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12337,21 +12341,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H317" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12361,35 +12365,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H318" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12399,35 +12403,35 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G319" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="H319" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12437,35 +12441,35 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G320" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="H320" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12475,7 +12479,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -12489,21 +12493,21 @@
         </is>
       </c>
       <c r="G321" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="H321" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12513,7 +12517,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -12527,21 +12531,21 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="H322" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12551,35 +12555,35 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H323" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12589,35 +12593,35 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G324" t="n">
-        <v>20.5217990875</v>
+        <v>29.429461</v>
       </c>
       <c r="H324" t="n">
-        <v>-103.3109970093</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12627,7 +12631,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12641,21 +12645,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>29.429461</v>
+        <v>41.50069</v>
       </c>
       <c r="H325" t="n">
-        <v>-98.487061</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12665,7 +12669,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12679,21 +12683,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>41.50069</v>
+        <v>35.93543</v>
       </c>
       <c r="H326" t="n">
-        <v>-81.68411999999999</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12703,7 +12707,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12717,21 +12721,21 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>35.93543</v>
+        <v>35.46655</v>
       </c>
       <c r="H327" t="n">
-        <v>-78.88075000000001</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12741,7 +12745,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12755,21 +12759,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>35.46655</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H328" t="n">
-        <v>-97.65373</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12779,7 +12783,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Anchorage</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12793,21 +12797,21 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>27.9755001068</v>
+        <v>61.158555</v>
       </c>
       <c r="H329" t="n">
-        <v>-82.533203125</v>
+        <v>-149.890208</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -12817,61 +12821,23 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G330" t="n">
-        <v>61.158555</v>
+        <v>44.64601</v>
       </c>
       <c r="H330" t="n">
-        <v>-149.890208</v>
-      </c>
-    </row>
-    <row r="331">
-      <c r="A331" s="1" t="inlineStr">
-        <is>
-          <t>YHZ</t>
-        </is>
-      </c>
-      <c r="B331" t="inlineStr">
-        <is>
-          <t>Halifax, Canada</t>
-        </is>
-      </c>
-      <c r="C331" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="D331" t="inlineStr">
-        <is>
-          <t>Halifax</t>
-        </is>
-      </c>
-      <c r="E331" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F331" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="G331" t="n">
-        <v>44.64601</v>
-      </c>
-      <c r="H331" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 7439dae34e14ad8e4c91944b22d4e4526001204b
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -2497,7 +2497,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Zürich, Switzerland</t>
+          <t>Zurich, Switzerland</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -4165,7 +4165,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Bogotá, Colombia</t>
+          <t>Bogota, Colombia</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -8059,7 +8059,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Hengshui, China</t>
+          <t>Shijiazhuang, China</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -8069,7 +8069,7 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>Hengshui</t>
+          <t>Shijiazhuang</t>
         </is>
       </c>
       <c r="E202" t="inlineStr">

</xml_diff>

<commit_message>
update generated data Triggered by 0fd53f7a457f148358be08d096c0c2e98660524a
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H330"/>
+  <dimension ref="A1:H331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10564,50 +10564,46 @@
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>XNN</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Xining, China</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Xining</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="G271" t="n">
-        <v>38.94449997</v>
-      </c>
-      <c r="H271" t="n">
-        <v>-77.45580292</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G271" t="inlineStr"/>
+      <c r="H271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -10617,7 +10613,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
@@ -10631,21 +10627,21 @@
         </is>
       </c>
       <c r="G272" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="H272" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -10655,7 +10651,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -10669,21 +10665,21 @@
         </is>
       </c>
       <c r="G273" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H273" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -10693,7 +10689,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -10707,21 +10703,21 @@
         </is>
       </c>
       <c r="G274" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="H274" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10731,35 +10727,35 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G275" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="H275" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10769,35 +10765,35 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G276" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="H276" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10807,7 +10803,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -10821,21 +10817,21 @@
         </is>
       </c>
       <c r="G277" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H277" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10845,7 +10841,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -10859,21 +10855,21 @@
         </is>
       </c>
       <c r="G278" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="H278" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10883,7 +10879,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -10897,21 +10893,21 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H279" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10921,7 +10917,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10935,21 +10931,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H280" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10959,7 +10955,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10973,21 +10969,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H281" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -10997,7 +10993,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -11011,21 +11007,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H282" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11035,7 +11031,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11049,21 +11045,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H283" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11073,7 +11069,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11087,21 +11083,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H284" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11111,7 +11107,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11125,21 +11121,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="H285" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11149,7 +11145,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11163,21 +11159,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H286" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11187,7 +11183,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11201,21 +11197,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H287" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11225,7 +11221,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11239,21 +11235,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="H288" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11263,7 +11259,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -11277,21 +11273,21 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="H289" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11301,7 +11297,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11315,21 +11311,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="H290" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11339,35 +11335,35 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G291" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H291" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11377,35 +11373,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H292" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11415,7 +11411,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -11429,21 +11425,21 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H293" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11453,35 +11449,35 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G294" t="n">
-        <v>45.4706001282</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H294" t="n">
-        <v>-73.7407989502</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11491,35 +11487,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H295" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11529,7 +11525,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11543,21 +11539,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H296" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11567,7 +11563,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -11581,21 +11577,21 @@
         </is>
       </c>
       <c r="G297" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H297" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11605,7 +11601,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -11619,21 +11615,21 @@
         </is>
       </c>
       <c r="G298" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H298" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11643,35 +11639,35 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G299" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H299" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11681,35 +11677,35 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G300" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H300" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11719,7 +11715,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11733,21 +11729,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H301" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11757,7 +11753,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -11771,21 +11767,21 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="H302" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11795,7 +11791,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -11809,21 +11805,21 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="H303" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11833,35 +11829,35 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G304" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="H304" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11871,35 +11867,35 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H305" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11909,7 +11905,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11923,21 +11919,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H306" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11947,7 +11943,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11961,21 +11957,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="H307" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11985,7 +11981,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -11999,21 +11995,21 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H308" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12023,7 +12019,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12037,21 +12033,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H309" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12061,35 +12057,35 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G310" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H310" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12099,35 +12095,35 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G311" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H311" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12137,12 +12133,12 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -12151,21 +12147,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H312" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12175,12 +12171,12 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -12189,21 +12185,21 @@
         </is>
       </c>
       <c r="G313" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H313" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12213,7 +12209,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -12227,21 +12223,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H314" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12251,35 +12247,35 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G315" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H315" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12289,7 +12285,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -12303,21 +12299,21 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H316" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12327,7 +12323,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12341,21 +12337,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="H317" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12365,35 +12361,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H318" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12403,35 +12399,35 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G319" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H319" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12441,35 +12437,35 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G320" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="H320" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12479,7 +12475,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -12493,21 +12489,21 @@
         </is>
       </c>
       <c r="G321" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="H321" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12517,7 +12513,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -12531,21 +12527,21 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="H322" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12555,35 +12551,35 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="H323" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12593,35 +12589,35 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G324" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H324" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12631,7 +12627,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12645,21 +12641,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>41.50069</v>
+        <v>29.429461</v>
       </c>
       <c r="H325" t="n">
-        <v>-81.68411999999999</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12669,7 +12665,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12683,21 +12679,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>35.93543</v>
+        <v>41.50069</v>
       </c>
       <c r="H326" t="n">
-        <v>-78.88075000000001</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12707,7 +12703,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12721,21 +12717,21 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>35.46655</v>
+        <v>35.93543</v>
       </c>
       <c r="H327" t="n">
-        <v>-97.65373</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12745,7 +12741,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12759,21 +12755,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>27.9755001068</v>
+        <v>35.46655</v>
       </c>
       <c r="H328" t="n">
-        <v>-82.533203125</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12783,7 +12779,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12797,47 +12793,85 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>61.158555</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H329" t="n">
-        <v>-149.890208</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
+          <t>ANC</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Anchorage, United States</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Anchorage</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="G330" t="n">
+        <v>61.158555</v>
+      </c>
+      <c r="H330" t="n">
+        <v>-149.890208</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="inlineStr">
+        <is>
           <t>YHZ</t>
         </is>
       </c>
-      <c r="B330" t="inlineStr">
+      <c r="B331" t="inlineStr">
         <is>
           <t>Halifax, Canada</t>
         </is>
       </c>
-      <c r="C330" t="inlineStr">
+      <c r="C331" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="D330" t="inlineStr">
+      <c r="D331" t="inlineStr">
         <is>
           <t>Halifax</t>
         </is>
       </c>
-      <c r="E330" t="inlineStr">
+      <c r="E331" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="F330" t="inlineStr">
+      <c r="F331" t="inlineStr">
         <is>
           <t>CA</t>
         </is>
       </c>
-      <c r="G330" t="n">
+      <c r="G331" t="n">
         <v>44.64601</v>
       </c>
-      <c r="H330" t="n">
+      <c r="H331" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by c6638db983ec6825bf535f11be7ba4673c9eab41
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H330"/>
+  <dimension ref="A1:H331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10560,50 +10560,50 @@
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Bishkek, Kyrgyzstan</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Bishkek</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>KG</t>
         </is>
       </c>
       <c r="G271" t="n">
-        <v>38.94449997</v>
+        <v>42.875608</v>
       </c>
       <c r="H271" t="n">
-        <v>-77.45580292</v>
+        <v>74.604613</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -10613,7 +10613,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
@@ -10627,21 +10627,21 @@
         </is>
       </c>
       <c r="G272" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="H272" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -10651,7 +10651,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -10665,21 +10665,21 @@
         </is>
       </c>
       <c r="G273" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H273" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -10689,7 +10689,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -10703,21 +10703,21 @@
         </is>
       </c>
       <c r="G274" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="H274" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10727,35 +10727,35 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G275" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="H275" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10765,35 +10765,35 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G276" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="H276" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10803,7 +10803,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -10817,21 +10817,21 @@
         </is>
       </c>
       <c r="G277" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H277" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10841,7 +10841,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -10855,21 +10855,21 @@
         </is>
       </c>
       <c r="G278" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="H278" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10879,7 +10879,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -10893,21 +10893,21 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H279" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10917,7 +10917,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10931,21 +10931,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H280" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10955,7 +10955,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10969,21 +10969,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H281" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -10993,7 +10993,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -11007,21 +11007,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H282" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11031,7 +11031,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11045,21 +11045,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H283" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11069,7 +11069,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11083,21 +11083,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H284" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11107,7 +11107,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11121,21 +11121,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="H285" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11145,7 +11145,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11159,21 +11159,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H286" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11183,7 +11183,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11197,21 +11197,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H287" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11221,7 +11221,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11235,21 +11235,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="H288" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11259,7 +11259,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -11273,21 +11273,21 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>26.17580032</v>
+        <v>33.94250107</v>
       </c>
       <c r="H289" t="n">
-        <v>-98.23860168</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MFE</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>McAllen, TX, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11297,7 +11297,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>McAllen</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11311,21 +11311,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>35.0424003601</v>
+        <v>26.17580032</v>
       </c>
       <c r="H290" t="n">
-        <v>-89.9766998291</v>
+        <v>-98.23860168</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11335,35 +11335,35 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G291" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H291" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11373,35 +11373,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H292" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11411,7 +11411,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -11425,21 +11425,21 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H293" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11449,35 +11449,35 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G294" t="n">
-        <v>45.4706001282</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H294" t="n">
-        <v>-73.7407989502</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11487,35 +11487,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H295" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11525,7 +11525,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11539,21 +11539,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H296" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11563,7 +11563,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -11577,21 +11577,21 @@
         </is>
       </c>
       <c r="G297" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H297" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11601,7 +11601,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -11615,21 +11615,21 @@
         </is>
       </c>
       <c r="G298" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H298" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11639,35 +11639,35 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G299" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H299" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11677,35 +11677,35 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G300" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H300" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11715,7 +11715,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11729,21 +11729,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H301" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11753,7 +11753,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -11767,21 +11767,21 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="H302" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11791,7 +11791,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -11805,21 +11805,21 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="H303" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11829,35 +11829,35 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G304" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="H304" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11867,35 +11867,35 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H305" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11905,7 +11905,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11919,21 +11919,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H306" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11943,7 +11943,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11957,21 +11957,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="H307" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11981,7 +11981,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -11995,21 +11995,21 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H308" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12019,7 +12019,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12033,21 +12033,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H309" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12057,35 +12057,35 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G310" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H310" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12095,35 +12095,35 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G311" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H311" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12133,12 +12133,12 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -12147,21 +12147,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H312" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12171,12 +12171,12 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -12185,21 +12185,21 @@
         </is>
       </c>
       <c r="G313" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H313" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12209,7 +12209,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -12223,21 +12223,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H314" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12247,35 +12247,35 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G315" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H315" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12285,7 +12285,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -12299,21 +12299,21 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H316" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12323,7 +12323,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12337,21 +12337,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="H317" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12361,35 +12361,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H318" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12399,35 +12399,35 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G319" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H319" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12437,35 +12437,35 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G320" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="H320" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12475,7 +12475,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -12489,21 +12489,21 @@
         </is>
       </c>
       <c r="G321" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="H321" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12513,7 +12513,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -12527,21 +12527,21 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="H322" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12551,35 +12551,35 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="H323" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12589,35 +12589,35 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G324" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H324" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12627,7 +12627,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12641,21 +12641,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>41.50069</v>
+        <v>29.429461</v>
       </c>
       <c r="H325" t="n">
-        <v>-81.68411999999999</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12665,7 +12665,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12679,21 +12679,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>35.93543</v>
+        <v>41.50069</v>
       </c>
       <c r="H326" t="n">
-        <v>-78.88075000000001</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12703,7 +12703,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12717,21 +12717,21 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>35.46655</v>
+        <v>35.93543</v>
       </c>
       <c r="H327" t="n">
-        <v>-97.65373</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12741,7 +12741,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12755,21 +12755,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>27.9755001068</v>
+        <v>35.46655</v>
       </c>
       <c r="H328" t="n">
-        <v>-82.533203125</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12779,7 +12779,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12793,47 +12793,85 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>61.158555</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H329" t="n">
-        <v>-149.890208</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
+          <t>ANC</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Anchorage, United States</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Anchorage</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="G330" t="n">
+        <v>61.158555</v>
+      </c>
+      <c r="H330" t="n">
+        <v>-149.890208</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="inlineStr">
+        <is>
           <t>YHZ</t>
         </is>
       </c>
-      <c r="B330" t="inlineStr">
+      <c r="B331" t="inlineStr">
         <is>
           <t>Halifax, Canada</t>
         </is>
       </c>
-      <c r="C330" t="inlineStr">
+      <c r="C331" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="D330" t="inlineStr">
+      <c r="D331" t="inlineStr">
         <is>
           <t>Halifax</t>
         </is>
       </c>
-      <c r="E330" t="inlineStr">
+      <c r="E331" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="F330" t="inlineStr">
+      <c r="F331" t="inlineStr">
         <is>
           <t>CA</t>
         </is>
       </c>
-      <c r="G330" t="n">
+      <c r="G331" t="n">
         <v>44.64601</v>
       </c>
-      <c r="H330" t="n">
+      <c r="H331" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 61817676a5884ab95ffe327339d22e897ab313a2
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H331"/>
+  <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11282,12 +11282,12 @@
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MFE</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>McAllen, TX, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11297,7 +11297,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>McAllen</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11311,21 +11311,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>26.17580032</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H290" t="n">
-        <v>-98.23860168</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11335,35 +11335,35 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G291" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H291" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11373,35 +11373,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H292" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11411,7 +11411,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -11425,21 +11425,21 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H293" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11449,35 +11449,35 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G294" t="n">
-        <v>44.8819999695</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H294" t="n">
-        <v>-93.22180175779999</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11487,35 +11487,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H295" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11525,7 +11525,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11539,21 +11539,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H296" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11563,7 +11563,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -11577,21 +11577,21 @@
         </is>
       </c>
       <c r="G297" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H297" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11601,7 +11601,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -11615,21 +11615,21 @@
         </is>
       </c>
       <c r="G298" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H298" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11639,35 +11639,35 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G299" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H299" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11677,35 +11677,35 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G300" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H300" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11715,7 +11715,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11729,21 +11729,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="H301" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11753,7 +11753,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -11767,21 +11767,21 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="H302" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11791,7 +11791,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -11805,21 +11805,21 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="H303" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11829,35 +11829,35 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G304" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H304" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11867,35 +11867,35 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H305" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11905,7 +11905,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11919,21 +11919,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="H306" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11943,7 +11943,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11957,21 +11957,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H307" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11981,7 +11981,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -11995,21 +11995,21 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H308" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12019,7 +12019,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12033,21 +12033,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H309" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12057,35 +12057,35 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G310" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H310" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12095,35 +12095,35 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G311" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H311" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12133,12 +12133,12 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -12147,21 +12147,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H312" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12171,12 +12171,12 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -12185,21 +12185,21 @@
         </is>
       </c>
       <c r="G313" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H313" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12209,7 +12209,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -12223,21 +12223,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H314" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12247,35 +12247,35 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G315" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H315" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12285,7 +12285,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -12299,21 +12299,21 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="H316" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12323,7 +12323,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12337,21 +12337,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H317" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12361,35 +12361,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H318" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12399,35 +12399,35 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G319" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="H319" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12437,35 +12437,35 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G320" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="H320" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12475,7 +12475,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -12489,21 +12489,21 @@
         </is>
       </c>
       <c r="G321" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="H321" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12513,7 +12513,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -12527,21 +12527,21 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="H322" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12551,35 +12551,35 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H323" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12589,35 +12589,35 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G324" t="n">
-        <v>20.5217990875</v>
+        <v>29.429461</v>
       </c>
       <c r="H324" t="n">
-        <v>-103.3109970093</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12627,7 +12627,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12641,21 +12641,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>29.429461</v>
+        <v>41.50069</v>
       </c>
       <c r="H325" t="n">
-        <v>-98.487061</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12665,7 +12665,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12679,21 +12679,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>41.50069</v>
+        <v>35.93543</v>
       </c>
       <c r="H326" t="n">
-        <v>-81.68411999999999</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12703,7 +12703,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12717,21 +12717,21 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>35.93543</v>
+        <v>35.46655</v>
       </c>
       <c r="H327" t="n">
-        <v>-78.88075000000001</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12741,7 +12741,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12755,21 +12755,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>35.46655</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H328" t="n">
-        <v>-97.65373</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12779,7 +12779,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Anchorage</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12793,21 +12793,21 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>27.9755001068</v>
+        <v>61.158555</v>
       </c>
       <c r="H329" t="n">
-        <v>-82.533203125</v>
+        <v>-149.890208</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -12817,61 +12817,23 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G330" t="n">
-        <v>61.158555</v>
+        <v>44.64601</v>
       </c>
       <c r="H330" t="n">
-        <v>-149.890208</v>
-      </c>
-    </row>
-    <row r="331">
-      <c r="A331" s="1" t="inlineStr">
-        <is>
-          <t>YHZ</t>
-        </is>
-      </c>
-      <c r="B331" t="inlineStr">
-        <is>
-          <t>Halifax, Canada</t>
-        </is>
-      </c>
-      <c r="C331" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="D331" t="inlineStr">
-        <is>
-          <t>Halifax</t>
-        </is>
-      </c>
-      <c r="E331" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F331" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="G331" t="n">
-        <v>44.64601</v>
-      </c>
-      <c r="H331" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by e8b7a4de9e71c656802c61b6280c538e4aeefabe
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H332"/>
+  <dimension ref="A1:H331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8650,84 +8650,80 @@
     <row r="218">
       <c r="A218" s="1" t="inlineStr">
         <is>
-          <t>LHE</t>
+          <t>PKX</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Lahore, Pakistan</t>
+          <t>Langfang, China</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>Lahore</t>
+          <t>Langfang</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>PK</t>
-        </is>
-      </c>
-      <c r="G218" t="n">
-        <v>31.5216007233</v>
-      </c>
-      <c r="H218" t="n">
-        <v>74.4036026001</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr"/>
+      <c r="H218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" s="1" t="inlineStr">
         <is>
-          <t>PKX</t>
+          <t>MFM</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Langfang, China</t>
+          <t>Macau</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
         <is>
-          <t>Langfang</t>
-        </is>
-      </c>
-      <c r="E219" t="inlineStr">
-        <is>
-          <t>China</t>
-        </is>
-      </c>
+          <t>Macau</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr"/>
       <c r="F219" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G219" t="inlineStr"/>
-      <c r="H219" t="inlineStr"/>
+          <t>MO</t>
+        </is>
+      </c>
+      <c r="G219" t="n">
+        <v>22.1495990753</v>
+      </c>
+      <c r="H219" t="n">
+        <v>113.592002869</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="inlineStr">
         <is>
-          <t>MFM</t>
+          <t>MLE</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Macau</t>
+          <t>Male, Maldives</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -8737,31 +8733,35 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>Macau</t>
-        </is>
-      </c>
-      <c r="E220" t="inlineStr"/>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Maldives</t>
+        </is>
+      </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>MV</t>
         </is>
       </c>
       <c r="G220" t="n">
-        <v>22.1495990753</v>
+        <v>4.1748</v>
       </c>
       <c r="H220" t="n">
-        <v>113.592002869</v>
+        <v>73.50888</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="inlineStr">
         <is>
-          <t>MLE</t>
+          <t>MNL</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Male, Maldives</t>
+          <t>Manila, Philippines</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -8771,35 +8771,35 @@
       </c>
       <c r="D221" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Manila</t>
         </is>
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>Maldives</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>MV</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="G221" t="n">
-        <v>4.1748</v>
+        <v>14.508600235</v>
       </c>
       <c r="H221" t="n">
-        <v>73.50888</v>
+        <v>121.019996643</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="inlineStr">
         <is>
-          <t>MNL</t>
+          <t>BOM</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Manila, Philippines</t>
+          <t>Mumbai, India</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -8809,35 +8809,35 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Manila</t>
+          <t>Mumbai</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G222" t="n">
-        <v>14.508600235</v>
+        <v>19.0886993408</v>
       </c>
       <c r="H222" t="n">
-        <v>121.019996643</v>
+        <v>72.8678970337</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="inlineStr">
         <is>
-          <t>BOM</t>
+          <t>NAG</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Mumbai, India</t>
+          <t>Nagpur, India</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -8847,7 +8847,7 @@
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>Nagpur</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
@@ -8861,21 +8861,21 @@
         </is>
       </c>
       <c r="G223" t="n">
-        <v>19.0886993408</v>
+        <v>21.1610714</v>
       </c>
       <c r="H223" t="n">
-        <v>72.8678970337</v>
+        <v>79.0024702</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="inlineStr">
         <is>
-          <t>NAG</t>
+          <t>OKA</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Nagpur, India</t>
+          <t>Naha, Japan</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -8885,35 +8885,35 @@
       </c>
       <c r="D224" t="inlineStr">
         <is>
-          <t>Nagpur</t>
+          <t>Naha</t>
         </is>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="G224" t="n">
-        <v>21.1610714</v>
+        <v>26.1958</v>
       </c>
       <c r="H224" t="n">
-        <v>79.0024702</v>
+        <v>127.646</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="inlineStr">
         <is>
-          <t>OKA</t>
+          <t>DEL</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Naha, Japan</t>
+          <t>New Delhi, India</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -8923,35 +8923,35 @@
       </c>
       <c r="D225" t="inlineStr">
         <is>
-          <t>Naha</t>
+          <t>New Delhi</t>
         </is>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G225" t="n">
-        <v>26.1958</v>
+        <v>28.5664997101</v>
       </c>
       <c r="H225" t="n">
-        <v>127.646</v>
+        <v>77.1031036377</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="inlineStr">
         <is>
-          <t>DEL</t>
+          <t>KIX</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>New Delhi, India</t>
+          <t>Osaka, Japan</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -8961,35 +8961,35 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>New Delhi</t>
+          <t>Osaka</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="G226" t="n">
-        <v>28.5664997101</v>
+        <v>34.4272994995</v>
       </c>
       <c r="H226" t="n">
-        <v>77.1031036377</v>
+        <v>135.244003296</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="inlineStr">
         <is>
-          <t>KIX</t>
+          <t>PAT</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Osaka, Japan</t>
+          <t>Patna, India</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -8999,35 +8999,35 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>Osaka</t>
+          <t>Patna</t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G227" t="n">
-        <v>34.4272994995</v>
+        <v>25.591299057</v>
       </c>
       <c r="H227" t="n">
-        <v>135.244003296</v>
+        <v>85.0879974365</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="inlineStr">
         <is>
-          <t>PAT</t>
+          <t>PNH</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Patna, India</t>
+          <t>Phnom Penh, Cambodia</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -9037,179 +9037,179 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>Patna</t>
+          <t>Phnom Penh</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Cambodia</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>KH</t>
         </is>
       </c>
       <c r="G228" t="n">
-        <v>25.591299057</v>
+        <v>11.5466003418</v>
       </c>
       <c r="H228" t="n">
-        <v>85.0879974365</v>
+        <v>104.84400177</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="inlineStr">
         <is>
-          <t>PNH</t>
+          <t>TAO</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Phnom Penh, Cambodia</t>
+          <t>Qingdao, China</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>Phnom Penh</t>
+          <t>Qingdao</t>
         </is>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Cambodia</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>KH</t>
-        </is>
-      </c>
-      <c r="G229" t="n">
-        <v>11.5466003418</v>
-      </c>
-      <c r="H229" t="n">
-        <v>104.84400177</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr"/>
+      <c r="H229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" s="1" t="inlineStr">
         <is>
-          <t>TAO</t>
+          <t>ICN</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Qingdao, China</t>
+          <t>Seoul, South Korea</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Qingdao</t>
+          <t>Seoul</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G230" t="inlineStr"/>
-      <c r="H230" t="inlineStr"/>
+          <t>KR</t>
+        </is>
+      </c>
+      <c r="G230" t="n">
+        <v>37.4691009521</v>
+      </c>
+      <c r="H230" t="n">
+        <v>126.450996399</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="inlineStr">
         <is>
-          <t>ICN</t>
+          <t>SHA</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Seoul, South Korea</t>
+          <t>Shanghai, China</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>Seoul</t>
+          <t>Shanghai</t>
         </is>
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>KR</t>
-        </is>
-      </c>
-      <c r="G231" t="n">
-        <v>37.4691009521</v>
-      </c>
-      <c r="H231" t="n">
-        <v>126.450996399</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr"/>
+      <c r="H231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" s="1" t="inlineStr">
         <is>
-          <t>SHA</t>
+          <t>SIN</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Shanghai, China</t>
+          <t>Singapore, Singapore</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>Shanghai</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G232" t="inlineStr"/>
-      <c r="H232" t="inlineStr"/>
+          <t>SG</t>
+        </is>
+      </c>
+      <c r="G232" t="n">
+        <v>1.3501900434</v>
+      </c>
+      <c r="H232" t="n">
+        <v>103.994003296</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="inlineStr">
         <is>
-          <t>SIN</t>
+          <t>URT</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Singapore, Singapore</t>
+          <t>Surat Thani, Thailand</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -9219,35 +9219,35 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Surat Thani</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>SG</t>
+          <t>TH</t>
         </is>
       </c>
       <c r="G233" t="n">
-        <v>1.3501900434</v>
+        <v>9.1325998306</v>
       </c>
       <c r="H233" t="n">
-        <v>103.994003296</v>
+        <v>99.135597229</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="inlineStr">
         <is>
-          <t>URT</t>
+          <t>TPE</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Surat Thani, Thailand</t>
+          <t>Taipei</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -9257,35 +9257,31 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>Surat Thani</t>
-        </is>
-      </c>
-      <c r="E234" t="inlineStr">
-        <is>
-          <t>Thailand</t>
-        </is>
-      </c>
+          <t>Taipei</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr"/>
       <c r="F234" t="inlineStr">
         <is>
-          <t>TH</t>
+          <t>TW</t>
         </is>
       </c>
       <c r="G234" t="n">
-        <v>9.1325998306</v>
+        <v>25.0776996613</v>
       </c>
       <c r="H234" t="n">
-        <v>99.135597229</v>
+        <v>121.233001709</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="inlineStr">
         <is>
-          <t>TPE</t>
+          <t>NRT</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Taipei</t>
+          <t>Tokyo, Japan</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -9295,31 +9291,35 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>Taipei</t>
-        </is>
-      </c>
-      <c r="E235" t="inlineStr"/>
+          <t>Tokyo</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>TW</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="G235" t="n">
-        <v>25.0776996613</v>
+        <v>35.7647018433</v>
       </c>
       <c r="H235" t="n">
-        <v>121.233001709</v>
+        <v>140.386001587</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="inlineStr">
         <is>
-          <t>NRT</t>
+          <t>ULN</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Tokyo, Japan</t>
+          <t>Ulaanbaatar, Mongolia</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -9329,35 +9329,35 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>Tokyo</t>
+          <t>Ulaanbaatar</t>
         </is>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Mongolia</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="G236" t="n">
-        <v>35.7647018433</v>
+        <v>47.8431015015</v>
       </c>
       <c r="H236" t="n">
-        <v>140.386001587</v>
+        <v>106.766998291</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="inlineStr">
         <is>
-          <t>ULN</t>
+          <t>VTE</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Ulaanbaatar, Mongolia</t>
+          <t>Vientiane, Laos</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -9367,217 +9367,217 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>Ulaanbaatar</t>
+          <t>Vientiane</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Mongolia</t>
+          <t>Laos</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>LA</t>
         </is>
       </c>
       <c r="G237" t="n">
-        <v>47.8431015015</v>
+        <v>17.9757</v>
       </c>
       <c r="H237" t="n">
-        <v>106.766998291</v>
+        <v>102.5683</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="inlineStr">
         <is>
-          <t>VTE</t>
+          <t>KHN</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Vientiane, Laos</t>
+          <t>Nanchang, China</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>Vientiane</t>
+          <t>Nanchang</t>
         </is>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Laos</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>LA</t>
-        </is>
-      </c>
-      <c r="G238" t="n">
-        <v>17.9757</v>
-      </c>
-      <c r="H238" t="n">
-        <v>102.5683</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G238" t="inlineStr"/>
+      <c r="H238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" s="1" t="inlineStr">
         <is>
-          <t>KHN</t>
+          <t>EVN</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Nanchang, China</t>
+          <t>Yerevan, Armenia</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Middle East</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>Nanchang</t>
+          <t>Yerevan</t>
         </is>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Armenia</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G239" t="inlineStr"/>
-      <c r="H239" t="inlineStr"/>
+          <t>AM</t>
+        </is>
+      </c>
+      <c r="G239" t="n">
+        <v>40.1473007202</v>
+      </c>
+      <c r="H239" t="n">
+        <v>44.3959007263</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="inlineStr">
         <is>
-          <t>EVN</t>
+          <t>JOG</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Yerevan, Armenia</t>
+          <t>Yogyakarta, Indonesia</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Middle East</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>Yerevan</t>
+          <t>Yogyakarta</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>Armenia</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>AM</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="G240" t="n">
-        <v>40.1473007202</v>
+        <v>-7.7881798744</v>
       </c>
       <c r="H240" t="n">
-        <v>44.3959007263</v>
+        <v>110.4319992065</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="inlineStr">
         <is>
-          <t>JOG</t>
+          <t>ZGN</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Yogyakarta, Indonesia</t>
+          <t>Zhongshan, China</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Yogyakarta</t>
+          <t>Zhongshan</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="G241" t="n">
-        <v>-7.7881798744</v>
-      </c>
-      <c r="H241" t="n">
-        <v>110.4319992065</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr"/>
+      <c r="H241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>ZGN</t>
+          <t>CGY</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Zhongshan, China</t>
+          <t>Cagayan de Oro, Philippines</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Zhongshan</t>
+          <t>Cagayan de Oro</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G242" t="inlineStr"/>
-      <c r="H242" t="inlineStr"/>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="G242" t="n">
+        <v>8.415619850200001</v>
+      </c>
+      <c r="H242" t="n">
+        <v>124.611000061</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>CGY</t>
+          <t>COK</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Cagayan de Oro, Philippines</t>
+          <t>Kochi, India</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -9587,35 +9587,35 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Cagayan de Oro</t>
+          <t>Kochi</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G243" t="n">
-        <v>8.415619850200001</v>
+        <v>9.9312</v>
       </c>
       <c r="H243" t="n">
-        <v>124.611000061</v>
+        <v>76.26730000000001</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>DPS</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Kochi, India</t>
+          <t>Denpasar, Indonesia</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -9625,35 +9625,35 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>Kochi</t>
+          <t>Denpasar</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="G244" t="n">
-        <v>9.9312</v>
+        <v>-8.748169899000001</v>
       </c>
       <c r="H244" t="n">
-        <v>76.26730000000001</v>
+        <v>115.1669998169</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>DPS</t>
+          <t>CNN</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Denpasar, Indonesia</t>
+          <t>Kannur, India</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -9663,73 +9663,69 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Denpasar</t>
+          <t>Kannur</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G245" t="n">
-        <v>-8.748169899000001</v>
+        <v>11.915858</v>
       </c>
       <c r="H245" t="n">
-        <v>115.1669998169</v>
+        <v>75.55094</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>CNN</t>
+          <t>SZX</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Kannur, India</t>
+          <t>Shenzhen, China</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Kannur</t>
+          <t>Shenzhen</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="G246" t="n">
-        <v>11.915858</v>
-      </c>
-      <c r="H246" t="n">
-        <v>75.55094</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr"/>
+      <c r="H246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>SZX</t>
+          <t>KWE</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Shenzhen, China</t>
+          <t>Guiyang, China</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -9739,7 +9735,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Shenzhen</t>
+          <t>Guiyang</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
@@ -9758,12 +9754,12 @@
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>KWE</t>
+          <t>HGH</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Guiyang, China</t>
+          <t>Shaoxing, China</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -9773,7 +9769,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Guiyang</t>
+          <t>Shaoxing</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -9792,12 +9788,12 @@
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>HGH</t>
+          <t>CZX</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Shaoxing, China</t>
+          <t>Changzhou, China</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -9807,7 +9803,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Shaoxing</t>
+          <t>Changzhou</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -9826,12 +9822,12 @@
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>CZX</t>
+          <t>KMG</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Changzhou, China</t>
+          <t>Kunming, China</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -9841,7 +9837,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Changzhou</t>
+          <t>Kunming</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
@@ -9860,84 +9856,84 @@
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>KMG</t>
+          <t>CNX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Kunming, China</t>
+          <t>Chiang Mai, Thailand</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Kunming</t>
+          <t>Chiang Mai</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G251" t="inlineStr"/>
-      <c r="H251" t="inlineStr"/>
+          <t>TH</t>
+        </is>
+      </c>
+      <c r="G251" t="n">
+        <v>18.7667999268</v>
+      </c>
+      <c r="H251" t="n">
+        <v>98.962600708</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>CNX</t>
+          <t>CGO</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Chiang Mai, Thailand</t>
+          <t>Zhengzhou, China</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>Chiang Mai</t>
+          <t>Zhengzhou</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>TH</t>
-        </is>
-      </c>
-      <c r="G252" t="n">
-        <v>18.7667999268</v>
-      </c>
-      <c r="H252" t="n">
-        <v>98.962600708</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr"/>
+      <c r="H252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>CGO</t>
+          <t>TYN</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Zhengzhou, China</t>
+          <t>Yangquan, China</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -9947,7 +9943,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>Zhengzhou</t>
+          <t>Yangquan</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
@@ -9966,12 +9962,12 @@
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>TYN</t>
+          <t>CSX</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Yangquan, China</t>
+          <t>Changsha, China</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -9981,7 +9977,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Yangquan</t>
+          <t>Changsha</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
@@ -10000,12 +9996,12 @@
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>CSX</t>
+          <t>DLC</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Changsha, China</t>
+          <t>Dalian, China</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -10015,7 +10011,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Changsha</t>
+          <t>Dalian</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
@@ -10034,12 +10030,12 @@
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>DLC</t>
+          <t>BHY</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Dalian, China</t>
+          <t>Beihai, China</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -10049,7 +10045,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Dalian</t>
+          <t>Beihai</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
@@ -10068,12 +10064,12 @@
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>BHY</t>
+          <t>CKG</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Beihai, China</t>
+          <t>Chongqing, China</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -10083,7 +10079,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Beihai</t>
+          <t>Chongqing</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
@@ -10102,12 +10098,12 @@
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>CKG</t>
+          <t>XFN</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Chongqing, China</t>
+          <t>Xiangyang, China</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -10117,7 +10113,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Chongqing</t>
+          <t>Xiangyang</t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
@@ -10136,118 +10132,122 @@
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>XFN</t>
+          <t>DAD</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Xiangyang, China</t>
+          <t>Da Nang, Vietnam</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Xiangyang</t>
+          <t>Da Nang</t>
         </is>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Vietnam</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G259" t="inlineStr"/>
-      <c r="H259" t="inlineStr"/>
+          <t>VN</t>
+        </is>
+      </c>
+      <c r="G259" t="n">
+        <v>16.02636</v>
+      </c>
+      <c r="H259" t="n">
+        <v>108.20869</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>DAD</t>
+          <t>JXG</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Da Nang, Vietnam</t>
+          <t>Jiaxing, China</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Da Nang</t>
+          <t>Jiaxing</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>VN</t>
-        </is>
-      </c>
-      <c r="G260" t="n">
-        <v>16.02636</v>
-      </c>
-      <c r="H260" t="n">
-        <v>108.20869</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr"/>
+      <c r="H260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>JXG</t>
+          <t>CRK</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Jiaxing, China</t>
+          <t>Tarlac City, Philippines</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Jiaxing</t>
+          <t>Tarlac City</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G261" t="inlineStr"/>
-      <c r="H261" t="inlineStr"/>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="G261" t="n">
+        <v>15.1859</v>
+      </c>
+      <c r="H261" t="n">
+        <v>120.5599</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>CRK</t>
+          <t>PBH</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Tarlac City, Philippines</t>
+          <t>Thimphu, Bhutan</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -10257,73 +10257,69 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Tarlac City</t>
+          <t>Thimphu</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Bhutan</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>BT</t>
         </is>
       </c>
       <c r="G262" t="n">
-        <v>15.1859</v>
+        <v>27.4712</v>
       </c>
       <c r="H262" t="n">
-        <v>120.5599</v>
+        <v>89.6339</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>PBH</t>
+          <t>XIY</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Thimphu, Bhutan</t>
+          <t>Baoji, China</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Thimphu</t>
+          <t>Baoji</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>Bhutan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>BT</t>
-        </is>
-      </c>
-      <c r="G263" t="n">
-        <v>27.4712</v>
-      </c>
-      <c r="H263" t="n">
-        <v>89.6339</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr"/>
+      <c r="H263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>XIY</t>
+          <t>CTU</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Baoji, China</t>
+          <t>Chengdu, China</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -10333,7 +10329,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Baoji</t>
+          <t>Chengdu</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
@@ -10352,118 +10348,122 @@
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>CTU</t>
+          <t>NQZ</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Chengdu, China</t>
+          <t>Astana, Kazakhstan</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Chengdu</t>
+          <t>Astana</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G265" t="inlineStr"/>
-      <c r="H265" t="inlineStr"/>
+          <t>KZ</t>
+        </is>
+      </c>
+      <c r="G265" t="n">
+        <v>51.167801</v>
+      </c>
+      <c r="H265" t="n">
+        <v>71.418893</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>NQZ</t>
+          <t>NNG</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Astana, Kazakhstan</t>
+          <t>Nanning, China</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Astana</t>
+          <t>Nanning</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G266" t="n">
-        <v>51.167801</v>
-      </c>
-      <c r="H266" t="n">
-        <v>71.418893</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr"/>
+      <c r="H266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>NNG</t>
+          <t>KCH</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Nanning, China</t>
+          <t>Kuching, Malaysia</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Nanning</t>
+          <t>Kuching</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G267" t="inlineStr"/>
-      <c r="H267" t="inlineStr"/>
+          <t>MY</t>
+        </is>
+      </c>
+      <c r="G267" t="n">
+        <v>1.709727</v>
+      </c>
+      <c r="H267" t="n">
+        <v>110.353455</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>KCH</t>
+          <t>AKX</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Kuching, Malaysia</t>
+          <t>Aktobe, Kazakhstan</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -10473,73 +10473,69 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Kuching</t>
+          <t>Aktobe</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>MY</t>
+          <t>KZ</t>
         </is>
       </c>
       <c r="G268" t="n">
-        <v>1.709727</v>
+        <v>50.286922</v>
       </c>
       <c r="H268" t="n">
-        <v>110.353455</v>
+        <v>57.224121</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>AKX</t>
+          <t>TEN</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Aktobe, Kazakhstan</t>
+          <t>Tongren, China</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Aktobe</t>
+          <t>Tongren</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G269" t="n">
-        <v>50.286922</v>
-      </c>
-      <c r="H269" t="n">
-        <v>57.224121</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr"/>
+      <c r="H269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>TEN</t>
+          <t>HYN</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Tongren, China</t>
+          <t>Taizhou, China</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -10549,7 +10545,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Tongren</t>
+          <t>Taizhou</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
@@ -10568,12 +10564,12 @@
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>HYN</t>
+          <t>XNN</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Taizhou, China</t>
+          <t>Xining, China</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -10583,7 +10579,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Taizhou</t>
+          <t>Xining</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
@@ -10602,84 +10598,88 @@
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>XNN</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Xining, China</t>
+          <t>Bishkek, Kyrgyzstan</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Xining</t>
+          <t>Bishkek</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G272" t="inlineStr"/>
-      <c r="H272" t="inlineStr"/>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="G272" t="n">
+        <v>42.875608</v>
+      </c>
+      <c r="H272" t="n">
+        <v>74.604613</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>FRU</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Bishkek, Kyrgyzstan</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Bishkek</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Kyrgyzstan</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G273" t="n">
-        <v>42.875608</v>
+        <v>38.94449997</v>
       </c>
       <c r="H273" t="n">
-        <v>74.604613</v>
+        <v>-77.45580292</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -10689,7 +10689,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -10703,21 +10703,21 @@
         </is>
       </c>
       <c r="G274" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H274" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10727,7 +10727,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -10741,21 +10741,21 @@
         </is>
       </c>
       <c r="G275" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="H275" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10765,7 +10765,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -10779,21 +10779,21 @@
         </is>
       </c>
       <c r="G276" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="H276" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10803,35 +10803,35 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G277" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="H277" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10841,35 +10841,35 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G278" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H278" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10879,7 +10879,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -10893,21 +10893,21 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="H279" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10917,7 +10917,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10931,21 +10931,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H280" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10955,7 +10955,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10969,21 +10969,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H281" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -10993,7 +10993,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -11007,21 +11007,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H282" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11031,7 +11031,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11045,21 +11045,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H283" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11069,7 +11069,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11083,21 +11083,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H284" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11107,7 +11107,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11121,21 +11121,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H285" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11145,7 +11145,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11159,21 +11159,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="H286" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11183,7 +11183,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11197,21 +11197,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H287" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11221,7 +11221,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11235,21 +11235,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H288" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11259,7 +11259,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -11273,21 +11273,21 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="H289" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11297,7 +11297,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11311,21 +11311,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="H290" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11335,7 +11335,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -11349,21 +11349,21 @@
         </is>
       </c>
       <c r="G291" t="n">
-        <v>33.94250107</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H291" t="n">
-        <v>-118.4079971</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11373,35 +11373,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H292" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11411,35 +11411,35 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G293" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H293" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11449,7 +11449,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
@@ -11463,21 +11463,21 @@
         </is>
       </c>
       <c r="G294" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H294" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11487,35 +11487,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>44.8819999695</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H295" t="n">
-        <v>-93.22180175779999</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11525,35 +11525,35 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G296" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H296" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11563,7 +11563,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -11577,21 +11577,21 @@
         </is>
       </c>
       <c r="G297" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H297" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11601,7 +11601,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -11615,21 +11615,21 @@
         </is>
       </c>
       <c r="G298" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H298" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11639,7 +11639,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
@@ -11653,21 +11653,21 @@
         </is>
       </c>
       <c r="G299" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H299" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11677,35 +11677,35 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G300" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H300" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11715,35 +11715,35 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G301" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H301" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11753,7 +11753,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -11767,21 +11767,21 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="H302" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11791,7 +11791,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -11805,21 +11805,21 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="H303" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11829,7 +11829,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -11843,21 +11843,21 @@
         </is>
       </c>
       <c r="G304" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="H304" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11867,35 +11867,35 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H305" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11905,35 +11905,35 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G306" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H306" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11943,7 +11943,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11957,21 +11957,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="H307" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11981,7 +11981,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -11995,21 +11995,21 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H308" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12019,7 +12019,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12033,21 +12033,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H309" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12057,7 +12057,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -12071,21 +12071,21 @@
         </is>
       </c>
       <c r="G310" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H310" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12095,35 +12095,35 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G311" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H311" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12133,35 +12133,35 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G312" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H312" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12171,12 +12171,12 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -12185,21 +12185,21 @@
         </is>
       </c>
       <c r="G313" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H313" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12209,12 +12209,12 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -12223,21 +12223,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H314" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12247,7 +12247,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -12261,21 +12261,21 @@
         </is>
       </c>
       <c r="G315" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H315" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12285,35 +12285,35 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G316" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H316" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12323,7 +12323,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12337,21 +12337,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="H317" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12361,7 +12361,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
@@ -12375,21 +12375,21 @@
         </is>
       </c>
       <c r="G318" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H318" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12399,35 +12399,35 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G319" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H319" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12437,35 +12437,35 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G320" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="H320" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12475,35 +12475,35 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G321" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="H321" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12513,7 +12513,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -12527,21 +12527,21 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="H322" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12551,7 +12551,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
@@ -12565,21 +12565,21 @@
         </is>
       </c>
       <c r="G323" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="H323" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12589,35 +12589,35 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G324" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H324" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12627,35 +12627,35 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G325" t="n">
-        <v>20.5217990875</v>
+        <v>29.429461</v>
       </c>
       <c r="H325" t="n">
-        <v>-103.3109970093</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12665,7 +12665,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12679,21 +12679,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>29.429461</v>
+        <v>41.50069</v>
       </c>
       <c r="H326" t="n">
-        <v>-98.487061</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12703,7 +12703,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12717,21 +12717,21 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>41.50069</v>
+        <v>35.93543</v>
       </c>
       <c r="H327" t="n">
-        <v>-81.68411999999999</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12741,7 +12741,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12755,21 +12755,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>35.93543</v>
+        <v>35.46655</v>
       </c>
       <c r="H328" t="n">
-        <v>-78.88075000000001</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12779,7 +12779,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12793,21 +12793,21 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>35.46655</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H329" t="n">
-        <v>-97.65373</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -12817,7 +12817,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Anchorage</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -12831,21 +12831,21 @@
         </is>
       </c>
       <c r="G330" t="n">
-        <v>27.9755001068</v>
+        <v>61.158555</v>
       </c>
       <c r="H330" t="n">
-        <v>-82.533203125</v>
+        <v>-149.890208</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -12855,61 +12855,23 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G331" t="n">
-        <v>61.158555</v>
+        <v>44.64601</v>
       </c>
       <c r="H331" t="n">
-        <v>-149.890208</v>
-      </c>
-    </row>
-    <row r="332">
-      <c r="A332" s="1" t="inlineStr">
-        <is>
-          <t>YHZ</t>
-        </is>
-      </c>
-      <c r="B332" t="inlineStr">
-        <is>
-          <t>Halifax, Canada</t>
-        </is>
-      </c>
-      <c r="C332" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="D332" t="inlineStr">
-        <is>
-          <t>Halifax</t>
-        </is>
-      </c>
-      <c r="E332" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F332" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="G332" t="n">
-        <v>44.64601</v>
-      </c>
-      <c r="H332" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 93c4fbb7492243114f4d93d8dba0cf9ba4e818a1
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H331"/>
+  <dimension ref="A1:H332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12875,6 +12875,40 @@
         <v>-63.66844</v>
       </c>
     </row>
+    <row r="332">
+      <c r="A332" s="1" t="inlineStr">
+        <is>
+          <t>CZL</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Constantine, Algeria</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>Africa</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Constantine</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr"/>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>DZ</t>
+        </is>
+      </c>
+      <c r="G332" t="n">
+        <v>36.335972</v>
+      </c>
+      <c r="H332" t="n">
+        <v>6.598562</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update generated data Triggered by 8cd5fb17a17cbbc9fa7ee0c296ee50c58caa3f84
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H332"/>
+  <dimension ref="A1:H331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9538,46 +9538,50 @@
     <row r="242">
       <c r="A242" s="1" t="inlineStr">
         <is>
-          <t>ZGN</t>
+          <t>CGY</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Zhongshan, China</t>
+          <t>Cagayan de Oro, Philippines</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
         <is>
-          <t>Zhongshan</t>
+          <t>Cagayan de Oro</t>
         </is>
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G242" t="inlineStr"/>
-      <c r="H242" t="inlineStr"/>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="G242" t="n">
+        <v>8.415619850200001</v>
+      </c>
+      <c r="H242" t="n">
+        <v>124.611000061</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="inlineStr">
         <is>
-          <t>CGY</t>
+          <t>COK</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Cagayan de Oro, Philippines</t>
+          <t>Kochi, India</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -9587,35 +9591,35 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>Cagayan de Oro</t>
+          <t>Kochi</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G243" t="n">
-        <v>8.415619850200001</v>
+        <v>9.9312</v>
       </c>
       <c r="H243" t="n">
-        <v>124.611000061</v>
+        <v>76.26730000000001</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="inlineStr">
         <is>
-          <t>COK</t>
+          <t>DPS</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Kochi, India</t>
+          <t>Denpasar, Indonesia</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -9625,35 +9629,35 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>Kochi</t>
+          <t>Denpasar</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="G244" t="n">
-        <v>9.9312</v>
+        <v>-8.748169899000001</v>
       </c>
       <c r="H244" t="n">
-        <v>76.26730000000001</v>
+        <v>115.1669998169</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="inlineStr">
         <is>
-          <t>DPS</t>
+          <t>CNN</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Denpasar, Indonesia</t>
+          <t>Kannur, India</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -9663,73 +9667,69 @@
       </c>
       <c r="D245" t="inlineStr">
         <is>
-          <t>Denpasar</t>
+          <t>Kannur</t>
         </is>
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="G245" t="n">
-        <v>-8.748169899000001</v>
+        <v>11.915858</v>
       </c>
       <c r="H245" t="n">
-        <v>115.1669998169</v>
+        <v>75.55094</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="inlineStr">
         <is>
-          <t>CNN</t>
+          <t>SZX</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Kannur, India</t>
+          <t>Shenzhen, China</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>Kannur</t>
+          <t>Shenzhen</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="G246" t="n">
-        <v>11.915858</v>
-      </c>
-      <c r="H246" t="n">
-        <v>75.55094</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr"/>
+      <c r="H246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" s="1" t="inlineStr">
         <is>
-          <t>SZX</t>
+          <t>KWE</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Shenzhen, China</t>
+          <t>Guiyang, China</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -9739,7 +9739,7 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>Shenzhen</t>
+          <t>Guiyang</t>
         </is>
       </c>
       <c r="E247" t="inlineStr">
@@ -9758,12 +9758,12 @@
     <row r="248">
       <c r="A248" s="1" t="inlineStr">
         <is>
-          <t>KWE</t>
+          <t>HGH</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Guiyang, China</t>
+          <t>Shaoxing, China</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -9773,7 +9773,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Guiyang</t>
+          <t>Shaoxing</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -9792,12 +9792,12 @@
     <row r="249">
       <c r="A249" s="1" t="inlineStr">
         <is>
-          <t>HGH</t>
+          <t>CZX</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Shaoxing, China</t>
+          <t>Changzhou, China</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -9807,7 +9807,7 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Shaoxing</t>
+          <t>Changzhou</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -9826,12 +9826,12 @@
     <row r="250">
       <c r="A250" s="1" t="inlineStr">
         <is>
-          <t>CZX</t>
+          <t>KMG</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Changzhou, China</t>
+          <t>Kunming, China</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -9841,7 +9841,7 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>Changzhou</t>
+          <t>Kunming</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
@@ -9860,84 +9860,84 @@
     <row r="251">
       <c r="A251" s="1" t="inlineStr">
         <is>
-          <t>KMG</t>
+          <t>CNX</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Kunming, China</t>
+          <t>Chiang Mai, Thailand</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>Kunming</t>
+          <t>Chiang Mai</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Thailand</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G251" t="inlineStr"/>
-      <c r="H251" t="inlineStr"/>
+          <t>TH</t>
+        </is>
+      </c>
+      <c r="G251" t="n">
+        <v>18.7667999268</v>
+      </c>
+      <c r="H251" t="n">
+        <v>98.962600708</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="inlineStr">
         <is>
-          <t>CNX</t>
+          <t>CGO</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Chiang Mai, Thailand</t>
+          <t>Zhengzhou, China</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>Chiang Mai</t>
+          <t>Zhengzhou</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>TH</t>
-        </is>
-      </c>
-      <c r="G252" t="n">
-        <v>18.7667999268</v>
-      </c>
-      <c r="H252" t="n">
-        <v>98.962600708</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr"/>
+      <c r="H252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" s="1" t="inlineStr">
         <is>
-          <t>CGO</t>
+          <t>TYN</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Zhengzhou, China</t>
+          <t>Yangquan, China</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -9947,7 +9947,7 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>Zhengzhou</t>
+          <t>Yangquan</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
@@ -9966,12 +9966,12 @@
     <row r="254">
       <c r="A254" s="1" t="inlineStr">
         <is>
-          <t>TYN</t>
+          <t>CSX</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Yangquan, China</t>
+          <t>Changsha, China</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -9981,7 +9981,7 @@
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>Yangquan</t>
+          <t>Changsha</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
@@ -10000,12 +10000,12 @@
     <row r="255">
       <c r="A255" s="1" t="inlineStr">
         <is>
-          <t>CSX</t>
+          <t>DLC</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Changsha, China</t>
+          <t>Dalian, China</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -10015,7 +10015,7 @@
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>Changsha</t>
+          <t>Dalian</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
@@ -10034,12 +10034,12 @@
     <row r="256">
       <c r="A256" s="1" t="inlineStr">
         <is>
-          <t>DLC</t>
+          <t>BHY</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Dalian, China</t>
+          <t>Beihai, China</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -10049,7 +10049,7 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Dalian</t>
+          <t>Beihai</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
@@ -10068,12 +10068,12 @@
     <row r="257">
       <c r="A257" s="1" t="inlineStr">
         <is>
-          <t>BHY</t>
+          <t>CKG</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Beihai, China</t>
+          <t>Chongqing, China</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -10083,7 +10083,7 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Beihai</t>
+          <t>Chongqing</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
@@ -10102,12 +10102,12 @@
     <row r="258">
       <c r="A258" s="1" t="inlineStr">
         <is>
-          <t>CKG</t>
+          <t>XFN</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Chongqing, China</t>
+          <t>Xiangyang, China</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -10117,7 +10117,7 @@
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>Chongqing</t>
+          <t>Xiangyang</t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
@@ -10136,118 +10136,122 @@
     <row r="259">
       <c r="A259" s="1" t="inlineStr">
         <is>
-          <t>XFN</t>
+          <t>DAD</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Xiangyang, China</t>
+          <t>Da Nang, Vietnam</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
         <is>
-          <t>Xiangyang</t>
+          <t>Da Nang</t>
         </is>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Vietnam</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G259" t="inlineStr"/>
-      <c r="H259" t="inlineStr"/>
+          <t>VN</t>
+        </is>
+      </c>
+      <c r="G259" t="n">
+        <v>16.02636</v>
+      </c>
+      <c r="H259" t="n">
+        <v>108.20869</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="inlineStr">
         <is>
-          <t>DAD</t>
+          <t>JXG</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Da Nang, Vietnam</t>
+          <t>Jiaxing, China</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>Da Nang</t>
+          <t>Jiaxing</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>VN</t>
-        </is>
-      </c>
-      <c r="G260" t="n">
-        <v>16.02636</v>
-      </c>
-      <c r="H260" t="n">
-        <v>108.20869</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr"/>
+      <c r="H260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" s="1" t="inlineStr">
         <is>
-          <t>JXG</t>
+          <t>CRK</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Jiaxing, China</t>
+          <t>Tarlac City, Philippines</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>Jiaxing</t>
+          <t>Tarlac City</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G261" t="inlineStr"/>
-      <c r="H261" t="inlineStr"/>
+          <t>PH</t>
+        </is>
+      </c>
+      <c r="G261" t="n">
+        <v>15.1859</v>
+      </c>
+      <c r="H261" t="n">
+        <v>120.5599</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="inlineStr">
         <is>
-          <t>CRK</t>
+          <t>PBH</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Tarlac City, Philippines</t>
+          <t>Thimphu, Bhutan</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -10257,73 +10261,69 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>Tarlac City</t>
+          <t>Thimphu</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Bhutan</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>BT</t>
         </is>
       </c>
       <c r="G262" t="n">
-        <v>15.1859</v>
+        <v>27.4712</v>
       </c>
       <c r="H262" t="n">
-        <v>120.5599</v>
+        <v>89.6339</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="inlineStr">
         <is>
-          <t>PBH</t>
+          <t>XIY</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Thimphu, Bhutan</t>
+          <t>Baoji, China</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Thimphu</t>
+          <t>Baoji</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>Bhutan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>BT</t>
-        </is>
-      </c>
-      <c r="G263" t="n">
-        <v>27.4712</v>
-      </c>
-      <c r="H263" t="n">
-        <v>89.6339</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr"/>
+      <c r="H263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>XIY</t>
+          <t>CTU</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Baoji, China</t>
+          <t>Chengdu, China</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -10333,7 +10333,7 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Baoji</t>
+          <t>Chengdu</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
@@ -10352,118 +10352,122 @@
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>CTU</t>
+          <t>NQZ</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Chengdu, China</t>
+          <t>Astana, Kazakhstan</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Chengdu</t>
+          <t>Astana</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G265" t="inlineStr"/>
-      <c r="H265" t="inlineStr"/>
+          <t>KZ</t>
+        </is>
+      </c>
+      <c r="G265" t="n">
+        <v>51.167801</v>
+      </c>
+      <c r="H265" t="n">
+        <v>71.418893</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>NQZ</t>
+          <t>NNG</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Astana, Kazakhstan</t>
+          <t>Nanning, China</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Astana</t>
+          <t>Nanning</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G266" t="n">
-        <v>51.167801</v>
-      </c>
-      <c r="H266" t="n">
-        <v>71.418893</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr"/>
+      <c r="H266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>NNG</t>
+          <t>KCH</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Nanning, China</t>
+          <t>Kuching, Malaysia</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Nanning</t>
+          <t>Kuching</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G267" t="inlineStr"/>
-      <c r="H267" t="inlineStr"/>
+          <t>MY</t>
+        </is>
+      </c>
+      <c r="G267" t="n">
+        <v>1.709727</v>
+      </c>
+      <c r="H267" t="n">
+        <v>110.353455</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>KCH</t>
+          <t>AKX</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Kuching, Malaysia</t>
+          <t>Aktobe, Kazakhstan</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -10473,73 +10477,69 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Kuching</t>
+          <t>Aktobe</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>MY</t>
+          <t>KZ</t>
         </is>
       </c>
       <c r="G268" t="n">
-        <v>1.709727</v>
+        <v>50.286922</v>
       </c>
       <c r="H268" t="n">
-        <v>110.353455</v>
+        <v>57.224121</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>AKX</t>
+          <t>TEN</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Aktobe, Kazakhstan</t>
+          <t>Tongren, China</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Aktobe</t>
+          <t>Tongren</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G269" t="n">
-        <v>50.286922</v>
-      </c>
-      <c r="H269" t="n">
-        <v>57.224121</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr"/>
+      <c r="H269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>TEN</t>
+          <t>HYN</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Tongren, China</t>
+          <t>Taizhou, China</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -10549,7 +10549,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Tongren</t>
+          <t>Taizhou</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
@@ -10568,12 +10568,12 @@
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>HYN</t>
+          <t>XNN</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Taizhou, China</t>
+          <t>Xining, China</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -10583,7 +10583,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Taizhou</t>
+          <t>Xining</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
@@ -10602,84 +10602,88 @@
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>XNN</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Xining, China</t>
+          <t>Bishkek, Kyrgyzstan</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Xining</t>
+          <t>Bishkek</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G272" t="inlineStr"/>
-      <c r="H272" t="inlineStr"/>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="G272" t="n">
+        <v>42.875608</v>
+      </c>
+      <c r="H272" t="n">
+        <v>74.604613</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>FRU</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Bishkek, Kyrgyzstan</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Bishkek</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Kyrgyzstan</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G273" t="n">
-        <v>42.875608</v>
+        <v>38.94449997</v>
       </c>
       <c r="H273" t="n">
-        <v>74.604613</v>
+        <v>-77.45580292</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -10689,7 +10693,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -10703,21 +10707,21 @@
         </is>
       </c>
       <c r="G274" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H274" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10727,7 +10731,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -10741,21 +10745,21 @@
         </is>
       </c>
       <c r="G275" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="H275" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10765,7 +10769,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -10779,21 +10783,21 @@
         </is>
       </c>
       <c r="G276" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="H276" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10803,35 +10807,35 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G277" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="H277" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10841,35 +10845,35 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G278" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H278" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10879,7 +10883,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -10893,21 +10897,21 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="H279" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10917,7 +10921,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10931,21 +10935,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H280" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10955,7 +10959,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10969,21 +10973,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H281" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -10993,7 +10997,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -11007,21 +11011,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H282" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11031,7 +11035,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11045,21 +11049,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H283" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11069,7 +11073,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11083,21 +11087,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H284" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11107,7 +11111,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11121,21 +11125,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H285" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11145,7 +11149,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11159,21 +11163,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="H286" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11183,7 +11187,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11197,21 +11201,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H287" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11221,7 +11225,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11235,21 +11239,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H288" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11259,7 +11263,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -11273,21 +11277,21 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="H289" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11297,7 +11301,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11311,21 +11315,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="H290" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11335,7 +11339,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -11349,21 +11353,21 @@
         </is>
       </c>
       <c r="G291" t="n">
-        <v>33.94250107</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H291" t="n">
-        <v>-118.4079971</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11373,35 +11377,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H292" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11411,35 +11415,35 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G293" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H293" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11449,7 +11453,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
@@ -11463,21 +11467,21 @@
         </is>
       </c>
       <c r="G294" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H294" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11487,35 +11491,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>44.8819999695</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H295" t="n">
-        <v>-93.22180175779999</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11525,35 +11529,35 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G296" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H296" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11563,7 +11567,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -11577,21 +11581,21 @@
         </is>
       </c>
       <c r="G297" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H297" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11601,7 +11605,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -11615,21 +11619,21 @@
         </is>
       </c>
       <c r="G298" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H298" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11639,7 +11643,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
@@ -11653,21 +11657,21 @@
         </is>
       </c>
       <c r="G299" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H299" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11677,35 +11681,35 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G300" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H300" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11715,35 +11719,35 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G301" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H301" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11753,7 +11757,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -11767,21 +11771,21 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="H302" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11791,7 +11795,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -11805,21 +11809,21 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="H303" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11829,7 +11833,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -11843,21 +11847,21 @@
         </is>
       </c>
       <c r="G304" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="H304" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11867,35 +11871,35 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H305" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11905,35 +11909,35 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G306" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H306" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11943,7 +11947,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11957,21 +11961,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="H307" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11981,7 +11985,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -11995,21 +11999,21 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H308" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12019,7 +12023,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12033,21 +12037,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H309" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12057,7 +12061,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -12071,21 +12075,21 @@
         </is>
       </c>
       <c r="G310" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H310" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12095,35 +12099,35 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G311" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H311" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12133,35 +12137,35 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G312" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H312" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12171,12 +12175,12 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -12185,21 +12189,21 @@
         </is>
       </c>
       <c r="G313" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H313" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12209,12 +12213,12 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -12223,21 +12227,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H314" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12247,7 +12251,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -12261,21 +12265,21 @@
         </is>
       </c>
       <c r="G315" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H315" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12285,35 +12289,35 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G316" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H316" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12323,7 +12327,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12337,21 +12341,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="H317" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12361,7 +12365,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
@@ -12375,21 +12379,21 @@
         </is>
       </c>
       <c r="G318" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H318" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12399,35 +12403,35 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G319" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H319" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12437,35 +12441,35 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G320" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="H320" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12475,35 +12479,35 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G321" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="H321" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12513,7 +12517,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -12527,21 +12531,21 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="H322" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12551,7 +12555,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
@@ -12565,21 +12569,21 @@
         </is>
       </c>
       <c r="G323" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="H323" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12589,35 +12593,35 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G324" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H324" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12627,35 +12631,35 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G325" t="n">
-        <v>20.5217990875</v>
+        <v>29.429461</v>
       </c>
       <c r="H325" t="n">
-        <v>-103.3109970093</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12665,7 +12669,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12679,21 +12683,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>29.429461</v>
+        <v>41.50069</v>
       </c>
       <c r="H326" t="n">
-        <v>-98.487061</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12703,7 +12707,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12717,21 +12721,21 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>41.50069</v>
+        <v>35.93543</v>
       </c>
       <c r="H327" t="n">
-        <v>-81.68411999999999</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12741,7 +12745,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12755,21 +12759,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>35.93543</v>
+        <v>35.46655</v>
       </c>
       <c r="H328" t="n">
-        <v>-78.88075000000001</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12779,7 +12783,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12793,21 +12797,21 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>35.46655</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H329" t="n">
-        <v>-97.65373</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -12817,7 +12821,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Anchorage</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -12831,21 +12835,21 @@
         </is>
       </c>
       <c r="G330" t="n">
-        <v>27.9755001068</v>
+        <v>61.158555</v>
       </c>
       <c r="H330" t="n">
-        <v>-82.533203125</v>
+        <v>-149.890208</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -12855,61 +12859,23 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G331" t="n">
-        <v>61.158555</v>
+        <v>44.64601</v>
       </c>
       <c r="H331" t="n">
-        <v>-149.890208</v>
-      </c>
-    </row>
-    <row r="332">
-      <c r="A332" s="1" t="inlineStr">
-        <is>
-          <t>YHZ</t>
-        </is>
-      </c>
-      <c r="B332" t="inlineStr">
-        <is>
-          <t>Halifax, Canada</t>
-        </is>
-      </c>
-      <c r="C332" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="D332" t="inlineStr">
-        <is>
-          <t>Halifax</t>
-        </is>
-      </c>
-      <c r="E332" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F332" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="G332" t="n">
-        <v>44.64601</v>
-      </c>
-      <c r="H332" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 6848c1979b40649296848443192275eb6bf0ed52
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H331"/>
+  <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2492,12 +2492,12 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>ZRH</t>
+          <t>LYS</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Zurich, Switzerland</t>
+          <t>Lyon, France</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2507,35 +2507,35 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Zurich</t>
+          <t>Lyon</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>47.4646987915</v>
+        <v>45.7263</v>
       </c>
       <c r="H55" t="n">
-        <v>8.549169540399999</v>
+        <v>5.0908</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>LYS</t>
+          <t>BOD</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Lyon, France</t>
+          <t>Bordeaux, France</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Lyon</t>
+          <t>Bordeaux</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2559,21 +2559,21 @@
         </is>
       </c>
       <c r="G56" t="n">
-        <v>45.7263</v>
+        <v>44.82946</v>
       </c>
       <c r="H56" t="n">
-        <v>5.0908</v>
+        <v>-0.58355</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>BOD</t>
+          <t>SKP</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Bordeaux, France</t>
+          <t>Skopje, North Macedonia</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2583,35 +2583,35 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Bordeaux</t>
+          <t>Skopje</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>MK</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>44.82946</v>
+        <v>41.9616012573</v>
       </c>
       <c r="H57" t="n">
-        <v>-0.58355</v>
+        <v>21.6214008331</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>SKP</t>
+          <t>ZRH</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Skopje, North Macedonia</t>
+          <t>Zurich, Switzerland</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2621,24 +2621,24 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Skopje</t>
+          <t>Zurich</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>MK</t>
+          <t>CH</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>41.9616012573</v>
+        <v>47.4646987915</v>
       </c>
       <c r="H58" t="n">
-        <v>21.6214008331</v>
+        <v>8.549169540399999</v>
       </c>
     </row>
     <row r="59">
@@ -10318,118 +10318,122 @@
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>CTU</t>
+          <t>NQZ</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Chengdu, China</t>
+          <t>Astana, Kazakhstan</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Chengdu</t>
+          <t>Astana</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G264" t="inlineStr"/>
-      <c r="H264" t="inlineStr"/>
+          <t>KZ</t>
+        </is>
+      </c>
+      <c r="G264" t="n">
+        <v>51.167801</v>
+      </c>
+      <c r="H264" t="n">
+        <v>71.418893</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>NQZ</t>
+          <t>NNG</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Astana, Kazakhstan</t>
+          <t>Nanning, China</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Astana</t>
+          <t>Nanning</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G265" t="n">
-        <v>51.167801</v>
-      </c>
-      <c r="H265" t="n">
-        <v>71.418893</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr"/>
+      <c r="H265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>NNG</t>
+          <t>KCH</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Nanning, China</t>
+          <t>Kuching, Malaysia</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Nanning</t>
+          <t>Kuching</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G266" t="inlineStr"/>
-      <c r="H266" t="inlineStr"/>
+          <t>MY</t>
+        </is>
+      </c>
+      <c r="G266" t="n">
+        <v>1.709727</v>
+      </c>
+      <c r="H266" t="n">
+        <v>110.353455</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>KCH</t>
+          <t>AKX</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Kuching, Malaysia</t>
+          <t>Aktobe, Kazakhstan</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -10439,73 +10443,69 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Kuching</t>
+          <t>Aktobe</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>MY</t>
+          <t>KZ</t>
         </is>
       </c>
       <c r="G267" t="n">
-        <v>1.709727</v>
+        <v>50.286922</v>
       </c>
       <c r="H267" t="n">
-        <v>110.353455</v>
+        <v>57.224121</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>AKX</t>
+          <t>TEN</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Aktobe, Kazakhstan</t>
+          <t>Tongren, China</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Aktobe</t>
+          <t>Tongren</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>KZ</t>
-        </is>
-      </c>
-      <c r="G268" t="n">
-        <v>50.286922</v>
-      </c>
-      <c r="H268" t="n">
-        <v>57.224121</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G268" t="inlineStr"/>
+      <c r="H268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>TEN</t>
+          <t>HYN</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Tongren, China</t>
+          <t>Taizhou, China</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -10515,7 +10515,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Tongren</t>
+          <t>Taizhou</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
@@ -10534,12 +10534,12 @@
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>HYN</t>
+          <t>XNN</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Taizhou, China</t>
+          <t>Xining, China</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -10549,7 +10549,7 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Taizhou</t>
+          <t>Xining</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
@@ -10568,84 +10568,88 @@
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>XNN</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Xining, China</t>
+          <t>Bishkek, Kyrgyzstan</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Xining</t>
+          <t>Bishkek</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="G271" t="inlineStr"/>
-      <c r="H271" t="inlineStr"/>
+          <t>KG</t>
+        </is>
+      </c>
+      <c r="G271" t="n">
+        <v>42.875608</v>
+      </c>
+      <c r="H271" t="n">
+        <v>74.604613</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>FRU</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Bishkek, Kyrgyzstan</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>Asia Pacific</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Bishkek</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Kyrgyzstan</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G272" t="n">
-        <v>42.875608</v>
+        <v>38.94449997</v>
       </c>
       <c r="H272" t="n">
-        <v>74.604613</v>
+        <v>-77.45580292</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -10655,7 +10659,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -10669,21 +10673,21 @@
         </is>
       </c>
       <c r="G273" t="n">
-        <v>38.94449997</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H273" t="n">
-        <v>-77.45580292</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -10693,7 +10697,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -10707,21 +10711,21 @@
         </is>
       </c>
       <c r="G274" t="n">
-        <v>33.6366996765</v>
+        <v>42.36429977</v>
       </c>
       <c r="H274" t="n">
-        <v>-84.4281005859</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10731,7 +10735,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -10745,21 +10749,21 @@
         </is>
       </c>
       <c r="G275" t="n">
-        <v>42.36429977</v>
+        <v>42.94049835</v>
       </c>
       <c r="H275" t="n">
-        <v>-71.00520324999999</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10769,35 +10773,35 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G276" t="n">
-        <v>42.94049835</v>
+        <v>51.113899231</v>
       </c>
       <c r="H276" t="n">
-        <v>-78.73220062</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10807,35 +10811,35 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G277" t="n">
-        <v>51.113899231</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H277" t="n">
-        <v>-114.019996643</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10845,7 +10849,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -10859,21 +10863,21 @@
         </is>
       </c>
       <c r="G278" t="n">
-        <v>35.2140007019</v>
+        <v>41.97859955</v>
       </c>
       <c r="H278" t="n">
-        <v>-80.94309997560001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10883,7 +10887,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -10897,21 +10901,21 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>41.97859955</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H279" t="n">
-        <v>-87.90480042</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10921,7 +10925,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10935,21 +10939,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>39.9980010986</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H280" t="n">
-        <v>-82.89189910890001</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10959,7 +10963,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10973,21 +10977,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>32.8968009949</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H281" t="n">
-        <v>-97.0380020142</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -10997,7 +11001,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -11011,21 +11015,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>39.8616981506</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H282" t="n">
-        <v>-104.672996521</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11035,7 +11039,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11049,21 +11053,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>42.2123985291</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H283" t="n">
-        <v>-83.35340118409999</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11073,7 +11077,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11087,21 +11091,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>21.3187007904</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H284" t="n">
-        <v>-157.9219970703</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11111,7 +11115,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11125,21 +11129,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>29.9843997955</v>
+        <v>39.717300415</v>
       </c>
       <c r="H285" t="n">
-        <v>-95.34140014650001</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11149,7 +11153,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11163,21 +11167,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>39.717300415</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H286" t="n">
-        <v>-86.2944030762</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11187,7 +11191,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11201,21 +11205,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>30.4941005707</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H287" t="n">
-        <v>-81.68789672849999</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11225,7 +11229,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11239,21 +11243,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>39.2975997925</v>
+        <v>36.08010101</v>
       </c>
       <c r="H288" t="n">
-        <v>-94.7138977051</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11263,7 +11267,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -11277,21 +11281,21 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>36.08010101</v>
+        <v>33.94250107</v>
       </c>
       <c r="H289" t="n">
-        <v>-115.1520004</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11301,7 +11305,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11315,21 +11319,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>33.94250107</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H290" t="n">
-        <v>-118.4079971</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11339,35 +11343,35 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G291" t="n">
-        <v>35.0424003601</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H291" t="n">
-        <v>-89.9766998291</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11377,35 +11381,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>19.4363002777</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H292" t="n">
-        <v>-99.07209777830001</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11415,7 +11419,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -11429,21 +11433,21 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>25.7931995392</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H293" t="n">
-        <v>-80.2906036377</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11453,35 +11457,35 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G294" t="n">
-        <v>44.8819999695</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H294" t="n">
-        <v>-93.22180175779999</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11491,35 +11495,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>45.4706001282</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H295" t="n">
-        <v>-73.7407989502</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11529,7 +11533,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11543,21 +11547,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>36.1245002747</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H296" t="n">
-        <v>-86.6781997681</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11567,7 +11571,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -11581,21 +11585,21 @@
         </is>
       </c>
       <c r="G297" t="n">
-        <v>40.6925010681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H297" t="n">
-        <v>-74.1687011719</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11605,7 +11609,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -11619,21 +11623,21 @@
         </is>
       </c>
       <c r="G298" t="n">
-        <v>36.8945999146</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H298" t="n">
-        <v>-76.2012023926</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11643,35 +11647,35 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G299" t="n">
-        <v>41.3031997681</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H299" t="n">
-        <v>-95.89409637449999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11681,35 +11685,35 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G300" t="n">
-        <v>45.3224983215</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H300" t="n">
-        <v>-75.66919708250001</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11719,7 +11723,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11733,21 +11737,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>39.8718986511</v>
+        <v>33.434299469</v>
       </c>
       <c r="H301" t="n">
-        <v>-75.24109649659999</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11757,7 +11761,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -11771,21 +11775,21 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>33.434299469</v>
+        <v>40.49150085</v>
       </c>
       <c r="H302" t="n">
-        <v>-112.012001038</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11795,7 +11799,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -11809,21 +11813,21 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>40.49150085</v>
+        <v>45.58869934</v>
       </c>
       <c r="H303" t="n">
-        <v>-80.23290253</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11833,35 +11837,35 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G304" t="n">
-        <v>45.58869934</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H304" t="n">
-        <v>-122.5979996</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11871,35 +11875,35 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>20.6173000336</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H305" t="n">
-        <v>-100.185997009</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11909,7 +11913,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11923,21 +11927,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>37.5051994324</v>
+        <v>38.695400238</v>
       </c>
       <c r="H306" t="n">
-        <v>-77.3197021484</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11947,7 +11951,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11961,21 +11965,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>38.695400238</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H307" t="n">
-        <v>-121.591003418</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11985,7 +11989,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -11999,21 +12003,21 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>40.7883987427</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H308" t="n">
-        <v>-111.977996826</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12023,7 +12027,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12037,21 +12041,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>32.7336006165</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H309" t="n">
-        <v>-117.190002441</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12061,35 +12065,35 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G310" t="n">
-        <v>37.3625984192</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H310" t="n">
-        <v>-121.929000855</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12099,35 +12103,35 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G311" t="n">
-        <v>52.1707992554</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H311" t="n">
-        <v>-106.699996948</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, South Dakota</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12137,12 +12141,12 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>South Dakota</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -12151,21 +12155,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>47.4490013123</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H312" t="n">
-        <v>-122.308998108</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12175,12 +12179,12 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -12189,21 +12193,21 @@
         </is>
       </c>
       <c r="G313" t="n">
-        <v>43.540819819502</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H313" t="n">
-        <v>-96.65511577730963</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12213,7 +12217,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -12227,21 +12231,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>38.7486991882</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H314" t="n">
-        <v>-90.37000274659999</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12251,35 +12255,35 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G315" t="n">
-        <v>30.3964996338</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H315" t="n">
-        <v>-84.3503036499</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12289,7 +12293,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -12303,21 +12307,21 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>43.6772003174</v>
+        <v>49.193901062</v>
       </c>
       <c r="H316" t="n">
-        <v>-79.63059997560001</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12327,7 +12331,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12341,21 +12345,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>49.193901062</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H317" t="n">
-        <v>-123.183998108</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12365,35 +12369,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>49.9099998474</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H318" t="n">
-        <v>-97.2398986816</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12403,35 +12407,35 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G319" t="n">
-        <v>37.6189994812</v>
+        <v>17.9951</v>
       </c>
       <c r="H319" t="n">
-        <v>-122.375</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12441,35 +12445,35 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G320" t="n">
-        <v>17.9951</v>
+        <v>44.8081</v>
       </c>
       <c r="H320" t="n">
-        <v>-76.7846</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12479,7 +12483,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -12493,21 +12497,21 @@
         </is>
       </c>
       <c r="G321" t="n">
-        <v>44.8081</v>
+        <v>30.1975</v>
       </c>
       <c r="H321" t="n">
-        <v>-68.795</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12517,7 +12521,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -12531,21 +12535,21 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>30.1975</v>
+        <v>35.0844</v>
       </c>
       <c r="H322" t="n">
-        <v>-97.6664</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12555,35 +12559,35 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>35.0844</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H323" t="n">
-        <v>-106.6504</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12593,35 +12597,35 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G324" t="n">
-        <v>20.5217990875</v>
+        <v>29.429461</v>
       </c>
       <c r="H324" t="n">
-        <v>-103.3109970093</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12631,7 +12635,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12645,21 +12649,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>29.429461</v>
+        <v>41.50069</v>
       </c>
       <c r="H325" t="n">
-        <v>-98.487061</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12669,7 +12673,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12683,21 +12687,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>41.50069</v>
+        <v>35.93543</v>
       </c>
       <c r="H326" t="n">
-        <v>-81.68411999999999</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12707,7 +12711,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12721,21 +12725,21 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>35.93543</v>
+        <v>35.46655</v>
       </c>
       <c r="H327" t="n">
-        <v>-78.88075000000001</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12745,7 +12749,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12759,21 +12763,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>35.46655</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H328" t="n">
-        <v>-97.65373</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Anchorage, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12783,7 +12787,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Anchorage</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12797,21 +12801,21 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>27.9755001068</v>
+        <v>61.158555</v>
       </c>
       <c r="H329" t="n">
-        <v>-82.533203125</v>
+        <v>-149.890208</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -12821,61 +12825,23 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G330" t="n">
-        <v>61.158555</v>
+        <v>44.64601</v>
       </c>
       <c r="H330" t="n">
-        <v>-149.890208</v>
-      </c>
-    </row>
-    <row r="331">
-      <c r="A331" s="1" t="inlineStr">
-        <is>
-          <t>YHZ</t>
-        </is>
-      </c>
-      <c r="B331" t="inlineStr">
-        <is>
-          <t>Halifax, Canada</t>
-        </is>
-      </c>
-      <c r="C331" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="D331" t="inlineStr">
-        <is>
-          <t>Halifax</t>
-        </is>
-      </c>
-      <c r="E331" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F331" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="G331" t="n">
-        <v>44.64601</v>
-      </c>
-      <c r="H331" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 0d5890206fc5c8d2130f62280015edc63074cbd7
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -4312,12 +4312,12 @@
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>CGB</t>
+          <t>CWB</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Cuiaba, Brazil</t>
+          <t>Curitiba, Brazil</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -4327,7 +4327,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Cuiaba</t>
+          <t>Curitiba</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -4341,21 +4341,21 @@
         </is>
       </c>
       <c r="G103" t="n">
-        <v>-15.59611</v>
+        <v>-25.5284996033</v>
       </c>
       <c r="H103" t="n">
-        <v>-56.09667</v>
+        <v>-49.1758003235</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>CWB</t>
+          <t>FLN</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Curitiba, Brazil</t>
+          <t>Florianopolis, Brazil</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -4365,7 +4365,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Curitiba</t>
+          <t>Florianopolis</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -4379,21 +4379,21 @@
         </is>
       </c>
       <c r="G104" t="n">
-        <v>-25.5284996033</v>
+        <v>-27.6702785492</v>
       </c>
       <c r="H104" t="n">
-        <v>-49.1758003235</v>
+        <v>-48.5525016785</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>FLN</t>
+          <t>FOR</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Florianopolis, Brazil</t>
+          <t>Fortaleza, Brazil</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -4403,7 +4403,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Florianopolis</t>
+          <t>Fortaleza</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -4417,21 +4417,21 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>-27.6702785492</v>
+        <v>-3.7762799263</v>
       </c>
       <c r="H105" t="n">
-        <v>-48.5525016785</v>
+        <v>-38.5326004028</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>FOR</t>
+          <t>GEO</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Fortaleza, Brazil</t>
+          <t>Georgetown, Guyana</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -4441,35 +4441,35 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Fortaleza</t>
+          <t>Georgetown</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Guyana</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GY</t>
         </is>
       </c>
       <c r="G106" t="n">
-        <v>-3.7762799263</v>
+        <v>6.825648</v>
       </c>
       <c r="H106" t="n">
-        <v>-38.5326004028</v>
+        <v>-58.163756</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>GEO</t>
+          <t>GYN</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Georgetown, Guyana</t>
+          <t>Goiania, Brazil</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -4479,111 +4479,111 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Georgetown</t>
+          <t>Goiania</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Guyana</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>GY</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G107" t="n">
-        <v>6.825648</v>
+        <v>-16.69727</v>
       </c>
       <c r="H107" t="n">
-        <v>-58.163756</v>
+        <v>-49.26851</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="inlineStr">
         <is>
-          <t>GYN</t>
+          <t>GUA</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Goiania, Brazil</t>
+          <t>Guatemala City, Guatemala</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Goiania</t>
+          <t>Guatemala City</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Guatemala</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>GT</t>
         </is>
       </c>
       <c r="G108" t="n">
-        <v>-16.69727</v>
+        <v>14.5832996368</v>
       </c>
       <c r="H108" t="n">
-        <v>-49.26851</v>
+        <v>-90.5274963379</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="inlineStr">
         <is>
-          <t>GUA</t>
+          <t>GYE</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Guatemala City, Guatemala</t>
+          <t>Guayaquil, Ecuador</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Guatemala City</t>
+          <t>Guayaquil</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>Guatemala</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>GT</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="G109" t="n">
-        <v>14.5832996368</v>
+        <v>-2.1894</v>
       </c>
       <c r="H109" t="n">
-        <v>-90.5274963379</v>
+        <v>-79.8891</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="inlineStr">
         <is>
-          <t>GYE</t>
+          <t>ITJ</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Guayaquil, Ecuador</t>
+          <t>Itajai, Brazil</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -4593,35 +4593,35 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Guayaquil</t>
+          <t>Itajai</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G110" t="n">
-        <v>-2.1894</v>
+        <v>-27.6116676331</v>
       </c>
       <c r="H110" t="n">
-        <v>-79.8891</v>
+        <v>-48.6727790833</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="inlineStr">
         <is>
-          <t>ITJ</t>
+          <t>JOI</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Itajai, Brazil</t>
+          <t>Joinville, Brazil</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -4631,7 +4631,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Itajai</t>
+          <t>Joinville</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -4645,21 +4645,21 @@
         </is>
       </c>
       <c r="G111" t="n">
-        <v>-27.6116676331</v>
+        <v>-26.304408</v>
       </c>
       <c r="H111" t="n">
-        <v>-48.6727790833</v>
+        <v>-48.846383</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="inlineStr">
         <is>
-          <t>JOI</t>
+          <t>JDO</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Joinville, Brazil</t>
+          <t>Juazeiro do Norte, Brazil</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4669,7 +4669,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Joinville</t>
+          <t>Juazeiro do Norte</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -4683,21 +4683,21 @@
         </is>
       </c>
       <c r="G112" t="n">
-        <v>-26.304408</v>
+        <v>-7.2242</v>
       </c>
       <c r="H112" t="n">
-        <v>-48.846383</v>
+        <v>-39.313</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="inlineStr">
         <is>
-          <t>JDO</t>
+          <t>LIM</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte, Brazil</t>
+          <t>Lima, Peru</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -4707,35 +4707,35 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Juazeiro do Norte</t>
+          <t>Lima</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="G113" t="n">
-        <v>-7.2242</v>
+        <v>-12.021900177</v>
       </c>
       <c r="H113" t="n">
-        <v>-39.313</v>
+        <v>-77.1143035889</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="inlineStr">
         <is>
-          <t>LIM</t>
+          <t>MAO</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Lima, Peru</t>
+          <t>Manaus, Brazil</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4745,35 +4745,35 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Manaus</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>PE</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G114" t="n">
-        <v>-12.021900177</v>
+        <v>-3.11286</v>
       </c>
       <c r="H114" t="n">
-        <v>-77.1143035889</v>
+        <v>-60.01949</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="inlineStr">
         <is>
-          <t>MAO</t>
+          <t>MDE</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Manaus, Brazil</t>
+          <t>Medellín, Colombia</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4783,35 +4783,35 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Manaus</t>
+          <t>Medellín</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="G115" t="n">
-        <v>-3.11286</v>
+        <v>6.16454</v>
       </c>
       <c r="H115" t="n">
-        <v>-60.01949</v>
+        <v>-75.42310000000001</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="inlineStr">
         <is>
-          <t>MDE</t>
+          <t>NQN</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Medellín, Colombia</t>
+          <t>Neuquen, Argentina</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -4821,35 +4821,35 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Medellín</t>
+          <t>Neuquen</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Argentina</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="G116" t="n">
-        <v>6.16454</v>
+        <v>-38.9490013123</v>
       </c>
       <c r="H116" t="n">
-        <v>-75.42310000000001</v>
+        <v>-68.1557006836</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="inlineStr">
         <is>
-          <t>NQN</t>
+          <t>PTY</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Neuquen, Argentina</t>
+          <t>Panama City, Panama</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -4859,35 +4859,35 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Neuquen</t>
+          <t>Panama City</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Argentina</t>
+          <t>Panama</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="G117" t="n">
-        <v>-38.9490013123</v>
+        <v>9.0713596344</v>
       </c>
       <c r="H117" t="n">
-        <v>-68.1557006836</v>
+        <v>-79.3834991455</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="inlineStr">
         <is>
-          <t>PTY</t>
+          <t>PBM</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Panama City, Panama</t>
+          <t>Paramaribo, Suriname</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4897,35 +4897,35 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Panama City</t>
+          <t>Paramaribo</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Panama</t>
+          <t>Suriname</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>SR</t>
         </is>
       </c>
       <c r="G118" t="n">
-        <v>9.0713596344</v>
+        <v>5.452831</v>
       </c>
       <c r="H118" t="n">
-        <v>-79.3834991455</v>
+        <v>-55.187783</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="inlineStr">
         <is>
-          <t>PBM</t>
+          <t>POA</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Paramaribo, Suriname</t>
+          <t>Porto Alegre, Brazil</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4935,35 +4935,35 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Paramaribo</t>
+          <t>Porto Alegre</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Suriname</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>SR</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G119" t="n">
-        <v>5.452831</v>
+        <v>-29.9944000244</v>
       </c>
       <c r="H119" t="n">
-        <v>-55.187783</v>
+        <v>-51.1713981628</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="inlineStr">
         <is>
-          <t>POA</t>
+          <t>UIO</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Porto Alegre, Brazil</t>
+          <t>Quito, Ecuador</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4973,35 +4973,35 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Porto Alegre</t>
+          <t>Quito</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Ecuador</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>EC</t>
         </is>
       </c>
       <c r="G120" t="n">
-        <v>-29.9944000244</v>
+        <v>-0.1291666667</v>
       </c>
       <c r="H120" t="n">
-        <v>-51.1713981628</v>
+        <v>-78.3575</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="inlineStr">
         <is>
-          <t>UIO</t>
+          <t>REC</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Quito, Ecuador</t>
+          <t>Recife, Brazil</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -5011,35 +5011,35 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Quito</t>
+          <t>Recife</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Ecuador</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>EC</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>-0.1291666667</v>
+        <v>-8.126489639300001</v>
       </c>
       <c r="H121" t="n">
-        <v>-78.3575</v>
+        <v>-34.9235992432</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="inlineStr">
         <is>
-          <t>REC</t>
+          <t>RAO</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Recife, Brazil</t>
+          <t>Ribeirao Preto, Brazil</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -5049,7 +5049,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Recife</t>
+          <t>Ribeirao Preto</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -5063,21 +5063,21 @@
         </is>
       </c>
       <c r="G122" t="n">
-        <v>-8.126489639300001</v>
+        <v>-21.1363887787</v>
       </c>
       <c r="H122" t="n">
-        <v>-34.9235992432</v>
+        <v>-47.7766685486</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="inlineStr">
         <is>
-          <t>RAO</t>
+          <t>GIG</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Ribeirao Preto, Brazil</t>
+          <t>Rio de Janeiro, Brazil</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -5087,7 +5087,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Ribeirao Preto</t>
+          <t>Rio de Janeiro</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -5101,21 +5101,21 @@
         </is>
       </c>
       <c r="G123" t="n">
-        <v>-21.1363887787</v>
+        <v>-22.8099994659</v>
       </c>
       <c r="H123" t="n">
-        <v>-47.7766685486</v>
+        <v>-43.2505569458</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="inlineStr">
         <is>
-          <t>GIG</t>
+          <t>SJO</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Rio de Janeiro, Brazil</t>
+          <t>San José, Costa Rica</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -5125,35 +5125,35 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Rio de Janeiro</t>
+          <t>San José</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>CR</t>
         </is>
       </c>
       <c r="G124" t="n">
-        <v>-22.8099994659</v>
+        <v>9.9938602448</v>
       </c>
       <c r="H124" t="n">
-        <v>-43.2505569458</v>
+        <v>-84.2088012695</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="inlineStr">
         <is>
-          <t>SJO</t>
+          <t>SCL</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>San José, Costa Rica</t>
+          <t>Santiago, Chile</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -5163,111 +5163,111 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>San José</t>
+          <t>Santiago</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>CR</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="G125" t="n">
-        <v>9.9938602448</v>
+        <v>-33.3930015564</v>
       </c>
       <c r="H125" t="n">
-        <v>-84.2088012695</v>
+        <v>-70.7857971191</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>SDQ</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Santiago, Chile</t>
+          <t>Santo Domingo, Dominican Republic</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Santiago</t>
+          <t>Santo Domingo</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Dominican Republic</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="G126" t="n">
-        <v>-33.3930015564</v>
+        <v>18.4297008514</v>
       </c>
       <c r="H126" t="n">
-        <v>-70.7857971191</v>
+        <v>-69.6688995361</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="inlineStr">
         <is>
-          <t>SDQ</t>
+          <t>SJP</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Santo Domingo, Dominican Republic</t>
+          <t>São José do Rio Preto, Brazil</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Santo Domingo</t>
+          <t>São José do Rio Preto</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Dominican Republic</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G127" t="n">
-        <v>18.4297008514</v>
+        <v>-20.807157</v>
       </c>
       <c r="H127" t="n">
-        <v>-69.6688995361</v>
+        <v>-49.378994</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="inlineStr">
         <is>
-          <t>SJP</t>
+          <t>SJK</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>São José do Rio Preto, Brazil</t>
+          <t>São José dos Campos, Brazil</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -5277,7 +5277,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>São José do Rio Preto</t>
+          <t>São José dos Campos</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -5291,21 +5291,21 @@
         </is>
       </c>
       <c r="G128" t="n">
-        <v>-20.807157</v>
+        <v>-23.1791</v>
       </c>
       <c r="H128" t="n">
-        <v>-49.378994</v>
+        <v>-45.8872</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="inlineStr">
         <is>
-          <t>SJK</t>
+          <t>GRU</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>São José dos Campos, Brazil</t>
+          <t>São Paulo, Brazil</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -5315,7 +5315,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>São José dos Campos</t>
+          <t>São Paulo</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -5329,21 +5329,21 @@
         </is>
       </c>
       <c r="G129" t="n">
-        <v>-23.1791</v>
+        <v>-23.4355564117</v>
       </c>
       <c r="H129" t="n">
-        <v>-45.8872</v>
+        <v>-46.4730567932</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="inlineStr">
         <is>
-          <t>GRU</t>
+          <t>SOD</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>São Paulo, Brazil</t>
+          <t>Sorocaba, Brazil</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Sorocaba</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -5367,21 +5367,21 @@
         </is>
       </c>
       <c r="G130" t="n">
-        <v>-23.4355564117</v>
+        <v>-23.54389</v>
       </c>
       <c r="H130" t="n">
-        <v>-46.4730567932</v>
+        <v>-46.63445</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="inlineStr">
         <is>
-          <t>SOD</t>
+          <t>TGU</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Sorocaba, Brazil</t>
+          <t>Tegucigalpa, Honduras</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -5391,35 +5391,35 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Sorocaba</t>
+          <t>Tegucigalpa</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Honduras</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>HN</t>
         </is>
       </c>
       <c r="G131" t="n">
-        <v>-23.54389</v>
+        <v>14.0608</v>
       </c>
       <c r="H131" t="n">
-        <v>-46.63445</v>
+        <v>-87.21720000000001</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="inlineStr">
         <is>
-          <t>TGU</t>
+          <t>NVT</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Tegucigalpa, Honduras</t>
+          <t>Timbo, Brazil</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -5429,35 +5429,35 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Tegucigalpa</t>
+          <t>Timbo</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Honduras</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>HN</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G132" t="n">
-        <v>14.0608</v>
+        <v>-26.8251</v>
       </c>
       <c r="H132" t="n">
-        <v>-87.21720000000001</v>
+        <v>-49.2695</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>UDI</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Timbo, Brazil</t>
+          <t>Uberlandia, Brazil</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -5467,7 +5467,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Timbo</t>
+          <t>Uberlandia</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -5481,21 +5481,21 @@
         </is>
       </c>
       <c r="G133" t="n">
-        <v>-26.8251</v>
+        <v>-18.8836116791</v>
       </c>
       <c r="H133" t="n">
-        <v>-49.2695</v>
+        <v>-48.225276947</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="inlineStr">
         <is>
-          <t>UDI</t>
+          <t>VIX</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Uberlandia, Brazil</t>
+          <t>Vitoria, Brazil</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -5505,7 +5505,7 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Uberlandia</t>
+          <t>Vitoria</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -5519,21 +5519,21 @@
         </is>
       </c>
       <c r="G134" t="n">
-        <v>-18.8836116791</v>
+        <v>-20.64871</v>
       </c>
       <c r="H134" t="n">
-        <v>-48.225276947</v>
+        <v>-41.90857</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>CAW</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Vitoria, Brazil</t>
+          <t>Campos dos Goytacazes, Brazil</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -5543,7 +5543,7 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Vitoria</t>
+          <t>Campos dos Goytacazes</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -5557,21 +5557,21 @@
         </is>
       </c>
       <c r="G135" t="n">
-        <v>-20.64871</v>
+        <v>-21.698299408</v>
       </c>
       <c r="H135" t="n">
-        <v>-41.90857</v>
+        <v>-41.301700592</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="inlineStr">
         <is>
-          <t>CAW</t>
+          <t>XAP</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes, Brazil</t>
+          <t>Chapeco, Brazil</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -5581,7 +5581,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Campos dos Goytacazes</t>
+          <t>Chapeco</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -5595,249 +5595,249 @@
         </is>
       </c>
       <c r="G136" t="n">
-        <v>-21.698299408</v>
+        <v>-27.1341991425</v>
       </c>
       <c r="H136" t="n">
-        <v>-41.301700592</v>
+        <v>-52.6566009521</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="inlineStr">
         <is>
-          <t>XAP</t>
+          <t>BGI</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Chapeco, Brazil</t>
+          <t>Bridgetown, Barbados</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Chapeco</t>
+          <t>Bridgetown</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Barbados</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>BB</t>
         </is>
       </c>
       <c r="G137" t="n">
-        <v>-27.1341991425</v>
+        <v>13.103562</v>
       </c>
       <c r="H137" t="n">
-        <v>-52.6566009521</v>
+        <v>-59.603226</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="inlineStr">
         <is>
-          <t>BGI</t>
+          <t>GND</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Bridgetown, Barbados</t>
+          <t>St. George's, Grenada</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Bridgetown</t>
+          <t>St. George's</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Barbados</t>
+          <t>Grenada</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>BB</t>
+          <t>GD</t>
         </is>
       </c>
       <c r="G138" t="n">
-        <v>13.103562</v>
+        <v>12.007116</v>
       </c>
       <c r="H138" t="n">
-        <v>-59.603226</v>
+        <v>-61.7882288</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="inlineStr">
         <is>
-          <t>GND</t>
+          <t>STI</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>St. George's, Grenada</t>
+          <t>Santiago de los Caballeros, Dominican Republic</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>St. George's</t>
+          <t>Santiago de los Caballeros</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Grenada</t>
+          <t>Dominican Republic</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>GD</t>
+          <t>DO</t>
         </is>
       </c>
       <c r="G139" t="n">
-        <v>12.007116</v>
+        <v>19.4060993195</v>
       </c>
       <c r="H139" t="n">
-        <v>-61.7882288</v>
+        <v>-70.60469818120001</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="inlineStr">
         <is>
-          <t>STI</t>
+          <t>LPB</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Santiago de los Caballeros, Dominican Republic</t>
+          <t>La Paz, Bolivia</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Santiago de los Caballeros</t>
+          <t>La Paz</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Dominican Republic</t>
+          <t>Bolivia</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>DO</t>
+          <t>BO</t>
         </is>
       </c>
       <c r="G140" t="n">
-        <v>19.4060993195</v>
+        <v>-16.4897</v>
       </c>
       <c r="H140" t="n">
-        <v>-70.60469818120001</v>
+        <v>-68.1193</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="inlineStr">
         <is>
-          <t>LPB</t>
+          <t>SJU</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>La Paz, Bolivia</t>
+          <t>San Juan, Puerto Rico</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>South America</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>La Paz</t>
+          <t>San Juan</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Bolivia</t>
+          <t>Puerto Rico</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>BO</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="G141" t="n">
-        <v>-16.4897</v>
+        <v>18.411391</v>
       </c>
       <c r="H141" t="n">
-        <v>-68.1193</v>
+        <v>-66.10279300000001</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="inlineStr">
         <is>
-          <t>SJU</t>
+          <t>BAQ</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>San Juan, Puerto Rico</t>
+          <t>Barranquilla, Colombia</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>South America</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>San Juan</t>
+          <t>Barranquilla</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Puerto Rico</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="G142" t="n">
-        <v>18.411391</v>
+        <v>10.8896</v>
       </c>
       <c r="H142" t="n">
-        <v>-66.10279300000001</v>
+        <v>-74.7808</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="inlineStr">
         <is>
-          <t>BAQ</t>
+          <t>PMW</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Barranquilla, Colombia</t>
+          <t>Palmas, Brazil</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -5847,35 +5847,35 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Barranquilla</t>
+          <t>Palmas</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G143" t="n">
-        <v>10.8896</v>
+        <v>-10.2915000916</v>
       </c>
       <c r="H143" t="n">
-        <v>-74.7808</v>
+        <v>-48.3569984436</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="inlineStr">
         <is>
-          <t>PMW</t>
+          <t>ARU</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Palmas, Brazil</t>
+          <t>Aracatuba, Brazil</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -5885,7 +5885,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Palmas</t>
+          <t>Aracatuba</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -5899,21 +5899,21 @@
         </is>
       </c>
       <c r="G144" t="n">
-        <v>-10.2915000916</v>
+        <v>-21.1413002014</v>
       </c>
       <c r="H144" t="n">
-        <v>-48.3569984436</v>
+        <v>-50.4247016907</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="inlineStr">
         <is>
-          <t>ARU</t>
+          <t>POS</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Aracatuba, Brazil</t>
+          <t>Port of Spain, Trinidad and Tobago</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -5923,35 +5923,35 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Aracatuba</t>
+          <t>Port of Spain</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Trinidad and Tobago</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>BR</t>
+          <t>TT</t>
         </is>
       </c>
       <c r="G145" t="n">
-        <v>-21.1413002014</v>
+        <v>10.5953998566</v>
       </c>
       <c r="H145" t="n">
-        <v>-50.4247016907</v>
+        <v>-61.3372001648</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="inlineStr">
         <is>
-          <t>POS</t>
+          <t>SSA</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Port of Spain, Trinidad and Tobago</t>
+          <t>Salvador, Brazil</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -5961,35 +5961,35 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Port of Spain</t>
+          <t>Salvador</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Trinidad and Tobago</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>TT</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="G146" t="n">
-        <v>10.5953998566</v>
+        <v>-12.9086112976</v>
       </c>
       <c r="H146" t="n">
-        <v>-61.3372001648</v>
+        <v>-38.3224983215</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="inlineStr">
         <is>
-          <t>SSA</t>
+          <t>CGB</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Salvador, Brazil</t>
+          <t>Cuiaba, Brazil</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -5999,7 +5999,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Salvador</t>
+          <t>Cuiaba</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -6013,10 +6013,10 @@
         </is>
       </c>
       <c r="G147" t="n">
-        <v>-12.9086112976</v>
+        <v>-15.59611</v>
       </c>
       <c r="H147" t="n">
-        <v>-38.3224983215</v>
+        <v>-56.09667</v>
       </c>
     </row>
     <row r="148">
@@ -6934,12 +6934,12 @@
     <row r="172">
       <c r="A172" s="1" t="inlineStr">
         <is>
-          <t>RUN</t>
+          <t>TUN</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Saint-Denis, Réunion</t>
+          <t>Tunis, Tunisia</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -6949,35 +6949,35 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Saint-Denis</t>
+          <t>Tunis</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Réunion</t>
+          <t>Tunisia</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>RE</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="G172" t="n">
-        <v>-20.8871002197</v>
+        <v>36.8510017395</v>
       </c>
       <c r="H172" t="n">
-        <v>55.5102996826</v>
+        <v>10.2271995544</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="inlineStr">
         <is>
-          <t>TUN</t>
+          <t>FIH</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Tunis, Tunisia</t>
+          <t>Kinshasa, DR Congo</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -6987,35 +6987,35 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Tunis</t>
+          <t>Kinshasa</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Tunisia</t>
+          <t>DR Congo</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>CD</t>
         </is>
       </c>
       <c r="G173" t="n">
-        <v>36.8510017395</v>
+        <v>-4.3857498169</v>
       </c>
       <c r="H173" t="n">
-        <v>10.2271995544</v>
+        <v>15.4446001053</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="inlineStr">
         <is>
-          <t>FIH</t>
+          <t>CAI</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Kinshasa, DR Congo</t>
+          <t>Cairo, Egypt</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -7025,35 +7025,35 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Kinshasa</t>
+          <t>Cairo</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>DR Congo</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>EG</t>
         </is>
       </c>
       <c r="G174" t="n">
-        <v>-4.3857498169</v>
+        <v>30.1219005585</v>
       </c>
       <c r="H174" t="n">
-        <v>15.4446001053</v>
+        <v>31.4055995941</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="inlineStr">
         <is>
-          <t>CAI</t>
+          <t>WDH</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Cairo, Egypt</t>
+          <t>Windhoek, Namibia</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -7063,35 +7063,35 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Cairo</t>
+          <t>Windhoek</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Namibia</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>NA</t>
         </is>
       </c>
       <c r="G175" t="n">
-        <v>30.1219005585</v>
+        <v>-22.565587</v>
       </c>
       <c r="H175" t="n">
-        <v>31.4055995941</v>
+        <v>17.085334</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="inlineStr">
         <is>
-          <t>WDH</t>
+          <t>ASK</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Windhoek, Namibia</t>
+          <t>Yamoussoukro, Ivory Coast</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -7101,35 +7101,35 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Windhoek</t>
+          <t>Yamoussoukro</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>Namibia</t>
+          <t>Ivory Coast</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>CI</t>
         </is>
       </c>
       <c r="G176" t="n">
-        <v>-22.565587</v>
+        <v>6.842178</v>
       </c>
       <c r="H176" t="n">
-        <v>17.085334</v>
+        <v>-5.259932</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="inlineStr">
         <is>
-          <t>ASK</t>
+          <t>ABJ</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Yamoussoukro, Ivory Coast</t>
+          <t>Abidjan, Ivory Coast</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -7139,7 +7139,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Yamoussoukro</t>
+          <t>Abidjan</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -7153,21 +7153,21 @@
         </is>
       </c>
       <c r="G177" t="n">
-        <v>6.842178</v>
+        <v>5.292598</v>
       </c>
       <c r="H177" t="n">
-        <v>-5.259932</v>
+        <v>-3.999133</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="inlineStr">
         <is>
-          <t>ABJ</t>
+          <t>EBB</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Abidjan, Ivory Coast</t>
+          <t>Kampala, Uganda</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -7177,35 +7177,35 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Abidjan</t>
+          <t>Kampala</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Ivory Coast</t>
+          <t>Uganda</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>CI</t>
+          <t>UG</t>
         </is>
       </c>
       <c r="G178" t="n">
-        <v>5.292598</v>
+        <v>0.3152</v>
       </c>
       <c r="H178" t="n">
-        <v>-3.999133</v>
+        <v>32.5816</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="inlineStr">
         <is>
-          <t>EBB</t>
+          <t>RUN</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Kampala, Uganda</t>
+          <t>Saint-Denis, Réunion</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -7215,24 +7215,24 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Kampala</t>
+          <t>Saint-Denis</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Uganda</t>
+          <t>Réunion</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>UG</t>
+          <t>RE</t>
         </is>
       </c>
       <c r="G179" t="n">
-        <v>0.3152</v>
+        <v>-20.8871002197</v>
       </c>
       <c r="H179" t="n">
-        <v>32.5816</v>
+        <v>55.5102996826</v>
       </c>
     </row>
     <row r="180">
@@ -12055,7 +12055,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Sioux Falls, South Dakota</t>
+          <t>Sioux Falls, SD, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12070,7 +12070,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>South Dakota</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">

</xml_diff>

<commit_message>
update generated data Triggered by 7e272f75421d465285dffb6c6eb6b86070fcef1b
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H328"/>
+  <dimension ref="A1:H329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10530,50 +10530,50 @@
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>MLG</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Malang, Indonesia</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Malang</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="G270" t="n">
-        <v>38.94449997</v>
+        <v>-8.100346999999999</v>
       </c>
       <c r="H270" t="n">
-        <v>-77.45580292</v>
+        <v>112.186641</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -10583,7 +10583,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
@@ -10597,21 +10597,21 @@
         </is>
       </c>
       <c r="G271" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="H271" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -10621,7 +10621,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
@@ -10635,21 +10635,21 @@
         </is>
       </c>
       <c r="G272" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H272" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -10659,7 +10659,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -10673,21 +10673,21 @@
         </is>
       </c>
       <c r="G273" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="H273" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -10697,35 +10697,35 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G274" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="H274" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10735,35 +10735,35 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G275" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="H275" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10773,7 +10773,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -10787,21 +10787,21 @@
         </is>
       </c>
       <c r="G276" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H276" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10811,7 +10811,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -10825,21 +10825,21 @@
         </is>
       </c>
       <c r="G277" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="H277" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10849,7 +10849,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -10863,21 +10863,21 @@
         </is>
       </c>
       <c r="G278" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H278" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10887,7 +10887,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -10901,21 +10901,21 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H279" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10925,7 +10925,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10939,21 +10939,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H280" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10977,21 +10977,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H281" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -11001,7 +11001,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -11015,21 +11015,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H282" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11039,7 +11039,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11053,21 +11053,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H283" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11077,7 +11077,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11091,21 +11091,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="H284" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11115,7 +11115,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11129,21 +11129,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H285" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11153,7 +11153,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11167,21 +11167,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H286" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11191,7 +11191,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11205,21 +11205,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="H287" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11229,7 +11229,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11243,21 +11243,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>35.0424003601</v>
+        <v>33.94250107</v>
       </c>
       <c r="H288" t="n">
-        <v>-89.9766998291</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11267,35 +11267,35 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G289" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H289" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11305,35 +11305,35 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G290" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H290" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11343,7 +11343,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -11357,21 +11357,21 @@
         </is>
       </c>
       <c r="G291" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H291" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11381,35 +11381,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>45.4706001282</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H292" t="n">
-        <v>-73.7407989502</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11419,35 +11419,35 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G293" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H293" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11457,7 +11457,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
@@ -11471,21 +11471,21 @@
         </is>
       </c>
       <c r="G294" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H294" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11495,7 +11495,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
@@ -11509,21 +11509,21 @@
         </is>
       </c>
       <c r="G295" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H295" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11533,7 +11533,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11547,21 +11547,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H296" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11571,35 +11571,35 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G297" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H297" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11609,35 +11609,35 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G298" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H298" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11647,7 +11647,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
@@ -11661,21 +11661,21 @@
         </is>
       </c>
       <c r="G299" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H299" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11685,7 +11685,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -11699,21 +11699,21 @@
         </is>
       </c>
       <c r="G300" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="H300" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11723,7 +11723,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11737,21 +11737,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="H301" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11761,35 +11761,35 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G302" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="H302" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11799,35 +11799,35 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G303" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H303" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11837,7 +11837,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -11851,21 +11851,21 @@
         </is>
       </c>
       <c r="G304" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H304" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11875,7 +11875,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
@@ -11889,21 +11889,21 @@
         </is>
       </c>
       <c r="G305" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="H305" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11913,7 +11913,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11927,21 +11927,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H306" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11951,7 +11951,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11965,21 +11965,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H307" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11989,35 +11989,35 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G308" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H308" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12027,35 +12027,35 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G309" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H309" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12065,7 +12065,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -12079,21 +12079,21 @@
         </is>
       </c>
       <c r="G310" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H310" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, SD, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12103,7 +12103,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -12117,21 +12117,21 @@
         </is>
       </c>
       <c r="G311" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H311" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12141,7 +12141,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
@@ -12155,21 +12155,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H312" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12179,35 +12179,35 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G313" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H313" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12217,7 +12217,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -12231,21 +12231,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H314" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12255,7 +12255,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -12269,21 +12269,21 @@
         </is>
       </c>
       <c r="G315" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="H315" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12293,35 +12293,35 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G316" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H316" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12331,35 +12331,35 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G317" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H317" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12369,35 +12369,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="H318" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12407,7 +12407,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
@@ -12421,21 +12421,21 @@
         </is>
       </c>
       <c r="G319" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="H319" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12445,7 +12445,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
@@ -12459,21 +12459,21 @@
         </is>
       </c>
       <c r="G320" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="H320" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12483,35 +12483,35 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G321" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="H321" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12521,35 +12521,35 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G322" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H322" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12559,7 +12559,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
@@ -12573,21 +12573,21 @@
         </is>
       </c>
       <c r="G323" t="n">
-        <v>41.50069</v>
+        <v>29.429461</v>
       </c>
       <c r="H323" t="n">
-        <v>-81.68411999999999</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12597,7 +12597,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
@@ -12611,21 +12611,21 @@
         </is>
       </c>
       <c r="G324" t="n">
-        <v>35.93543</v>
+        <v>41.50069</v>
       </c>
       <c r="H324" t="n">
-        <v>-78.88075000000001</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12635,7 +12635,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12649,21 +12649,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>35.46655</v>
+        <v>35.93543</v>
       </c>
       <c r="H325" t="n">
-        <v>-97.65373</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12673,7 +12673,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12687,21 +12687,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>27.9755001068</v>
+        <v>35.46655</v>
       </c>
       <c r="H326" t="n">
-        <v>-82.533203125</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12711,7 +12711,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12725,47 +12725,85 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>61.158555</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H327" t="n">
-        <v>-149.890208</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
+          <t>ANC</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Anchorage, United States</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Anchorage</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="G328" t="n">
+        <v>61.158555</v>
+      </c>
+      <c r="H328" t="n">
+        <v>-149.890208</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="inlineStr">
+        <is>
           <t>YHZ</t>
         </is>
       </c>
-      <c r="B328" t="inlineStr">
+      <c r="B329" t="inlineStr">
         <is>
           <t>Halifax, Canada</t>
         </is>
       </c>
-      <c r="C328" t="inlineStr">
+      <c r="C329" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="D328" t="inlineStr">
+      <c r="D329" t="inlineStr">
         <is>
           <t>Halifax</t>
         </is>
       </c>
-      <c r="E328" t="inlineStr">
+      <c r="E329" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="F328" t="inlineStr">
+      <c r="F329" t="inlineStr">
         <is>
           <t>CA</t>
         </is>
       </c>
-      <c r="G328" t="n">
+      <c r="G329" t="n">
         <v>44.64601</v>
       </c>
-      <c r="H328" t="n">
+      <c r="H329" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 78a23f53b071fcff8ed81825416b4d9904329eea
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H328"/>
+  <dimension ref="A1:H329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10530,50 +10530,50 @@
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>LHE</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Lahore, Pakistan</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Asia Pacific</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Lahore</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>PK</t>
         </is>
       </c>
       <c r="G270" t="n">
-        <v>38.94449997</v>
+        <v>31.5216007233</v>
       </c>
       <c r="H270" t="n">
-        <v>-77.45580292</v>
+        <v>74.4036026001</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -10583,7 +10583,7 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
@@ -10597,21 +10597,21 @@
         </is>
       </c>
       <c r="G271" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="H271" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -10621,7 +10621,7 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
@@ -10635,21 +10635,21 @@
         </is>
       </c>
       <c r="G272" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H272" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -10659,7 +10659,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -10673,21 +10673,21 @@
         </is>
       </c>
       <c r="G273" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="H273" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -10697,35 +10697,35 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G274" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="H274" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10735,35 +10735,35 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G275" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="H275" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10773,7 +10773,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -10787,21 +10787,21 @@
         </is>
       </c>
       <c r="G276" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H276" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10811,7 +10811,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -10825,21 +10825,21 @@
         </is>
       </c>
       <c r="G277" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="H277" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10849,7 +10849,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -10863,21 +10863,21 @@
         </is>
       </c>
       <c r="G278" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H278" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10887,7 +10887,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -10901,21 +10901,21 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H279" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10925,7 +10925,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10939,21 +10939,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H280" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10963,7 +10963,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10977,21 +10977,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H281" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -11001,7 +11001,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -11015,21 +11015,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H282" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11039,7 +11039,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11053,21 +11053,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H283" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11077,7 +11077,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11091,21 +11091,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="H284" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11115,7 +11115,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11129,21 +11129,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H285" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11153,7 +11153,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11167,21 +11167,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H286" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11191,7 +11191,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11205,21 +11205,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="H287" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11229,7 +11229,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11243,21 +11243,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>35.0424003601</v>
+        <v>33.94250107</v>
       </c>
       <c r="H288" t="n">
-        <v>-89.9766998291</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11267,35 +11267,35 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G289" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H289" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11305,35 +11305,35 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G290" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H290" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11343,7 +11343,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -11357,21 +11357,21 @@
         </is>
       </c>
       <c r="G291" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H291" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11381,35 +11381,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>45.4706001282</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H292" t="n">
-        <v>-73.7407989502</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11419,35 +11419,35 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G293" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H293" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11457,7 +11457,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
@@ -11471,21 +11471,21 @@
         </is>
       </c>
       <c r="G294" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H294" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11495,7 +11495,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
@@ -11509,21 +11509,21 @@
         </is>
       </c>
       <c r="G295" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H295" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11533,7 +11533,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11547,21 +11547,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H296" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11571,35 +11571,35 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G297" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H297" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11609,35 +11609,35 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G298" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H298" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11647,7 +11647,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
@@ -11661,21 +11661,21 @@
         </is>
       </c>
       <c r="G299" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H299" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11685,7 +11685,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -11699,21 +11699,21 @@
         </is>
       </c>
       <c r="G300" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="H300" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11723,7 +11723,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11737,21 +11737,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="H301" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11761,35 +11761,35 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G302" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="H302" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11799,35 +11799,35 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G303" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H303" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11837,7 +11837,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -11851,21 +11851,21 @@
         </is>
       </c>
       <c r="G304" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H304" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11875,7 +11875,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
@@ -11889,21 +11889,21 @@
         </is>
       </c>
       <c r="G305" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="H305" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11913,7 +11913,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11927,21 +11927,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H306" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11951,7 +11951,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11965,21 +11965,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H307" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11989,35 +11989,35 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G308" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H308" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12027,35 +12027,35 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G309" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H309" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12065,7 +12065,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -12079,21 +12079,21 @@
         </is>
       </c>
       <c r="G310" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H310" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, SD, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12103,7 +12103,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -12117,21 +12117,21 @@
         </is>
       </c>
       <c r="G311" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H311" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12141,7 +12141,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
@@ -12155,21 +12155,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H312" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12179,35 +12179,35 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G313" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H313" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12217,7 +12217,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -12231,21 +12231,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H314" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12255,7 +12255,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -12269,21 +12269,21 @@
         </is>
       </c>
       <c r="G315" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="H315" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12293,35 +12293,35 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G316" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H316" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12331,35 +12331,35 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G317" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H317" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12369,35 +12369,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="H318" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12407,7 +12407,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
@@ -12421,21 +12421,21 @@
         </is>
       </c>
       <c r="G319" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="H319" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12445,7 +12445,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
@@ -12459,21 +12459,21 @@
         </is>
       </c>
       <c r="G320" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="H320" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12483,35 +12483,35 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G321" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="H321" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12521,35 +12521,35 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G322" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H322" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12559,7 +12559,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
@@ -12573,21 +12573,21 @@
         </is>
       </c>
       <c r="G323" t="n">
-        <v>41.50069</v>
+        <v>29.429461</v>
       </c>
       <c r="H323" t="n">
-        <v>-81.68411999999999</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12597,7 +12597,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
@@ -12611,21 +12611,21 @@
         </is>
       </c>
       <c r="G324" t="n">
-        <v>35.93543</v>
+        <v>41.50069</v>
       </c>
       <c r="H324" t="n">
-        <v>-78.88075000000001</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12635,7 +12635,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12649,21 +12649,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>35.46655</v>
+        <v>35.93543</v>
       </c>
       <c r="H325" t="n">
-        <v>-97.65373</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12673,7 +12673,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12687,21 +12687,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>27.9755001068</v>
+        <v>35.46655</v>
       </c>
       <c r="H326" t="n">
-        <v>-82.533203125</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12711,7 +12711,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12725,47 +12725,85 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>61.158555</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H327" t="n">
-        <v>-149.890208</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
+          <t>ANC</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Anchorage, United States</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Anchorage</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="F328" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="G328" t="n">
+        <v>61.158555</v>
+      </c>
+      <c r="H328" t="n">
+        <v>-149.890208</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="inlineStr">
+        <is>
           <t>YHZ</t>
         </is>
       </c>
-      <c r="B328" t="inlineStr">
+      <c r="B329" t="inlineStr">
         <is>
           <t>Halifax, Canada</t>
         </is>
       </c>
-      <c r="C328" t="inlineStr">
+      <c r="C329" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="D328" t="inlineStr">
+      <c r="D329" t="inlineStr">
         <is>
           <t>Halifax</t>
         </is>
       </c>
-      <c r="E328" t="inlineStr">
+      <c r="E329" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="F328" t="inlineStr">
+      <c r="F329" t="inlineStr">
         <is>
           <t>CA</t>
         </is>
       </c>
-      <c r="G328" t="n">
+      <c r="G329" t="n">
         <v>44.64601</v>
       </c>
-      <c r="H328" t="n">
+      <c r="H329" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by d91ac5afbdf1cd06b27b24e82e9a544bdebe11cb
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H330"/>
+  <dimension ref="A1:H331"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10606,50 +10606,46 @@
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>CTU</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Chengdu, China</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Ashburn</t>
+          <t>Chengdu</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="G272" t="n">
-        <v>38.94449997</v>
-      </c>
-      <c r="H272" t="n">
-        <v>-77.45580292</v>
-      </c>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="G272" t="inlineStr"/>
+      <c r="H272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -10659,7 +10655,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Atlanta</t>
+          <t>Ashburn</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -10673,21 +10669,21 @@
         </is>
       </c>
       <c r="G273" t="n">
-        <v>33.6366996765</v>
+        <v>38.94449997</v>
       </c>
       <c r="H273" t="n">
-        <v>-84.4281005859</v>
+        <v>-77.45580292</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -10697,7 +10693,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Boston</t>
+          <t>Atlanta</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -10711,21 +10707,21 @@
         </is>
       </c>
       <c r="G274" t="n">
-        <v>42.36429977</v>
+        <v>33.6366996765</v>
       </c>
       <c r="H274" t="n">
-        <v>-71.00520324999999</v>
+        <v>-84.4281005859</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -10735,7 +10731,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Buffalo</t>
+          <t>Boston</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -10749,21 +10745,21 @@
         </is>
       </c>
       <c r="G275" t="n">
-        <v>42.94049835</v>
+        <v>42.36429977</v>
       </c>
       <c r="H275" t="n">
-        <v>-78.73220062</v>
+        <v>-71.00520324999999</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -10773,35 +10769,35 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Calgary</t>
+          <t>Buffalo</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G276" t="n">
-        <v>51.113899231</v>
+        <v>42.94049835</v>
       </c>
       <c r="H276" t="n">
-        <v>-114.019996643</v>
+        <v>-78.73220062</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -10811,35 +10807,35 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Charlotte</t>
+          <t>Calgary</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G277" t="n">
-        <v>35.2140007019</v>
+        <v>51.113899231</v>
       </c>
       <c r="H277" t="n">
-        <v>-80.94309997560001</v>
+        <v>-114.019996643</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -10849,7 +10845,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Chicago</t>
+          <t>Charlotte</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -10863,21 +10859,21 @@
         </is>
       </c>
       <c r="G278" t="n">
-        <v>41.97859955</v>
+        <v>35.2140007019</v>
       </c>
       <c r="H278" t="n">
-        <v>-87.90480042</v>
+        <v>-80.94309997560001</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -10887,7 +10883,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Columbus</t>
+          <t>Chicago</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -10901,21 +10897,21 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>39.9980010986</v>
+        <v>41.97859955</v>
       </c>
       <c r="H279" t="n">
-        <v>-82.89189910890001</v>
+        <v>-87.90480042</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -10925,7 +10921,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Dallas</t>
+          <t>Columbus</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -10939,21 +10935,21 @@
         </is>
       </c>
       <c r="G280" t="n">
-        <v>32.8968009949</v>
+        <v>39.9980010986</v>
       </c>
       <c r="H280" t="n">
-        <v>-97.0380020142</v>
+        <v>-82.89189910890001</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -10963,7 +10959,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Denver</t>
+          <t>Dallas</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -10977,21 +10973,21 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>39.8616981506</v>
+        <v>32.8968009949</v>
       </c>
       <c r="H281" t="n">
-        <v>-104.672996521</v>
+        <v>-97.0380020142</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -11001,7 +10997,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Detroit</t>
+          <t>Denver</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -11015,21 +11011,21 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>42.2123985291</v>
+        <v>39.8616981506</v>
       </c>
       <c r="H282" t="n">
-        <v>-83.35340118409999</v>
+        <v>-104.672996521</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -11039,7 +11035,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Honolulu</t>
+          <t>Detroit</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -11053,21 +11049,21 @@
         </is>
       </c>
       <c r="G283" t="n">
-        <v>21.3187007904</v>
+        <v>42.2123985291</v>
       </c>
       <c r="H283" t="n">
-        <v>-157.9219970703</v>
+        <v>-83.35340118409999</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -11077,7 +11073,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Houston</t>
+          <t>Honolulu</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -11091,21 +11087,21 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>29.9843997955</v>
+        <v>21.3187007904</v>
       </c>
       <c r="H284" t="n">
-        <v>-95.34140014650001</v>
+        <v>-157.9219970703</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -11115,7 +11111,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Indianapolis</t>
+          <t>Houston</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -11129,21 +11125,21 @@
         </is>
       </c>
       <c r="G285" t="n">
-        <v>39.717300415</v>
+        <v>29.9843997955</v>
       </c>
       <c r="H285" t="n">
-        <v>-86.2944030762</v>
+        <v>-95.34140014650001</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -11153,7 +11149,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Jacksonville</t>
+          <t>Indianapolis</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -11167,21 +11163,21 @@
         </is>
       </c>
       <c r="G286" t="n">
-        <v>30.4941005707</v>
+        <v>39.717300415</v>
       </c>
       <c r="H286" t="n">
-        <v>-81.68789672849999</v>
+        <v>-86.2944030762</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -11191,7 +11187,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Kansas City</t>
+          <t>Jacksonville</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -11205,21 +11201,21 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>39.2975997925</v>
+        <v>30.4941005707</v>
       </c>
       <c r="H287" t="n">
-        <v>-94.7138977051</v>
+        <v>-81.68789672849999</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -11229,7 +11225,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Las Vegas</t>
+          <t>Kansas City</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -11243,21 +11239,21 @@
         </is>
       </c>
       <c r="G288" t="n">
-        <v>36.08010101</v>
+        <v>39.2975997925</v>
       </c>
       <c r="H288" t="n">
-        <v>-115.1520004</v>
+        <v>-94.7138977051</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -11267,7 +11263,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Las Vegas</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -11281,21 +11277,21 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>33.94250107</v>
+        <v>36.08010101</v>
       </c>
       <c r="H289" t="n">
-        <v>-118.4079971</v>
+        <v>-115.1520004</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -11305,7 +11301,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Los Angeles</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -11319,21 +11315,21 @@
         </is>
       </c>
       <c r="G290" t="n">
-        <v>35.0424003601</v>
+        <v>33.94250107</v>
       </c>
       <c r="H290" t="n">
-        <v>-89.9766998291</v>
+        <v>-118.4079971</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -11343,35 +11339,35 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G291" t="n">
-        <v>19.4363002777</v>
+        <v>35.0424003601</v>
       </c>
       <c r="H291" t="n">
-        <v>-99.07209777830001</v>
+        <v>-89.9766998291</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -11381,35 +11377,35 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G292" t="n">
-        <v>25.7931995392</v>
+        <v>19.4363002777</v>
       </c>
       <c r="H292" t="n">
-        <v>-80.2906036377</v>
+        <v>-99.07209777830001</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -11419,7 +11415,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Minneapolis</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -11433,21 +11429,21 @@
         </is>
       </c>
       <c r="G293" t="n">
-        <v>44.8819999695</v>
+        <v>25.7931995392</v>
       </c>
       <c r="H293" t="n">
-        <v>-93.22180175779999</v>
+        <v>-80.2906036377</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -11457,35 +11453,35 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Montréal</t>
+          <t>Minneapolis</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G294" t="n">
-        <v>45.4706001282</v>
+        <v>44.8819999695</v>
       </c>
       <c r="H294" t="n">
-        <v>-73.7407989502</v>
+        <v>-93.22180175779999</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -11495,35 +11491,35 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>36.1245002747</v>
+        <v>45.4706001282</v>
       </c>
       <c r="H295" t="n">
-        <v>-86.6781997681</v>
+        <v>-73.7407989502</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -11533,7 +11529,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Newark</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -11547,21 +11543,21 @@
         </is>
       </c>
       <c r="G296" t="n">
-        <v>40.6925010681</v>
+        <v>36.1245002747</v>
       </c>
       <c r="H296" t="n">
-        <v>-74.1687011719</v>
+        <v>-86.6781997681</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -11571,7 +11567,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Newark</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -11585,21 +11581,21 @@
         </is>
       </c>
       <c r="G297" t="n">
-        <v>36.8945999146</v>
+        <v>40.6925010681</v>
       </c>
       <c r="H297" t="n">
-        <v>-76.2012023926</v>
+        <v>-74.1687011719</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -11609,7 +11605,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Omaha</t>
+          <t>Norfolk</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -11623,21 +11619,21 @@
         </is>
       </c>
       <c r="G298" t="n">
-        <v>41.3031997681</v>
+        <v>36.8945999146</v>
       </c>
       <c r="H298" t="n">
-        <v>-95.89409637449999</v>
+        <v>-76.2012023926</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -11647,35 +11643,35 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G299" t="n">
-        <v>45.3224983215</v>
+        <v>41.3031997681</v>
       </c>
       <c r="H299" t="n">
-        <v>-75.66919708250001</v>
+        <v>-95.89409637449999</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -11685,35 +11681,35 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G300" t="n">
-        <v>39.8718986511</v>
+        <v>45.3224983215</v>
       </c>
       <c r="H300" t="n">
-        <v>-75.24109649659999</v>
+        <v>-75.66919708250001</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -11723,7 +11719,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Phoenix</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -11737,21 +11733,21 @@
         </is>
       </c>
       <c r="G301" t="n">
-        <v>33.434299469</v>
+        <v>39.8718986511</v>
       </c>
       <c r="H301" t="n">
-        <v>-112.012001038</v>
+        <v>-75.24109649659999</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -11761,7 +11757,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Phoenix</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -11775,21 +11771,21 @@
         </is>
       </c>
       <c r="G302" t="n">
-        <v>40.49150085</v>
+        <v>33.434299469</v>
       </c>
       <c r="H302" t="n">
-        <v>-80.23290253</v>
+        <v>-112.012001038</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -11799,7 +11795,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Portland</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -11813,21 +11809,21 @@
         </is>
       </c>
       <c r="G303" t="n">
-        <v>45.58869934</v>
+        <v>40.49150085</v>
       </c>
       <c r="H303" t="n">
-        <v>-122.5979996</v>
+        <v>-80.23290253</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -11837,35 +11833,35 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Queretaro</t>
+          <t>Portland</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G304" t="n">
-        <v>20.6173000336</v>
+        <v>45.58869934</v>
       </c>
       <c r="H304" t="n">
-        <v>-100.185997009</v>
+        <v>-122.5979996</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -11875,35 +11871,35 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Richmond</t>
+          <t>Queretaro</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>37.5051994324</v>
+        <v>20.6173000336</v>
       </c>
       <c r="H305" t="n">
-        <v>-77.3197021484</v>
+        <v>-100.185997009</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -11913,7 +11909,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Sacramento</t>
+          <t>Richmond</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11927,21 +11923,21 @@
         </is>
       </c>
       <c r="G306" t="n">
-        <v>38.695400238</v>
+        <v>37.5051994324</v>
       </c>
       <c r="H306" t="n">
-        <v>-121.591003418</v>
+        <v>-77.3197021484</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -11951,7 +11947,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Salt Lake City</t>
+          <t>Sacramento</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11965,21 +11961,21 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>40.7883987427</v>
+        <v>38.695400238</v>
       </c>
       <c r="H307" t="n">
-        <v>-111.977996826</v>
+        <v>-121.591003418</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -11989,7 +11985,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>San Diego</t>
+          <t>Salt Lake City</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -12003,21 +11999,21 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>32.7336006165</v>
+        <v>40.7883987427</v>
       </c>
       <c r="H308" t="n">
-        <v>-117.190002441</v>
+        <v>-111.977996826</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -12027,7 +12023,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>San Jose</t>
+          <t>San Diego</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -12041,21 +12037,21 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>37.3625984192</v>
+        <v>32.7336006165</v>
       </c>
       <c r="H309" t="n">
-        <v>-121.929000855</v>
+        <v>-117.190002441</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -12065,35 +12061,35 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Saskatoon</t>
+          <t>San Jose</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G310" t="n">
-        <v>52.1707992554</v>
+        <v>37.3625984192</v>
       </c>
       <c r="H310" t="n">
-        <v>-106.699996948</v>
+        <v>-121.929000855</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -12103,35 +12099,35 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Seattle</t>
+          <t>Saskatoon</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G311" t="n">
-        <v>47.4490013123</v>
+        <v>52.1707992554</v>
       </c>
       <c r="H311" t="n">
-        <v>-122.308998108</v>
+        <v>-106.699996948</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -12141,7 +12137,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Sioux Falls</t>
+          <t>Seattle</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
@@ -12155,21 +12151,21 @@
         </is>
       </c>
       <c r="G312" t="n">
-        <v>43.540819819502</v>
+        <v>47.4490013123</v>
       </c>
       <c r="H312" t="n">
-        <v>-96.65511577730963</v>
+        <v>-122.308998108</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, SD, United States</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -12179,7 +12175,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>St. Louis</t>
+          <t>Sioux Falls</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
@@ -12193,21 +12189,21 @@
         </is>
       </c>
       <c r="G313" t="n">
-        <v>38.7486991882</v>
+        <v>43.540819819502</v>
       </c>
       <c r="H313" t="n">
-        <v>-90.37000274659999</v>
+        <v>-96.65511577730963</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -12217,7 +12213,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Tallahassee</t>
+          <t>St. Louis</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -12231,21 +12227,21 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>30.3964996338</v>
+        <v>38.7486991882</v>
       </c>
       <c r="H314" t="n">
-        <v>-84.3503036499</v>
+        <v>-90.37000274659999</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -12255,35 +12251,35 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Toronto</t>
+          <t>Tallahassee</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G315" t="n">
-        <v>43.6772003174</v>
+        <v>30.3964996338</v>
       </c>
       <c r="H315" t="n">
-        <v>-79.63059997560001</v>
+        <v>-84.3503036499</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -12293,7 +12289,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Vancouver</t>
+          <t>Toronto</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -12307,21 +12303,21 @@
         </is>
       </c>
       <c r="G316" t="n">
-        <v>49.193901062</v>
+        <v>43.6772003174</v>
       </c>
       <c r="H316" t="n">
-        <v>-123.183998108</v>
+        <v>-79.63059997560001</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -12331,7 +12327,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Winnipeg</t>
+          <t>Vancouver</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -12345,21 +12341,21 @@
         </is>
       </c>
       <c r="G317" t="n">
-        <v>49.9099998474</v>
+        <v>49.193901062</v>
       </c>
       <c r="H317" t="n">
-        <v>-97.2398986816</v>
+        <v>-123.183998108</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -12369,35 +12365,35 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="G318" t="n">
-        <v>37.6189994812</v>
+        <v>49.9099998474</v>
       </c>
       <c r="H318" t="n">
-        <v>-122.375</v>
+        <v>-97.2398986816</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -12407,35 +12403,35 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G319" t="n">
-        <v>17.9951</v>
+        <v>37.6189994812</v>
       </c>
       <c r="H319" t="n">
-        <v>-76.7846</v>
+        <v>-122.375</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -12445,35 +12441,35 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
       <c r="G320" t="n">
-        <v>44.8081</v>
+        <v>17.9951</v>
       </c>
       <c r="H320" t="n">
-        <v>-68.795</v>
+        <v>-76.7846</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -12483,7 +12479,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -12497,21 +12493,21 @@
         </is>
       </c>
       <c r="G321" t="n">
-        <v>30.1975</v>
+        <v>44.8081</v>
       </c>
       <c r="H321" t="n">
-        <v>-97.6664</v>
+        <v>-68.795</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -12521,7 +12517,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -12535,21 +12531,21 @@
         </is>
       </c>
       <c r="G322" t="n">
-        <v>35.0844</v>
+        <v>30.1975</v>
       </c>
       <c r="H322" t="n">
-        <v>-106.6504</v>
+        <v>-97.6664</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -12559,35 +12555,35 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
       <c r="G323" t="n">
-        <v>20.5217990875</v>
+        <v>35.0844</v>
       </c>
       <c r="H323" t="n">
-        <v>-103.3109970093</v>
+        <v>-106.6504</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -12597,35 +12593,35 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
       <c r="G324" t="n">
-        <v>29.429461</v>
+        <v>20.5217990875</v>
       </c>
       <c r="H324" t="n">
-        <v>-98.487061</v>
+        <v>-103.3109970093</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -12635,7 +12631,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -12649,21 +12645,21 @@
         </is>
       </c>
       <c r="G325" t="n">
-        <v>41.50069</v>
+        <v>29.429461</v>
       </c>
       <c r="H325" t="n">
-        <v>-81.68411999999999</v>
+        <v>-98.487061</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -12673,7 +12669,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12687,21 +12683,21 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>35.93543</v>
+        <v>41.50069</v>
       </c>
       <c r="H326" t="n">
-        <v>-78.88075000000001</v>
+        <v>-81.68411999999999</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -12711,7 +12707,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -12725,21 +12721,21 @@
         </is>
       </c>
       <c r="G327" t="n">
-        <v>35.46655</v>
+        <v>35.93543</v>
       </c>
       <c r="H327" t="n">
-        <v>-97.65373</v>
+        <v>-78.88075000000001</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -12749,7 +12745,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -12763,21 +12759,21 @@
         </is>
       </c>
       <c r="G328" t="n">
-        <v>27.9755001068</v>
+        <v>35.46655</v>
       </c>
       <c r="H328" t="n">
-        <v>-82.533203125</v>
+        <v>-97.65373</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -12787,7 +12783,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -12801,47 +12797,85 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>61.158555</v>
+        <v>27.9755001068</v>
       </c>
       <c r="H329" t="n">
-        <v>-149.890208</v>
+        <v>-82.533203125</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
+          <t>ANC</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Anchorage, United States</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Anchorage</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="F330" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="G330" t="n">
+        <v>61.158555</v>
+      </c>
+      <c r="H330" t="n">
+        <v>-149.890208</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="inlineStr">
+        <is>
           <t>YHZ</t>
         </is>
       </c>
-      <c r="B330" t="inlineStr">
+      <c r="B331" t="inlineStr">
         <is>
           <t>Halifax, Canada</t>
         </is>
       </c>
-      <c r="C330" t="inlineStr">
+      <c r="C331" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="D330" t="inlineStr">
+      <c r="D331" t="inlineStr">
         <is>
           <t>Halifax</t>
         </is>
       </c>
-      <c r="E330" t="inlineStr">
+      <c r="E331" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="F330" t="inlineStr">
+      <c r="F331" t="inlineStr">
         <is>
           <t>CA</t>
         </is>
       </c>
-      <c r="G330" t="n">
+      <c r="G331" t="n">
         <v>44.64601</v>
       </c>
-      <c r="H330" t="n">
+      <c r="H331" t="n">
         <v>-63.66844</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update generated data Triggered by 7ec6fcf438bc6acf4ce83a504dcb55334eb82eba
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F332"/>
+  <dimension ref="A1:F333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9100,44 +9100,44 @@
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>AGR</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Agra, India</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Ashburn, VA</t>
+          <t>Agra</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IN</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -9147,7 +9147,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Atlanta, GA</t>
+          <t>Ashburn, VA</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -9164,12 +9164,12 @@
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -9179,7 +9179,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Boston, MA</t>
+          <t>Atlanta, GA</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -9196,12 +9196,12 @@
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -9211,7 +9211,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Buffalo, NY</t>
+          <t>Boston, MA</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -9228,12 +9228,12 @@
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -9243,29 +9243,29 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Calgary, AB</t>
+          <t>Buffalo, NY</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -9275,29 +9275,29 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Charlotte, NC</t>
+          <t>Calgary, AB</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -9307,7 +9307,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Chicago, IL</t>
+          <t>Charlotte, NC</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -9324,12 +9324,12 @@
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -9339,7 +9339,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Columbus, OH</t>
+          <t>Chicago, IL</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -9356,12 +9356,12 @@
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -9371,7 +9371,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Dallas, TX</t>
+          <t>Columbus, OH</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -9388,12 +9388,12 @@
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -9403,7 +9403,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Denver, CO</t>
+          <t>Dallas, TX</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -9420,12 +9420,12 @@
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -9435,7 +9435,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Detroit, MI</t>
+          <t>Denver, CO</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -9452,12 +9452,12 @@
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -9467,7 +9467,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Honolulu, HI</t>
+          <t>Detroit, MI</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -9484,12 +9484,12 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -9499,7 +9499,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Houston, TX</t>
+          <t>Honolulu, HI</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -9516,12 +9516,12 @@
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -9531,7 +9531,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Indianapolis, IN</t>
+          <t>Houston, TX</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -9548,12 +9548,12 @@
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Jacksonville, FL</t>
+          <t>Indianapolis, IN</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -9580,12 +9580,12 @@
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -9595,7 +9595,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Kansas City, MO</t>
+          <t>Jacksonville, FL</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -9612,12 +9612,12 @@
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -9627,7 +9627,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Las Vegas, NV</t>
+          <t>Kansas City, MO</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -9644,12 +9644,12 @@
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -9659,7 +9659,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Los Angeles, CA</t>
+          <t>Las Vegas, NV</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -9676,12 +9676,12 @@
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -9691,7 +9691,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Memphis, TN</t>
+          <t>Los Angeles, CA</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
@@ -9708,12 +9708,12 @@
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -9723,29 +9723,29 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis, TN</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -9755,29 +9755,29 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Miami, FL</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -9787,7 +9787,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Minneapolis, MN</t>
+          <t>Miami, FL</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
@@ -9804,12 +9804,12 @@
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -9819,29 +9819,29 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Montréal, QC</t>
+          <t>Minneapolis, MN</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -9851,29 +9851,29 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal, QC</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -9883,7 +9883,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Newark, NJ</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -9900,12 +9900,12 @@
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -9915,7 +9915,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Norfolk, VA</t>
+          <t>Newark, NJ</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
@@ -9932,12 +9932,12 @@
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -9947,7 +9947,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Omaha, NE</t>
+          <t>Norfolk, VA</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -9964,12 +9964,12 @@
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -9979,29 +9979,29 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha, NE</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -10011,29 +10011,29 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -10043,7 +10043,7 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Phoenix, AZ</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -10060,12 +10060,12 @@
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -10075,7 +10075,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA</t>
+          <t>Phoenix, AZ</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -10092,12 +10092,12 @@
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -10107,7 +10107,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Portland, OR</t>
+          <t>Pittsburgh, PA</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
@@ -10124,12 +10124,12 @@
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -10139,29 +10139,29 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Queretaro, MX</t>
+          <t>Portland, OR</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -10171,29 +10171,29 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Richmond, VA</t>
+          <t>Queretaro, MX</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -10203,7 +10203,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Sacramento, CA</t>
+          <t>Richmond, VA</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -10220,12 +10220,12 @@
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -10235,7 +10235,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT</t>
+          <t>Sacramento, CA</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -10252,12 +10252,12 @@
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -10267,7 +10267,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>San Diego, CA</t>
+          <t>Salt Lake City, UT</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -10284,12 +10284,12 @@
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -10299,7 +10299,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>San Jose, CA</t>
+          <t>San Diego, CA</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -10316,12 +10316,12 @@
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -10331,29 +10331,29 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Saskatoon, SK</t>
+          <t>San Jose, CA</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -10363,29 +10363,29 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Seattle, WA</t>
+          <t>Saskatoon, SK</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -10395,7 +10395,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD</t>
+          <t>Seattle, WA</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -10412,12 +10412,12 @@
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, SD, United States</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -10427,7 +10427,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>St. Louis, MO</t>
+          <t>Sioux Falls, SD</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -10444,12 +10444,12 @@
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -10459,7 +10459,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Tallahassee, FL</t>
+          <t>St. Louis, MO</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -10476,12 +10476,12 @@
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -10491,29 +10491,29 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Toronto, ON</t>
+          <t>Tallahassee, FL</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -10523,7 +10523,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Vancouver, BC</t>
+          <t>Toronto, ON</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
@@ -10540,12 +10540,12 @@
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -10555,7 +10555,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Winnipeg, MB</t>
+          <t>Vancouver, BC</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
@@ -10572,12 +10572,12 @@
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -10587,29 +10587,29 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg, MB</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -10619,29 +10619,29 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -10651,29 +10651,29 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -10683,7 +10683,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
@@ -10700,12 +10700,12 @@
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -10715,7 +10715,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
@@ -10732,12 +10732,12 @@
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -10747,29 +10747,29 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -10779,29 +10779,29 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -10811,7 +10811,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -10828,12 +10828,12 @@
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -10843,7 +10843,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -10860,12 +10860,12 @@
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -10875,7 +10875,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -10892,12 +10892,12 @@
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -10907,7 +10907,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -10924,12 +10924,12 @@
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -10939,7 +10939,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
@@ -10956,30 +10956,62 @@
     <row r="332">
       <c r="A332" s="1" t="inlineStr">
         <is>
+          <t>ANC</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Anchorage, United States</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Anchorage</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="F332" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="1" t="inlineStr">
+        <is>
           <t>YHZ</t>
         </is>
       </c>
-      <c r="B332" t="inlineStr">
+      <c r="B333" t="inlineStr">
         <is>
           <t>Halifax, Canada</t>
         </is>
       </c>
-      <c r="C332" t="inlineStr">
+      <c r="C333" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="D332" t="inlineStr">
+      <c r="D333" t="inlineStr">
         <is>
           <t>Halifax</t>
         </is>
       </c>
-      <c r="E332" t="inlineStr">
+      <c r="E333" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="F332" t="inlineStr">
+      <c r="F333" t="inlineStr">
         <is>
           <t>CA</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 09f794622ce1a391e92677d17f9f7c60e4f8a477
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F333"/>
+  <dimension ref="A1:F334"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9132,44 +9132,44 @@
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>CJB</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Coimbatore, India</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Asia</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Ashburn, VA</t>
+          <t>Coimbatore</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>IN</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -9179,7 +9179,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Atlanta, GA</t>
+          <t>Ashburn, VA</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -9196,12 +9196,12 @@
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -9211,7 +9211,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Boston, MA</t>
+          <t>Atlanta, GA</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -9228,12 +9228,12 @@
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -9243,7 +9243,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Buffalo, NY</t>
+          <t>Boston, MA</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -9260,12 +9260,12 @@
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -9275,29 +9275,29 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Calgary, AB</t>
+          <t>Buffalo, NY</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -9307,29 +9307,29 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Charlotte, NC</t>
+          <t>Calgary, AB</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -9339,7 +9339,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Chicago, IL</t>
+          <t>Charlotte, NC</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -9356,12 +9356,12 @@
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -9371,7 +9371,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Columbus, OH</t>
+          <t>Chicago, IL</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -9388,12 +9388,12 @@
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -9403,7 +9403,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Dallas, TX</t>
+          <t>Columbus, OH</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -9420,12 +9420,12 @@
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -9435,7 +9435,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Denver, CO</t>
+          <t>Dallas, TX</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -9452,12 +9452,12 @@
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -9467,7 +9467,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Detroit, MI</t>
+          <t>Denver, CO</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -9484,12 +9484,12 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -9499,7 +9499,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Honolulu, HI</t>
+          <t>Detroit, MI</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -9516,12 +9516,12 @@
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -9531,7 +9531,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Houston, TX</t>
+          <t>Honolulu, HI</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -9548,12 +9548,12 @@
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Indianapolis, IN</t>
+          <t>Houston, TX</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -9580,12 +9580,12 @@
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -9595,7 +9595,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Jacksonville, FL</t>
+          <t>Indianapolis, IN</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -9612,12 +9612,12 @@
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -9627,7 +9627,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Kansas City, MO</t>
+          <t>Jacksonville, FL</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -9644,12 +9644,12 @@
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -9659,7 +9659,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Las Vegas, NV</t>
+          <t>Kansas City, MO</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -9676,12 +9676,12 @@
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -9691,7 +9691,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Los Angeles, CA</t>
+          <t>Las Vegas, NV</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
@@ -9708,12 +9708,12 @@
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -9723,7 +9723,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Memphis, TN</t>
+          <t>Los Angeles, CA</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -9740,12 +9740,12 @@
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -9755,29 +9755,29 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Memphis, TN</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -9787,29 +9787,29 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Miami, FL</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -9819,7 +9819,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Minneapolis, MN</t>
+          <t>Miami, FL</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -9836,12 +9836,12 @@
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -9851,29 +9851,29 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Montréal, QC</t>
+          <t>Minneapolis, MN</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -9883,29 +9883,29 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Montréal, QC</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -9915,7 +9915,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Newark, NJ</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
@@ -9932,12 +9932,12 @@
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -9947,7 +9947,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Norfolk, VA</t>
+          <t>Newark, NJ</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -9964,12 +9964,12 @@
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -9979,7 +9979,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Omaha, NE</t>
+          <t>Norfolk, VA</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -9996,12 +9996,12 @@
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -10011,29 +10011,29 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Omaha, NE</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -10043,29 +10043,29 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -10075,7 +10075,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Phoenix, AZ</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -10092,12 +10092,12 @@
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -10107,7 +10107,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA</t>
+          <t>Phoenix, AZ</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
@@ -10124,12 +10124,12 @@
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -10139,7 +10139,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Portland, OR</t>
+          <t>Pittsburgh, PA</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -10156,12 +10156,12 @@
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -10171,29 +10171,29 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Queretaro, MX</t>
+          <t>Portland, OR</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -10203,29 +10203,29 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Richmond, VA</t>
+          <t>Queretaro, MX</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -10235,7 +10235,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Sacramento, CA</t>
+          <t>Richmond, VA</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -10252,12 +10252,12 @@
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -10267,7 +10267,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT</t>
+          <t>Sacramento, CA</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -10284,12 +10284,12 @@
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -10299,7 +10299,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>San Diego, CA</t>
+          <t>Salt Lake City, UT</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -10316,12 +10316,12 @@
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -10331,7 +10331,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>San Jose, CA</t>
+          <t>San Diego, CA</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
@@ -10348,12 +10348,12 @@
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -10363,29 +10363,29 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Saskatoon, SK</t>
+          <t>San Jose, CA</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -10395,29 +10395,29 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Seattle, WA</t>
+          <t>Saskatoon, SK</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD, United States</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -10427,7 +10427,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD</t>
+          <t>Seattle, WA</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -10444,12 +10444,12 @@
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Sioux Falls, SD, United States</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -10459,7 +10459,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>St. Louis, MO</t>
+          <t>Sioux Falls, SD</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -10476,12 +10476,12 @@
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -10491,7 +10491,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Tallahassee, FL</t>
+          <t>St. Louis, MO</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -10508,12 +10508,12 @@
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -10523,29 +10523,29 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Toronto, ON</t>
+          <t>Tallahassee, FL</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -10555,7 +10555,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Vancouver, BC</t>
+          <t>Toronto, ON</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
@@ -10572,12 +10572,12 @@
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -10587,7 +10587,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Winnipeg, MB</t>
+          <t>Vancouver, BC</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
@@ -10604,12 +10604,12 @@
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -10619,29 +10619,29 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>Winnipeg, MB</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Francisco, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -10651,29 +10651,29 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Francisco</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -10683,29 +10683,29 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>Bangor, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -10715,7 +10715,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>Bangor</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
@@ -10732,12 +10732,12 @@
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Austin, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -10747,7 +10747,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Austin</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -10764,12 +10764,12 @@
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Albuquerque, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -10779,29 +10779,29 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Albuquerque</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -10811,29 +10811,29 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>San Antonio, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -10843,7 +10843,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>San Antonio</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -10860,12 +10860,12 @@
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Cleveland, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -10875,7 +10875,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Cleveland</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -10892,12 +10892,12 @@
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Durham, United States</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -10907,7 +10907,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Durham</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -10924,12 +10924,12 @@
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Oklahoma City, United States</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -10939,7 +10939,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Oklahoma City</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
@@ -10956,12 +10956,12 @@
     <row r="332">
       <c r="A332" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Tampa, United States</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -10971,7 +10971,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Tampa</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
@@ -10988,30 +10988,62 @@
     <row r="333">
       <c r="A333" s="1" t="inlineStr">
         <is>
+          <t>ANC</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Anchorage, United States</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>North America</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>Anchorage</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="F333" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="1" t="inlineStr">
+        <is>
           <t>YHZ</t>
         </is>
       </c>
-      <c r="B333" t="inlineStr">
+      <c r="B334" t="inlineStr">
         <is>
           <t>Halifax, Canada</t>
         </is>
       </c>
-      <c r="C333" t="inlineStr">
+      <c r="C334" t="inlineStr">
         <is>
           <t>North America</t>
         </is>
       </c>
-      <c r="D333" t="inlineStr">
+      <c r="D334" t="inlineStr">
         <is>
           <t>Halifax</t>
         </is>
       </c>
-      <c r="E333" t="inlineStr">
+      <c r="E334" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="F333" t="inlineStr">
+      <c r="F334" t="inlineStr">
         <is>
           <t>CA</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by db2dc48af8cf7d3ae7d68d09a11d380b54650c2f
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -628,12 +628,12 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>BTS</t>
+          <t>BOD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Bratislava, Slovakia</t>
+          <t>Bordeaux, France</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -643,29 +643,29 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Bratislava</t>
+          <t>Bordeaux</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>FR</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>BRU</t>
+          <t>BTS</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Brussels, Belgium</t>
+          <t>Bratislava, Slovakia</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -675,29 +675,29 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Brussels</t>
+          <t>Bratislava</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>BE</t>
+          <t>SK</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>OTP</t>
+          <t>BRU</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bucharest, Romania</t>
+          <t>Brussels, Belgium</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -707,29 +707,29 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Bucharest</t>
+          <t>Brussels</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Romania</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>BE</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>BUD</t>
+          <t>OTP</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Budapest, Hungary</t>
+          <t>Bucharest, Romania</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -739,29 +739,29 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Budapest</t>
+          <t>Bucharest</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Romania</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>HU</t>
+          <t>RO</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>KIV</t>
+          <t>BUD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Chișinău, Moldova</t>
+          <t>Budapest, Hungary</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -771,29 +771,29 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Chișinău</t>
+          <t>Budapest</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Moldova</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>MD</t>
+          <t>HU</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>CPH</t>
+          <t>KIV</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Copenhagen, Denmark</t>
+          <t>Chișinău, Moldova</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -803,29 +803,29 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Copenhagen</t>
+          <t>Chișinău</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Moldova</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>DK</t>
+          <t>MD</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>DUB</t>
+          <t>CPH</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Dublin, Ireland</t>
+          <t>Copenhagen, Denmark</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -835,29 +835,29 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Dublin</t>
+          <t>Copenhagen</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>DK</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>DUS</t>
+          <t>DUB</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Düsseldorf, Germany</t>
+          <t>Dublin, Ireland</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -867,29 +867,29 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Düsseldorf</t>
+          <t>Dublin</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>IE</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>FRA</t>
+          <t>DUS</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Frankfurt, Germany</t>
+          <t>Düsseldorf, Germany</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Frankfurt</t>
+          <t>Düsseldorf</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -916,12 +916,12 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>GVA</t>
+          <t>FRA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Geneva, Switzerland</t>
+          <t>Frankfurt, Germany</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -931,29 +931,29 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Geneva</t>
+          <t>Frankfurt</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>DE</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>GOT</t>
+          <t>GVA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Gothenburg, Sweden</t>
+          <t>Geneva, Switzerland</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -963,29 +963,29 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Gothenburg</t>
+          <t>Geneva</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>CH</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>HAM</t>
+          <t>GOT</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Hamburg, Germany</t>
+          <t>Gothenburg, Sweden</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -995,29 +995,29 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Hamburg</t>
+          <t>Gothenburg</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>SE</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>HEL</t>
+          <t>HAM</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Helsinki, Finland</t>
+          <t>Hamburg, Germany</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1027,29 +1027,29 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Helsinki</t>
+          <t>Hamburg</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>FI</t>
+          <t>DE</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>IST</t>
+          <t>HEL</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Istanbul, Turkey</t>
+          <t>Helsinki, Finland</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1059,29 +1059,29 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Istanbul</t>
+          <t>Helsinki</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>TR</t>
+          <t>FI</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>ADB</t>
+          <t>IST</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Izmir, Turkey</t>
+          <t>Istanbul, Turkey</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Izmir</t>
+          <t>Istanbul</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1108,12 +1108,12 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>KBP</t>
+          <t>ADB</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Kyiv, Ukraine</t>
+          <t>Izmir, Turkey</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1123,29 +1123,29 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Kyiv</t>
+          <t>Izmir</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>UA</t>
+          <t>TR</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>LIS</t>
+          <t>KBP</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Lisbon, Portugal</t>
+          <t>Kyiv, Ukraine</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1155,29 +1155,29 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Lisbon</t>
+          <t>Kyiv</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>UA</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>LHR</t>
+          <t>LIS</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>London, United Kingdom</t>
+          <t>Lisbon, Portugal</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1187,29 +1187,29 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>Lisbon</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>PT</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>LUX</t>
+          <t>LHR</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Luxembourg City, Luxembourg</t>
+          <t>London, United Kingdom</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1219,29 +1219,29 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Luxembourg City</t>
+          <t>London</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Luxembourg</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>LU</t>
+          <t>GB</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>MAD</t>
+          <t>LUX</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Madrid, Spain</t>
+          <t>Luxembourg City, Luxembourg</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1251,29 +1251,29 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Luxembourg City</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Luxembourg</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>LU</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>MAN</t>
+          <t>LYS</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Manchester, United Kingdom</t>
+          <t>Lyon, France</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1283,29 +1283,29 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Manchester</t>
+          <t>Lyon</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>FR</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>MRS</t>
+          <t>MAD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Marseille, France</t>
+          <t>Madrid, Spain</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1315,29 +1315,29 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Marseille</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>ES</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>MXP</t>
+          <t>MAN</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Milan, Italy</t>
+          <t>Manchester, United Kingdom</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1347,29 +1347,29 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Milan</t>
+          <t>Manchester</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>GB</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>MSQ</t>
+          <t>MRS</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Minsk, Belarus</t>
+          <t>Marseille, France</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1379,29 +1379,29 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Minsk</t>
+          <t>Marseille</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Belarus</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>BY</t>
+          <t>FR</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>DME</t>
+          <t>MXP</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Moscow, Russia</t>
+          <t>Milan, Italy</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1411,29 +1411,29 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Moscow</t>
+          <t>Milan</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>IT</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>MUC</t>
+          <t>MSQ</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Munich, Germany</t>
+          <t>Minsk, Belarus</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1443,29 +1443,29 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Munich</t>
+          <t>Minsk</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Belarus</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>BY</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>LCA</t>
+          <t>DME</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Nicosia, Cyprus</t>
+          <t>Moscow, Russia</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1475,29 +1475,29 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Nicosia</t>
+          <t>Moscow</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Russia</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>CY</t>
+          <t>RU</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>OSL</t>
+          <t>MUC</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Oslo, Norway</t>
+          <t>Munich, Germany</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1507,29 +1507,29 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Oslo</t>
+          <t>Munich</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>DE</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>PMO</t>
+          <t>LCA</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Palermo, Italy</t>
+          <t>Nicosia, Cyprus</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1539,29 +1539,29 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Nicosia</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>CY</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>CDG</t>
+          <t>OSL</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Paris, France</t>
+          <t>Oslo, Norway</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1571,29 +1571,29 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>Oslo</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>PRG</t>
+          <t>PMO</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Prague, Czech Republic</t>
+          <t>Palermo, Italy</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1603,25 +1603,29 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Prague</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr"/>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>KEF</t>
+          <t>CDG</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Reykjavík, Iceland</t>
+          <t>Paris, France</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1631,29 +1635,29 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Reykjavík</t>
+          <t>Paris</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>IS</t>
+          <t>FR</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>RIX</t>
+          <t>PRG</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Riga, Latvia</t>
+          <t>Prague, Czech Republic</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1663,29 +1667,25 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Riga</t>
+          <t>Prague</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Latvia</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>LV</t>
-        </is>
-      </c>
+          <t>Czech Republic</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>FCO</t>
+          <t>KEF</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Rome, Italy</t>
+          <t>Reykjavík, Iceland</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1695,29 +1695,29 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Rome</t>
+          <t>Reykjavík</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>IS</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>LED</t>
+          <t>RIX</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Saint Petersburg, Russia</t>
+          <t>Riga, Latvia</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1727,29 +1727,29 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Saint Petersburg</t>
+          <t>Riga</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>Latvia</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>LV</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>SOF</t>
+          <t>FCO</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Sofia, Bulgaria</t>
+          <t>Rome, Italy</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1759,29 +1759,29 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Sofia</t>
+          <t>Rome</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>BG</t>
+          <t>IT</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>ARN</t>
+          <t>LED</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Stockholm, Sweden</t>
+          <t>Saint Petersburg, Russia</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1791,29 +1791,29 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Stockholm</t>
+          <t>Saint Petersburg</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Russia</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>RU</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>STR</t>
+          <t>MLA</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Stuttgart, Germany</t>
+          <t>Santa Venera, Malta</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1823,29 +1823,29 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Santa Venera</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Malta</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>MT</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>TLL</t>
+          <t>SKP</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Tallinn, Estonia</t>
+          <t>Skopje, North Macedonia</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1855,29 +1855,29 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Tallinn</t>
+          <t>Skopje</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Estonia</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>EE</t>
+          <t>MK</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>TBS</t>
+          <t>SOF</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Tbilisi, Georgia</t>
+          <t>Sofia, Bulgaria</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1887,29 +1887,29 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Tbilisi</t>
+          <t>Sofia</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>BG</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>SKG</t>
+          <t>ARN</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Thessaloniki, Greece</t>
+          <t>Stockholm, Sweden</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1919,29 +1919,29 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Thessaloniki</t>
+          <t>Stockholm</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>GR</t>
+          <t>SE</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>TIA</t>
+          <t>STR</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Tirana, Albania</t>
+          <t>Stuttgart, Germany</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1951,29 +1951,29 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Tirana</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Albania</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>DE</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>VIE</t>
+          <t>TLL</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Vienna, Austria</t>
+          <t>Tallinn, Estonia</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1983,29 +1983,29 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Vienna</t>
+          <t>Tallinn</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Estonia</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>EE</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>VNO</t>
+          <t>TBS</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Vilnius, Lithuania</t>
+          <t>Tbilisi, Georgia</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2015,29 +2015,29 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Vilnius</t>
+          <t>Tbilisi</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>LT</t>
+          <t>GE</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>WAW</t>
+          <t>SKG</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Warsaw, Poland</t>
+          <t>Thessaloniki, Greece</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2047,29 +2047,29 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Warsaw</t>
+          <t>Thessaloniki</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>PL</t>
+          <t>GR</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>ZAG</t>
+          <t>TIA</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Zagreb, Croatia</t>
+          <t>Tirana, Albania</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2079,29 +2079,29 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Zagreb</t>
+          <t>Tirana</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Albania</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>AL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>LYS</t>
+          <t>VIE</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Lyon, France</t>
+          <t>Vienna, Austria</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2111,29 +2111,29 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Lyon</t>
+          <t>Vienna</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>AT</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>BOD</t>
+          <t>VNO</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Bordeaux, France</t>
+          <t>Vilnius, Lithuania</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2143,29 +2143,29 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Bordeaux</t>
+          <t>Vilnius</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Lithuania</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>LT</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>SKP</t>
+          <t>WAW</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Skopje, North Macedonia</t>
+          <t>Warsaw, Poland</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2175,29 +2175,29 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Skopje</t>
+          <t>Warsaw</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>MK</t>
+          <t>PL</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>ZRH</t>
+          <t>WRO</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Zurich, Switzerland</t>
+          <t>Wroclaw, Poland</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2207,29 +2207,29 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Zurich</t>
+          <t>Wroclaw</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>PL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>WRO</t>
+          <t>ZAG</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Wroclaw, Poland</t>
+          <t>Zagreb, Croatia</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2239,29 +2239,29 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Wroclaw</t>
+          <t>Zagreb</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>PL</t>
+          <t>HR</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>MLA</t>
+          <t>ZRH</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Santa Venera, Malta</t>
+          <t>Zurich, Switzerland</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2271,17 +2271,17 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Santa Venera</t>
+          <t>Zurich</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Malta</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>CH</t>
         </is>
       </c>
     </row>
@@ -9164,12 +9164,12 @@
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Albuquerque, NM, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -9179,7 +9179,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Ashburn, VA</t>
+          <t>Albuquerque, NM</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -9196,12 +9196,12 @@
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Anchorage, AK, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -9211,7 +9211,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Atlanta, GA</t>
+          <t>Anchorage, AK</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -9228,12 +9228,12 @@
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -9243,7 +9243,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Boston, MA</t>
+          <t>Ashburn, VA</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -9260,12 +9260,12 @@
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -9275,7 +9275,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Buffalo, NY</t>
+          <t>Atlanta, GA</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -9292,12 +9292,12 @@
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Austin, TX, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -9307,29 +9307,29 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Calgary, AB</t>
+          <t>Austin, TX</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Bangor, ME, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -9339,7 +9339,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Charlotte, NC</t>
+          <t>Bangor, ME</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -9356,12 +9356,12 @@
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -9371,7 +9371,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Chicago, IL</t>
+          <t>Boston, MA</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -9388,12 +9388,12 @@
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -9403,7 +9403,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Columbus, OH</t>
+          <t>Buffalo, NY</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -9420,12 +9420,12 @@
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -9435,29 +9435,29 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Dallas, TX</t>
+          <t>Calgary, AB</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -9467,7 +9467,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Denver, CO</t>
+          <t>Charlotte, NC</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -9484,12 +9484,12 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -9499,7 +9499,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Detroit, MI</t>
+          <t>Chicago, IL</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -9516,12 +9516,12 @@
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Cleveland, OH, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -9531,7 +9531,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Honolulu, HI</t>
+          <t>Cleveland, OH</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -9548,12 +9548,12 @@
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Houston, TX</t>
+          <t>Columbus, OH</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -9580,12 +9580,12 @@
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -9595,7 +9595,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Indianapolis, IN</t>
+          <t>Dallas, TX</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -9612,12 +9612,12 @@
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -9627,7 +9627,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Jacksonville, FL</t>
+          <t>Denver, CO</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -9644,12 +9644,12 @@
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -9659,7 +9659,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Kansas City, MO</t>
+          <t>Detroit, MI</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -9676,12 +9676,12 @@
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Durham, NC, United States</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -9691,7 +9691,7 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Las Vegas, NV</t>
+          <t>Durham, NC</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
@@ -9708,12 +9708,12 @@
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -9723,29 +9723,29 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Los Angeles, CA</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -9755,29 +9755,29 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Memphis, TN</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -9787,29 +9787,29 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Honolulu, HI</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -9819,7 +9819,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Miami, FL</t>
+          <t>Houston, TX</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -9836,12 +9836,12 @@
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -9851,7 +9851,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Minneapolis, MN</t>
+          <t>Indianapolis, IN</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -9868,12 +9868,12 @@
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -9883,29 +9883,29 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Montréal, QC</t>
+          <t>Jacksonville, FL</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -9915,7 +9915,7 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Kansas City, MO</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
@@ -9932,12 +9932,12 @@
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -9947,29 +9947,29 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Newark, NJ</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -9979,7 +9979,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Norfolk, VA</t>
+          <t>Las Vegas, NV</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -9996,12 +9996,12 @@
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -10011,7 +10011,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Omaha, NE</t>
+          <t>Los Angeles, CA</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -10028,12 +10028,12 @@
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -10043,29 +10043,29 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Memphis, TN</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -10075,29 +10075,29 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -10107,7 +10107,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Phoenix, AZ</t>
+          <t>Miami, FL</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
@@ -10124,12 +10124,12 @@
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -10139,7 +10139,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA</t>
+          <t>Minneapolis, MN</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -10156,12 +10156,12 @@
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -10171,29 +10171,29 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Portland, OR</t>
+          <t>Montréal, QC</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -10203,29 +10203,29 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Queretaro, MX</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -10235,7 +10235,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Richmond, VA</t>
+          <t>Newark, NJ</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -10252,12 +10252,12 @@
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -10267,7 +10267,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Sacramento, CA</t>
+          <t>Norfolk, VA</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -10284,12 +10284,12 @@
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>Oklahoma City, OK, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -10299,7 +10299,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT</t>
+          <t>Oklahoma City, OK</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -10316,12 +10316,12 @@
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -10331,7 +10331,7 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>San Diego, CA</t>
+          <t>Omaha, NE</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
@@ -10348,12 +10348,12 @@
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -10363,29 +10363,29 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>San Jose, CA</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -10395,29 +10395,29 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Saskatoon, SK</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -10427,7 +10427,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Seattle, WA</t>
+          <t>Phoenix, AZ</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -10444,12 +10444,12 @@
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -10459,7 +10459,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD</t>
+          <t>Pittsburgh, PA</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -10476,12 +10476,12 @@
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -10491,7 +10491,7 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>St. Louis, MO</t>
+          <t>Portland, OR</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
@@ -10508,12 +10508,12 @@
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -10523,29 +10523,29 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Tallahassee, FL</t>
+          <t>Queretaro, MX</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -10555,29 +10555,29 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Toronto, ON</t>
+          <t>Richmond, VA</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -10587,29 +10587,29 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Vancouver, BC</t>
+          <t>Sacramento, CA</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>YWG</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Winnipeg, MB, Canada</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -10619,29 +10619,29 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Winnipeg, MB</t>
+          <t>Salt Lake City, UT</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>San Francisco, United States</t>
+          <t>San Antonio, TX, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -10651,7 +10651,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>San Francisco</t>
+          <t>San Antonio, TX</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -10668,12 +10668,12 @@
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -10683,29 +10683,29 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>San Diego, CA</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Bangor, United States</t>
+          <t>San Francisco, CA, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -10715,7 +10715,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>Bangor</t>
+          <t>San Francisco, CA</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
@@ -10732,12 +10732,12 @@
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Austin, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -10747,7 +10747,7 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Austin</t>
+          <t>San Jose, CA</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
@@ -10764,12 +10764,12 @@
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Albuquerque, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -10779,29 +10779,29 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Albuquerque</t>
+          <t>Saskatoon, SK</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -10811,29 +10811,29 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Seattle, WA</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>San Antonio, United States</t>
+          <t>Sioux Falls, SD, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -10843,7 +10843,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>San Antonio</t>
+          <t>Sioux Falls, SD</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -10860,12 +10860,12 @@
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Cleveland, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -10875,7 +10875,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Cleveland</t>
+          <t>St. Louis, MO</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -10892,12 +10892,12 @@
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Durham, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -10907,7 +10907,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Durham</t>
+          <t>Tallahassee, FL</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -10924,12 +10924,12 @@
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Oklahoma City, United States</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -10939,7 +10939,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Oklahoma City</t>
+          <t>Tampa, FL</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
@@ -10956,12 +10956,12 @@
     <row r="332">
       <c r="A332" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Tampa, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -10971,29 +10971,29 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Tampa</t>
+          <t>Toronto, ON</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Anchorage, United States</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -11003,29 +11003,29 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Anchorage</t>
+          <t>Vancouver, BC</t>
         </is>
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="inlineStr">
         <is>
-          <t>YHZ</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>Halifax, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
@@ -11035,7 +11035,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>Halifax</t>
+          <t>Winnipeg, MB</t>
         </is>
       </c>
       <c r="E334" t="inlineStr">

</xml_diff>

<commit_message>
update generated data Triggered by 287c7f06ba7504118a7fe0e5db2dda76f6f6f2d9
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F334"/>
+  <dimension ref="A1:F333"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8780,12 +8780,12 @@
     <row r="264">
       <c r="A264" s="1" t="inlineStr">
         <is>
-          <t>NNG</t>
+          <t>KCH</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Nanning, China</t>
+          <t>Kuching, Malaysia</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -8795,29 +8795,29 @@
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>Nanning</t>
+          <t>Kuching</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Malaysia</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>MY</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="inlineStr">
         <is>
-          <t>KCH</t>
+          <t>AKX</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Kuching, Malaysia</t>
+          <t>Aktobe, Kazakhstan</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -8827,29 +8827,29 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>Kuching</t>
+          <t>Aktobe</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Malaysia</t>
+          <t>Kazakhstan</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>MY</t>
+          <t>KZ</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="inlineStr">
         <is>
-          <t>AKX</t>
+          <t>TEN</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Aktobe, Kazakhstan</t>
+          <t>Tongren, China</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -8859,29 +8859,29 @@
       </c>
       <c r="D266" t="inlineStr">
         <is>
-          <t>Aktobe</t>
+          <t>Tongren</t>
         </is>
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Kazakhstan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>KZ</t>
+          <t>CN</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="inlineStr">
         <is>
-          <t>TEN</t>
+          <t>HYN</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Tongren, China</t>
+          <t>Taizhou, China</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -8891,7 +8891,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>Tongren</t>
+          <t>Taizhou</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
@@ -8908,12 +8908,12 @@
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>HYN</t>
+          <t>XNN</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Taizhou, China</t>
+          <t>Xining, China</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -8923,7 +8923,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Taizhou</t>
+          <t>Xining</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
@@ -8940,12 +8940,12 @@
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>XNN</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Xining, China</t>
+          <t>Bishkek, Kyrgyzstan</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -8955,29 +8955,29 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Xining</t>
+          <t>Bishkek</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>KG</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>FRU</t>
+          <t>MLG</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Bishkek, Kyrgyzstan</t>
+          <t>Malang, Indonesia</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -8987,29 +8987,29 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Bishkek</t>
+          <t>Malang</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Kyrgyzstan</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>ID</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>MLG</t>
+          <t>LHE</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Malang, Indonesia</t>
+          <t>Lahore, Pakistan</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -9019,29 +9019,29 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Malang</t>
+          <t>Lahore</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>PK</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>LHE</t>
+          <t>CTU</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Lahore, Pakistan</t>
+          <t>Chengdu, China</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -9051,29 +9051,29 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Lahore</t>
+          <t>Chengdu</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>PK</t>
+          <t>CN</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>CTU</t>
+          <t>AGR</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Chengdu, China</t>
+          <t>Agra, India</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -9083,29 +9083,29 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Chengdu</t>
+          <t>Agra</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>IN</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>AGR</t>
+          <t>CJB</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Agra, India</t>
+          <t>Coimbatore, India</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -9115,7 +9115,7 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Agra</t>
+          <t>Coimbatore</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
@@ -9132,44 +9132,44 @@
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>CJB</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Coimbatore, India</t>
+          <t>Albuquerque, NM, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Coimbatore</t>
+          <t>Albuquerque, NM</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Albuquerque, NM, United States</t>
+          <t>Anchorage, AK, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -9179,7 +9179,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Albuquerque, NM</t>
+          <t>Anchorage, AK</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -9196,12 +9196,12 @@
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Anchorage, AK, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -9211,7 +9211,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Anchorage, AK</t>
+          <t>Ashburn, VA</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -9228,12 +9228,12 @@
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -9243,7 +9243,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Ashburn, VA</t>
+          <t>Atlanta, GA</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -9260,12 +9260,12 @@
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Austin, TX, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -9275,7 +9275,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Atlanta, GA</t>
+          <t>Austin, TX</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -9292,12 +9292,12 @@
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Austin, TX, United States</t>
+          <t>Bangor, ME, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -9307,7 +9307,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Austin, TX</t>
+          <t>Bangor, ME</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -9324,12 +9324,12 @@
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Bangor, ME, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -9339,7 +9339,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Bangor, ME</t>
+          <t>Boston, MA</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -9356,12 +9356,12 @@
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -9371,7 +9371,7 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Boston, MA</t>
+          <t>Buffalo, NY</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -9388,12 +9388,12 @@
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -9403,29 +9403,29 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Buffalo, NY</t>
+          <t>Calgary, AB</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -9435,29 +9435,29 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Calgary, AB</t>
+          <t>Charlotte, NC</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -9467,7 +9467,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Charlotte, NC</t>
+          <t>Chicago, IL</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -9484,12 +9484,12 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Cleveland, OH, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -9499,7 +9499,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Chicago, IL</t>
+          <t>Cleveland, OH</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -9516,12 +9516,12 @@
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Cleveland, OH, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -9531,7 +9531,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Cleveland, OH</t>
+          <t>Columbus, OH</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -9548,12 +9548,12 @@
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Columbus, OH</t>
+          <t>Dallas, TX</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -9580,12 +9580,12 @@
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -9595,7 +9595,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Dallas, TX</t>
+          <t>Denver, CO</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -9612,12 +9612,12 @@
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -9627,7 +9627,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Denver, CO</t>
+          <t>Detroit, MI</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -9644,12 +9644,12 @@
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Durham, NC, United States</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -9659,7 +9659,7 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Detroit, MI</t>
+          <t>Durham, NC</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -9676,12 +9676,12 @@
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Durham, NC, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -9691,29 +9691,29 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Durham, NC</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -9723,29 +9723,29 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>YHZ</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Halifax, Canada</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -9755,29 +9755,29 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Halifax</t>
+          <t>Honolulu, HI</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -9787,7 +9787,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Honolulu, HI</t>
+          <t>Houston, TX</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
@@ -9804,12 +9804,12 @@
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -9819,7 +9819,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Houston, TX</t>
+          <t>Indianapolis, IN</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -9836,12 +9836,12 @@
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -9851,7 +9851,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Indianapolis, IN</t>
+          <t>Jacksonville, FL</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -9868,12 +9868,12 @@
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -9883,7 +9883,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Jacksonville, FL</t>
+          <t>Kansas City, MO</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -9900,12 +9900,12 @@
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -9915,29 +9915,29 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Kansas City, MO</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -9947,29 +9947,29 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Las Vegas, NV</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -9979,7 +9979,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Las Vegas, NV</t>
+          <t>Los Angeles, CA</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -9996,12 +9996,12 @@
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -10011,7 +10011,7 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Los Angeles, CA</t>
+          <t>Memphis, TN</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
@@ -10028,12 +10028,12 @@
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -10043,29 +10043,29 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Memphis, TN</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -10075,29 +10075,29 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami, FL</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -10107,7 +10107,7 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Miami, FL</t>
+          <t>Minneapolis, MN</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
@@ -10124,12 +10124,12 @@
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -10139,29 +10139,29 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Minneapolis, MN</t>
+          <t>Montréal, QC</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -10171,29 +10171,29 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Montréal, QC</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -10203,7 +10203,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark, NJ</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -10220,12 +10220,12 @@
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -10235,7 +10235,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Newark, NJ</t>
+          <t>Norfolk, VA</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -10252,12 +10252,12 @@
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Oklahoma City, OK, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -10267,7 +10267,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Norfolk, VA</t>
+          <t>Oklahoma City, OK</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -10284,12 +10284,12 @@
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Oklahoma City, OK, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -10299,7 +10299,7 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Oklahoma City, OK</t>
+          <t>Omaha, NE</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
@@ -10316,12 +10316,12 @@
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -10331,29 +10331,29 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Omaha, NE</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -10363,29 +10363,29 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -10395,7 +10395,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix, AZ</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -10412,12 +10412,12 @@
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -10427,7 +10427,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Phoenix, AZ</t>
+          <t>Pittsburgh, PA</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -10444,12 +10444,12 @@
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -10459,7 +10459,7 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA</t>
+          <t>Portland, OR</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
@@ -10476,12 +10476,12 @@
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -10491,29 +10491,29 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Portland, OR</t>
+          <t>Queretaro, MX</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -10523,29 +10523,29 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Queretaro, MX</t>
+          <t>Richmond, VA</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -10555,7 +10555,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Richmond, VA</t>
+          <t>Sacramento, CA</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
@@ -10572,12 +10572,12 @@
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -10587,7 +10587,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Sacramento, CA</t>
+          <t>Salt Lake City, UT</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
@@ -10604,12 +10604,12 @@
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Antonio, TX, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -10619,7 +10619,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT</t>
+          <t>San Antonio, TX</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -10636,12 +10636,12 @@
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>San Antonio, TX, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -10651,7 +10651,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>San Antonio, TX</t>
+          <t>San Diego, CA</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -10668,12 +10668,12 @@
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Francisco, CA, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -10683,7 +10683,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>San Diego, CA</t>
+          <t>San Francisco, CA</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
@@ -10700,12 +10700,12 @@
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>San Francisco, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -10715,7 +10715,7 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>San Francisco, CA</t>
+          <t>San Jose, CA</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
@@ -10732,12 +10732,12 @@
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -10747,29 +10747,29 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>San Jose, CA</t>
+          <t>Saskatoon, SK</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -10779,29 +10779,29 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Saskatoon, SK</t>
+          <t>Seattle, WA</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, SD, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -10811,7 +10811,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Seattle, WA</t>
+          <t>Sioux Falls, SD</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -10828,12 +10828,12 @@
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -10843,7 +10843,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD</t>
+          <t>St. Louis, MO</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -10860,12 +10860,12 @@
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -10875,7 +10875,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>St. Louis, MO</t>
+          <t>Tallahassee, FL</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -10892,12 +10892,12 @@
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -10907,7 +10907,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Tallahassee, FL</t>
+          <t>Tampa, FL</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -10924,12 +10924,12 @@
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -10939,29 +10939,29 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Tampa, FL</t>
+          <t>Toronto, ON</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -10971,7 +10971,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Toronto, ON</t>
+          <t>Vancouver, BC</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
@@ -10988,12 +10988,12 @@
     <row r="333">
       <c r="A333" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
@@ -11003,7 +11003,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>Vancouver, BC</t>
+          <t>Winnipeg, MB</t>
         </is>
       </c>
       <c r="E333" t="inlineStr">
@@ -11012,38 +11012,6 @@
         </is>
       </c>
       <c r="F333" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334" s="1" t="inlineStr">
-        <is>
-          <t>YWG</t>
-        </is>
-      </c>
-      <c r="B334" t="inlineStr">
-        <is>
-          <t>Winnipeg, MB, Canada</t>
-        </is>
-      </c>
-      <c r="C334" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="D334" t="inlineStr">
-        <is>
-          <t>Winnipeg, MB</t>
-        </is>
-      </c>
-      <c r="E334" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F334" t="inlineStr">
         <is>
           <t>CA</t>
         </is>

</xml_diff>

<commit_message>
update generated data Triggered by 0f0713500e61e26fd35ed92880bfd3fba2a530ef
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -1813,7 +1813,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Santa Venera, Malta</t>
+          <t>Valletta, Malta</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Santa Venera</t>
+          <t>Valletta</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">

</xml_diff>

<commit_message>
update generated data Triggered by 837774e74448cff0a45e673f3d99921cb5d02ced
</commit_message>
<xml_diff>
--- a/DC-Colos.xlsx
+++ b/DC-Colos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F333"/>
+  <dimension ref="A1:F332"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8908,12 +8908,12 @@
     <row r="268">
       <c r="A268" s="1" t="inlineStr">
         <is>
-          <t>XNN</t>
+          <t>FRU</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Xining, China</t>
+          <t>Bishkek, Kyrgyzstan</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -8923,29 +8923,29 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Xining</t>
+          <t>Bishkek</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>KG</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="inlineStr">
         <is>
-          <t>FRU</t>
+          <t>MLG</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Bishkek, Kyrgyzstan</t>
+          <t>Malang, Indonesia</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -8955,29 +8955,29 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>Bishkek</t>
+          <t>Malang</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Kyrgyzstan</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>KG</t>
+          <t>ID</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="inlineStr">
         <is>
-          <t>MLG</t>
+          <t>LHE</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Malang, Indonesia</t>
+          <t>Lahore, Pakistan</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -8987,29 +8987,29 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Malang</t>
+          <t>Lahore</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>PK</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="inlineStr">
         <is>
-          <t>LHE</t>
+          <t>CTU</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Lahore, Pakistan</t>
+          <t>Chengdu, China</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -9019,29 +9019,29 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>Lahore</t>
+          <t>Chengdu</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>PK</t>
+          <t>CN</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="inlineStr">
         <is>
-          <t>CTU</t>
+          <t>AGR</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Chengdu, China</t>
+          <t>Agra, India</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -9051,29 +9051,29 @@
       </c>
       <c r="D272" t="inlineStr">
         <is>
-          <t>Chengdu</t>
+          <t>Agra</t>
         </is>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>CN</t>
+          <t>IN</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="inlineStr">
         <is>
-          <t>AGR</t>
+          <t>CJB</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Agra, India</t>
+          <t>Coimbatore, India</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -9083,7 +9083,7 @@
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>Agra</t>
+          <t>Coimbatore</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -9100,44 +9100,44 @@
     <row r="274">
       <c r="A274" s="1" t="inlineStr">
         <is>
-          <t>CJB</t>
+          <t>ABQ</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Coimbatore, India</t>
+          <t>Albuquerque, NM, United States</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>Asia</t>
+          <t>North America</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>Coimbatore</t>
+          <t>Albuquerque, NM</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="inlineStr">
         <is>
-          <t>ABQ</t>
+          <t>ANC</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Albuquerque, NM, United States</t>
+          <t>Anchorage, AK, United States</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -9147,7 +9147,7 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>Albuquerque, NM</t>
+          <t>Anchorage, AK</t>
         </is>
       </c>
       <c r="E275" t="inlineStr">
@@ -9164,12 +9164,12 @@
     <row r="276">
       <c r="A276" s="1" t="inlineStr">
         <is>
-          <t>ANC</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Anchorage, AK, United States</t>
+          <t>Ashburn, VA, United States</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -9179,7 +9179,7 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>Anchorage, AK</t>
+          <t>Ashburn, VA</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -9196,12 +9196,12 @@
     <row r="277">
       <c r="A277" s="1" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Ashburn, VA, United States</t>
+          <t>Atlanta, GA, United States</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -9211,7 +9211,7 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>Ashburn, VA</t>
+          <t>Atlanta, GA</t>
         </is>
       </c>
       <c r="E277" t="inlineStr">
@@ -9228,12 +9228,12 @@
     <row r="278">
       <c r="A278" s="1" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>AUS</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Atlanta, GA, United States</t>
+          <t>Austin, TX, United States</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -9243,7 +9243,7 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Atlanta, GA</t>
+          <t>Austin, TX</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
@@ -9260,12 +9260,12 @@
     <row r="279">
       <c r="A279" s="1" t="inlineStr">
         <is>
-          <t>AUS</t>
+          <t>BGR</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Austin, TX, United States</t>
+          <t>Bangor, ME, United States</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -9275,7 +9275,7 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>Austin, TX</t>
+          <t>Bangor, ME</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -9292,12 +9292,12 @@
     <row r="280">
       <c r="A280" s="1" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Bangor, ME, United States</t>
+          <t>Boston, MA, United States</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -9307,7 +9307,7 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>Bangor, ME</t>
+          <t>Boston, MA</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
@@ -9324,12 +9324,12 @@
     <row r="281">
       <c r="A281" s="1" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>BUF</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Boston, MA, United States</t>
+          <t>Buffalo, NY, United States</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -9339,7 +9339,7 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>Boston, MA</t>
+          <t>Buffalo, NY</t>
         </is>
       </c>
       <c r="E281" t="inlineStr">
@@ -9356,12 +9356,12 @@
     <row r="282">
       <c r="A282" s="1" t="inlineStr">
         <is>
-          <t>BUF</t>
+          <t>YYC</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Buffalo, NY, United States</t>
+          <t>Calgary, AB, Canada</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -9371,29 +9371,29 @@
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>Buffalo, NY</t>
+          <t>Calgary, AB</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="inlineStr">
         <is>
-          <t>YYC</t>
+          <t>CLT</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Calgary, AB, Canada</t>
+          <t>Charlotte, NC, United States</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -9403,29 +9403,29 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Calgary, AB</t>
+          <t>Charlotte, NC</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="inlineStr">
         <is>
-          <t>CLT</t>
+          <t>ORD</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Charlotte, NC, United States</t>
+          <t>Chicago, IL, United States</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -9435,7 +9435,7 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>Charlotte, NC</t>
+          <t>Chicago, IL</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
@@ -9452,12 +9452,12 @@
     <row r="285">
       <c r="A285" s="1" t="inlineStr">
         <is>
-          <t>ORD</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Chicago, IL, United States</t>
+          <t>Cleveland, OH, United States</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -9467,7 +9467,7 @@
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Chicago, IL</t>
+          <t>Cleveland, OH</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -9484,12 +9484,12 @@
     <row r="286">
       <c r="A286" s="1" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>CMH</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Cleveland, OH, United States</t>
+          <t>Columbus, OH, United States</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -9499,7 +9499,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>Cleveland, OH</t>
+          <t>Columbus, OH</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -9516,12 +9516,12 @@
     <row r="287">
       <c r="A287" s="1" t="inlineStr">
         <is>
-          <t>CMH</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Columbus, OH, United States</t>
+          <t>Dallas, TX, United States</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -9531,7 +9531,7 @@
       </c>
       <c r="D287" t="inlineStr">
         <is>
-          <t>Columbus, OH</t>
+          <t>Dallas, TX</t>
         </is>
       </c>
       <c r="E287" t="inlineStr">
@@ -9548,12 +9548,12 @@
     <row r="288">
       <c r="A288" s="1" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Dallas, TX, United States</t>
+          <t>Denver, CO, United States</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>Dallas, TX</t>
+          <t>Denver, CO</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -9580,12 +9580,12 @@
     <row r="289">
       <c r="A289" s="1" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>DTW</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Denver, CO, United States</t>
+          <t>Detroit, MI, United States</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -9595,7 +9595,7 @@
       </c>
       <c r="D289" t="inlineStr">
         <is>
-          <t>Denver, CO</t>
+          <t>Detroit, MI</t>
         </is>
       </c>
       <c r="E289" t="inlineStr">
@@ -9612,12 +9612,12 @@
     <row r="290">
       <c r="A290" s="1" t="inlineStr">
         <is>
-          <t>DTW</t>
+          <t>RDU</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Detroit, MI, United States</t>
+          <t>Durham, NC, United States</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -9627,7 +9627,7 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>Detroit, MI</t>
+          <t>Durham, NC</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
@@ -9644,12 +9644,12 @@
     <row r="291">
       <c r="A291" s="1" t="inlineStr">
         <is>
-          <t>RDU</t>
+          <t>GDL</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Durham, NC, United States</t>
+          <t>Guadalajara, Mexico</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -9659,29 +9659,29 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Durham, NC</t>
+          <t>Guadalajara</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="inlineStr">
         <is>
-          <t>GDL</t>
+          <t>YHZ</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Guadalajara, Mexico</t>
+          <t>Halifax, Canada</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -9691,29 +9691,29 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>Guadalajara</t>
+          <t>Halifax</t>
         </is>
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="inlineStr">
         <is>
-          <t>YHZ</t>
+          <t>HNL</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Halifax, Canada</t>
+          <t>Honolulu, HI, United States</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -9723,29 +9723,29 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>Halifax</t>
+          <t>Honolulu, HI</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="inlineStr">
         <is>
-          <t>HNL</t>
+          <t>IAH</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Honolulu, HI, United States</t>
+          <t>Houston, TX, United States</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -9755,7 +9755,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>Honolulu, HI</t>
+          <t>Houston, TX</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
@@ -9772,12 +9772,12 @@
     <row r="295">
       <c r="A295" s="1" t="inlineStr">
         <is>
-          <t>IAH</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Houston, TX, United States</t>
+          <t>Indianapolis, IN, United States</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -9787,7 +9787,7 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Houston, TX</t>
+          <t>Indianapolis, IN</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
@@ -9804,12 +9804,12 @@
     <row r="296">
       <c r="A296" s="1" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>JAX</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Indianapolis, IN, United States</t>
+          <t>Jacksonville, FL, United States</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -9819,7 +9819,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Indianapolis, IN</t>
+          <t>Jacksonville, FL</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -9836,12 +9836,12 @@
     <row r="297">
       <c r="A297" s="1" t="inlineStr">
         <is>
-          <t>JAX</t>
+          <t>MCI</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Jacksonville, FL, United States</t>
+          <t>Kansas City, MO, United States</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -9851,7 +9851,7 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>Jacksonville, FL</t>
+          <t>Kansas City, MO</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -9868,12 +9868,12 @@
     <row r="298">
       <c r="A298" s="1" t="inlineStr">
         <is>
-          <t>MCI</t>
+          <t>KIN</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>Kansas City, MO, United States</t>
+          <t>Kingston, Jamaica</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -9883,29 +9883,29 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>Kansas City, MO</t>
+          <t>Kingston</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Jamaica</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>JM</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="inlineStr">
         <is>
-          <t>KIN</t>
+          <t>LAS</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Kingston, Jamaica</t>
+          <t>Las Vegas, NV, United States</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -9915,29 +9915,29 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>Kingston</t>
+          <t>Las Vegas, NV</t>
         </is>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Jamaica</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>JM</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>LAX</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Las Vegas, NV, United States</t>
+          <t>Los Angeles, CA, United States</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -9947,7 +9947,7 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Las Vegas, NV</t>
+          <t>Los Angeles, CA</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -9964,12 +9964,12 @@
     <row r="301">
       <c r="A301" s="1" t="inlineStr">
         <is>
-          <t>LAX</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Los Angeles, CA, United States</t>
+          <t>Memphis, TN, United States</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -9979,7 +9979,7 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>Los Angeles, CA</t>
+          <t>Memphis, TN</t>
         </is>
       </c>
       <c r="E301" t="inlineStr">
@@ -9996,12 +9996,12 @@
     <row r="302">
       <c r="A302" s="1" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MEX</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Memphis, TN, United States</t>
+          <t>Mexico City, Mexico</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -10011,29 +10011,29 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>Memphis, TN</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="inlineStr">
         <is>
-          <t>MEX</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Mexico City, Mexico</t>
+          <t>Miami, FL, United States</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -10043,29 +10043,29 @@
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Miami, FL</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MSP</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Miami, FL, United States</t>
+          <t>Minneapolis, MN, United States</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -10075,7 +10075,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Miami, FL</t>
+          <t>Minneapolis, MN</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -10092,12 +10092,12 @@
     <row r="305">
       <c r="A305" s="1" t="inlineStr">
         <is>
-          <t>MSP</t>
+          <t>YUL</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Minneapolis, MN, United States</t>
+          <t>Montréal, QC, Canada</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -10107,29 +10107,29 @@
       </c>
       <c r="D305" t="inlineStr">
         <is>
-          <t>Minneapolis, MN</t>
+          <t>Montréal, QC</t>
         </is>
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="inlineStr">
         <is>
-          <t>YUL</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Montréal, QC, Canada</t>
+          <t>Nashville, United States</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -10139,29 +10139,29 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>Montréal, QC</t>
+          <t>Nashville</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>EWR</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Nashville, United States</t>
+          <t>Newark, NJ, United States</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -10171,7 +10171,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>Nashville</t>
+          <t>Newark, NJ</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -10188,12 +10188,12 @@
     <row r="308">
       <c r="A308" s="1" t="inlineStr">
         <is>
-          <t>EWR</t>
+          <t>ORF</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Newark, NJ, United States</t>
+          <t>Norfolk, VA, United States</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -10203,7 +10203,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>Newark, NJ</t>
+          <t>Norfolk, VA</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -10220,12 +10220,12 @@
     <row r="309">
       <c r="A309" s="1" t="inlineStr">
         <is>
-          <t>ORF</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Norfolk, VA, United States</t>
+          <t>Oklahoma City, OK, United States</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -10235,7 +10235,7 @@
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>Norfolk, VA</t>
+          <t>Oklahoma City, OK</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -10252,12 +10252,12 @@
     <row r="310">
       <c r="A310" s="1" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>OMA</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Oklahoma City, OK, United States</t>
+          <t>Omaha, NE, United States</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -10267,7 +10267,7 @@
       </c>
       <c r="D310" t="inlineStr">
         <is>
-          <t>Oklahoma City, OK</t>
+          <t>Omaha, NE</t>
         </is>
       </c>
       <c r="E310" t="inlineStr">
@@ -10284,12 +10284,12 @@
     <row r="311">
       <c r="A311" s="1" t="inlineStr">
         <is>
-          <t>OMA</t>
+          <t>YOW</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Omaha, NE, United States</t>
+          <t>Ottawa, Canada</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -10299,29 +10299,29 @@
       </c>
       <c r="D311" t="inlineStr">
         <is>
-          <t>Omaha, NE</t>
+          <t>Ottawa</t>
         </is>
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="inlineStr">
         <is>
-          <t>YOW</t>
+          <t>PHL</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Ottawa, Canada</t>
+          <t>Philadelphia, United States</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -10331,29 +10331,29 @@
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>Ottawa</t>
+          <t>Philadelphia</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="inlineStr">
         <is>
-          <t>PHL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Philadelphia, United States</t>
+          <t>Phoenix, AZ, United States</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -10363,7 +10363,7 @@
       </c>
       <c r="D313" t="inlineStr">
         <is>
-          <t>Philadelphia</t>
+          <t>Phoenix, AZ</t>
         </is>
       </c>
       <c r="E313" t="inlineStr">
@@ -10380,12 +10380,12 @@
     <row r="314">
       <c r="A314" s="1" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>PIT</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Phoenix, AZ, United States</t>
+          <t>Pittsburgh, PA, United States</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -10395,7 +10395,7 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Phoenix, AZ</t>
+          <t>Pittsburgh, PA</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
@@ -10412,12 +10412,12 @@
     <row r="315">
       <c r="A315" s="1" t="inlineStr">
         <is>
-          <t>PIT</t>
+          <t>PDX</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA, United States</t>
+          <t>Portland, OR, United States</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -10427,7 +10427,7 @@
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>Pittsburgh, PA</t>
+          <t>Portland, OR</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -10444,12 +10444,12 @@
     <row r="316">
       <c r="A316" s="1" t="inlineStr">
         <is>
-          <t>PDX</t>
+          <t>QRO</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Portland, OR, United States</t>
+          <t>Queretaro, MX, Mexico</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -10459,29 +10459,29 @@
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>Portland, OR</t>
+          <t>Queretaro, MX</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>MX</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="inlineStr">
         <is>
-          <t>QRO</t>
+          <t>RIC</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Queretaro, MX, Mexico</t>
+          <t>Richmond, VA, United States</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -10491,29 +10491,29 @@
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Queretaro, MX</t>
+          <t>Richmond, VA</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>MX</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>SMF</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Richmond, VA, United States</t>
+          <t>Sacramento, CA, United States</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -10523,7 +10523,7 @@
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Richmond, VA</t>
+          <t>Sacramento, CA</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
@@ -10540,12 +10540,12 @@
     <row r="319">
       <c r="A319" s="1" t="inlineStr">
         <is>
-          <t>SMF</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Sacramento, CA, United States</t>
+          <t>Salt Lake City, UT, United States</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -10555,7 +10555,7 @@
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Sacramento, CA</t>
+          <t>Salt Lake City, UT</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
@@ -10572,12 +10572,12 @@
     <row r="320">
       <c r="A320" s="1" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SAT</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT, United States</t>
+          <t>San Antonio, TX, United States</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -10587,7 +10587,7 @@
       </c>
       <c r="D320" t="inlineStr">
         <is>
-          <t>Salt Lake City, UT</t>
+          <t>San Antonio, TX</t>
         </is>
       </c>
       <c r="E320" t="inlineStr">
@@ -10604,12 +10604,12 @@
     <row r="321">
       <c r="A321" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>SAN</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>San Antonio, TX, United States</t>
+          <t>San Diego, CA, United States</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">
@@ -10619,7 +10619,7 @@
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>San Antonio, TX</t>
+          <t>San Diego, CA</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -10636,12 +10636,12 @@
     <row r="322">
       <c r="A322" s="1" t="inlineStr">
         <is>
-          <t>SAN</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>San Diego, CA, United States</t>
+          <t>San Francisco, CA, United States</t>
         </is>
       </c>
       <c r="C322" t="inlineStr">
@@ -10651,7 +10651,7 @@
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>San Diego, CA</t>
+          <t>San Francisco, CA</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -10668,12 +10668,12 @@
     <row r="323">
       <c r="A323" s="1" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>SJC</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>San Francisco, CA, United States</t>
+          <t>San Jose, CA, United States</t>
         </is>
       </c>
       <c r="C323" t="inlineStr">
@@ -10683,7 +10683,7 @@
       </c>
       <c r="D323" t="inlineStr">
         <is>
-          <t>San Francisco, CA</t>
+          <t>San Jose, CA</t>
         </is>
       </c>
       <c r="E323" t="inlineStr">
@@ -10700,12 +10700,12 @@
     <row r="324">
       <c r="A324" s="1" t="inlineStr">
         <is>
-          <t>SJC</t>
+          <t>YXE</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>San Jose, CA, United States</t>
+          <t>Saskatoon, SK, Canada</t>
         </is>
       </c>
       <c r="C324" t="inlineStr">
@@ -10715,29 +10715,29 @@
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>San Jose, CA</t>
+          <t>Saskatoon, SK</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="inlineStr">
         <is>
-          <t>YXE</t>
+          <t>SEA</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Saskatoon, SK, Canada</t>
+          <t>Seattle, WA, United States</t>
         </is>
       </c>
       <c r="C325" t="inlineStr">
@@ -10747,29 +10747,29 @@
       </c>
       <c r="D325" t="inlineStr">
         <is>
-          <t>Saskatoon, SK</t>
+          <t>Seattle, WA</t>
         </is>
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>US</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="inlineStr">
         <is>
-          <t>SEA</t>
+          <t>FSD</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Seattle, WA, United States</t>
+          <t>Sioux Falls, SD, United States</t>
         </is>
       </c>
       <c r="C326" t="inlineStr">
@@ -10779,7 +10779,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>Seattle, WA</t>
+          <t>Sioux Falls, SD</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -10796,12 +10796,12 @@
     <row r="327">
       <c r="A327" s="1" t="inlineStr">
         <is>
-          <t>FSD</t>
+          <t>STL</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD, United States</t>
+          <t>St. Louis, MO, United States</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
@@ -10811,7 +10811,7 @@
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>Sioux Falls, SD</t>
+          <t>St. Louis, MO</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -10828,12 +10828,12 @@
     <row r="328">
       <c r="A328" s="1" t="inlineStr">
         <is>
-          <t>STL</t>
+          <t>TLH</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>St. Louis, MO, United States</t>
+          <t>Tallahassee, FL, United States</t>
         </is>
       </c>
       <c r="C328" t="inlineStr">
@@ -10843,7 +10843,7 @@
       </c>
       <c r="D328" t="inlineStr">
         <is>
-          <t>St. Louis, MO</t>
+          <t>Tallahassee, FL</t>
         </is>
       </c>
       <c r="E328" t="inlineStr">
@@ -10860,12 +10860,12 @@
     <row r="329">
       <c r="A329" s="1" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>TPA</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>Tallahassee, FL, United States</t>
+          <t>Tampa, FL, United States</t>
         </is>
       </c>
       <c r="C329" t="inlineStr">
@@ -10875,7 +10875,7 @@
       </c>
       <c r="D329" t="inlineStr">
         <is>
-          <t>Tallahassee, FL</t>
+          <t>Tampa, FL</t>
         </is>
       </c>
       <c r="E329" t="inlineStr">
@@ -10892,12 +10892,12 @@
     <row r="330">
       <c r="A330" s="1" t="inlineStr">
         <is>
-          <t>TPA</t>
+          <t>YYZ</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>Tampa, FL, United States</t>
+          <t>Toronto, ON, Canada</t>
         </is>
       </c>
       <c r="C330" t="inlineStr">
@@ -10907,29 +10907,29 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>Tampa, FL</t>
+          <t>Toronto, ON</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>CA</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="inlineStr">
         <is>
-          <t>YYZ</t>
+          <t>YVR</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Toronto, ON, Canada</t>
+          <t>Vancouver, BC, Canada</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
@@ -10939,7 +10939,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>Toronto, ON</t>
+          <t>Vancouver, BC</t>
         </is>
       </c>
       <c r="E331" t="inlineStr">
@@ -10956,12 +10956,12 @@
     <row r="332">
       <c r="A332" s="1" t="inlineStr">
         <is>
-          <t>YVR</t>
+          <t>YWG</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>Vancouver, BC, Canada</t>
+          <t>Winnipeg, MB, Canada</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
@@ -10971,7 +10971,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>Vancouver, BC</t>
+          <t>Winnipeg, MB</t>
         </is>
       </c>
       <c r="E332" t="inlineStr">
@@ -10980,38 +10980,6 @@
         </is>
       </c>
       <c r="F332" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-    </row>
-    <row r="333">
-      <c r="A333" s="1" t="inlineStr">
-        <is>
-          <t>YWG</t>
-        </is>
-      </c>
-      <c r="B333" t="inlineStr">
-        <is>
-          <t>Winnipeg, MB, Canada</t>
-        </is>
-      </c>
-      <c r="C333" t="inlineStr">
-        <is>
-          <t>North America</t>
-        </is>
-      </c>
-      <c r="D333" t="inlineStr">
-        <is>
-          <t>Winnipeg, MB</t>
-        </is>
-      </c>
-      <c r="E333" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F333" t="inlineStr">
         <is>
           <t>CA</t>
         </is>

</xml_diff>